<commit_message>
Add direction description data to report template
</commit_message>
<xml_diff>
--- a/comptages/report/template.xlsx
+++ b/comptages/report/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="289">
   <si>
     <t xml:space="preserve">Aller</t>
   </si>
@@ -632,7 +632,7 @@
     <t xml:space="preserve">Model</t>
   </si>
   <si>
-    <t xml:space="preserve">Modèle : M680_L</t>
+    <t xml:space="preserve">Modèle : M660_LT</t>
   </si>
   <si>
     <t xml:space="preserve">Class</t>
@@ -665,6 +665,18 @@
     <t xml:space="preserve">Remarque : </t>
   </si>
   <si>
+    <t xml:space="preserve">Direction 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peseux Gir. de la Maison de Commune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auvernier Gir. de Brena</t>
+  </si>
+  <si>
     <t xml:space="preserve">Data by day</t>
   </si>
   <si>
@@ -692,16 +704,10 @@
     <t xml:space="preserve">total</t>
   </si>
   <si>
-    <t xml:space="preserve">Direction 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">light</t>
   </si>
   <si>
     <t xml:space="preserve">heavy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction 2</t>
   </si>
   <si>
     <t xml:space="preserve">Data speed </t>
@@ -2201,7 +2207,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2209,11 +2215,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10301,7 +10307,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="216" t="str">
@@ -10311,7 +10317,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="216" t="str">
@@ -10331,17 +10337,17 @@
     <row r="8" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D9" s="218" t="n">
         <f aca="false">Data1!J2</f>
         <v>0</v>
       </c>
       <c r="M9" s="219" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="W9" s="220" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -10350,7 +10356,7 @@
       <c r="A12" s="52"/>
       <c r="B12" s="52"/>
       <c r="C12" s="221" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D12" s="221"/>
       <c r="E12" s="221"/>
@@ -10362,7 +10368,7 @@
       <c r="K12" s="221"/>
       <c r="L12" s="222"/>
       <c r="M12" s="221" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="N12" s="221"/>
       <c r="O12" s="221"/>
@@ -10374,7 +10380,7 @@
       <c r="U12" s="221"/>
       <c r="V12" s="222"/>
       <c r="W12" s="221" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="X12" s="221"/>
       <c r="Y12" s="221"/>
@@ -10388,7 +10394,7 @@
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="224"/>
       <c r="B13" s="225" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C13" s="226" t="s">
         <v>31</v>
@@ -10412,10 +10418,10 @@
         <v>37</v>
       </c>
       <c r="J13" s="230" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="K13" s="231" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="L13" s="224"/>
       <c r="M13" s="226" t="str">
@@ -13344,7 +13350,7 @@
     </row>
     <row r="40" s="224" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="245" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C40" s="246" t="n">
         <f aca="false">SUM(C14:C37)</f>
@@ -13560,7 +13566,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="54" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B3" s="254" t="str">
         <f aca="false">Data1!A2</f>
@@ -13569,7 +13575,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="54" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B4" s="56" t="str">
         <f aca="false">Data1!G2</f>
@@ -13610,7 +13616,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="257" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B8" s="258" t="str">
         <f aca="false">B3</f>
@@ -13640,7 +13646,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="262" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B11" s="263" t="str">
         <f aca="false">Data2!BI9</f>
@@ -13672,7 +13678,7 @@
       </c>
       <c r="I11" s="80"/>
       <c r="J11" s="266" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="K11" s="261"/>
     </row>
@@ -14665,7 +14671,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B37" s="276" t="n">
         <f aca="false">SUM(B12:B35)/Data_category!$L$29</f>
@@ -14706,7 +14712,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B38" s="280" t="n">
         <f aca="false">SUM(B18:B33)/Data_category!$L$29</f>
@@ -14747,7 +14753,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B39" s="284" t="n">
         <f aca="false">B37-B38</f>
@@ -14797,7 +14803,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="257" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B41" s="216" t="str">
         <f aca="false">B4</f>
@@ -14827,7 +14833,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="262" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B44" s="290" t="str">
         <f aca="false">B11</f>
@@ -14859,7 +14865,7 @@
       </c>
       <c r="I44" s="80"/>
       <c r="J44" s="266" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="K44" s="261"/>
     </row>
@@ -15852,7 +15858,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B70" s="276" t="n">
         <f aca="false">SUM(B45:B68)/Data_category!$L$57</f>
@@ -15893,7 +15899,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B71" s="280" t="n">
         <f aca="false">SUM(B51:B66)/Data_category!$L$57</f>
@@ -15934,7 +15940,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B72" s="284" t="n">
         <f aca="false">B70-B71</f>
@@ -16128,7 +16134,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="54" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B3" s="56" t="str">
         <f aca="false">Data1!A2</f>
@@ -16137,7 +16143,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="54" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B4" s="56" t="str">
         <f aca="false">Data1!G2</f>
@@ -16181,7 +16187,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="257" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B8" s="216" t="str">
         <f aca="false">B3</f>
@@ -16219,7 +16225,7 @@
       <c r="H11" s="213"/>
       <c r="I11" s="308"/>
       <c r="J11" s="309" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="K11" s="261"/>
     </row>
@@ -16688,7 +16694,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B38" s="276" t="n">
         <f aca="false">SWISS7_H!B37</f>
@@ -16727,7 +16733,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B39" s="280" t="n">
         <f aca="false">SWISS7_H!B38</f>
@@ -16766,7 +16772,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B40" s="284" t="n">
         <f aca="false">SWISS7_H!B39</f>
@@ -16805,7 +16811,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="257" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B43" s="216" t="str">
         <f aca="false">B4</f>
@@ -16840,7 +16846,7 @@
       <c r="H46" s="295"/>
       <c r="I46" s="295"/>
       <c r="J46" s="266" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="K46" s="261"/>
     </row>
@@ -17309,7 +17315,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B73" s="276" t="n">
         <f aca="false">SWISS7_H!B70</f>
@@ -17348,7 +17354,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B74" s="280" t="n">
         <f aca="false">SWISS7_H!B71</f>
@@ -17387,7 +17393,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B75" s="284" t="n">
         <f aca="false">SWISS7_H!B72</f>
@@ -17500,7 +17506,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="54" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B3" s="254" t="str">
         <f aca="false">Data1!A2</f>
@@ -17509,7 +17515,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="54" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B4" s="56" t="str">
         <f aca="false">Data1!G2</f>
@@ -17556,7 +17562,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="257" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B8" s="258" t="str">
         <f aca="false">B3</f>
@@ -17580,15 +17586,15 @@
       <c r="K10" s="289"/>
       <c r="L10" s="332"/>
       <c r="M10" s="260" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="N10" s="261" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="262" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B11" s="290" t="str">
         <f aca="false">Data2!BI11</f>
@@ -17632,7 +17638,7 @@
       </c>
       <c r="L11" s="100"/>
       <c r="M11" s="266" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="N11" s="261"/>
     </row>
@@ -18935,7 +18941,7 @@
     <row r="36" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B37" s="276" t="n">
         <f aca="false">SUM(B12:B35)/Data_category!$L$29</f>
@@ -18989,7 +18995,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B38" s="280" t="n">
         <f aca="false">SUM(B18:B33)/Data_category!$L$29</f>
@@ -19043,7 +19049,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B39" s="284" t="n">
         <f aca="false">B37-B38</f>
@@ -19107,7 +19113,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="257" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B41" s="216" t="str">
         <f aca="false">B4</f>
@@ -19131,7 +19137,7 @@
       <c r="K43" s="289"/>
       <c r="L43" s="332"/>
       <c r="M43" s="260" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="N43" s="261" t="str">
         <f aca="false">N10</f>
@@ -19140,7 +19146,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="262" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B44" s="290" t="str">
         <f aca="false">B11</f>
@@ -19184,7 +19190,7 @@
       </c>
       <c r="L44" s="100"/>
       <c r="M44" s="266" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="N44" s="261"/>
     </row>
@@ -20487,7 +20493,7 @@
     <row r="69" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B70" s="276" t="n">
         <f aca="false">SUM(B45:B68)/Data_category!$L$57</f>
@@ -20541,7 +20547,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B71" s="280" t="n">
         <f aca="false">SUM(B51:B66)/Data_category!$L$57</f>
@@ -20595,7 +20601,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B72" s="284" t="n">
         <f aca="false">B70-B71</f>
@@ -20823,7 +20829,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="54" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B3" s="56" t="str">
         <f aca="false">Data1!A2</f>
@@ -20832,7 +20838,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="54" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B4" s="56" t="str">
         <f aca="false">Data1!G2</f>
@@ -20882,7 +20888,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="257" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B8" s="216" t="str">
         <f aca="false">B3</f>
@@ -20908,7 +20914,7 @@
       <c r="L10" s="306"/>
       <c r="M10" s="307"/>
       <c r="N10" s="261" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20925,7 +20931,7 @@
       <c r="K11" s="213"/>
       <c r="L11" s="308"/>
       <c r="M11" s="309" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="N11" s="261"/>
     </row>
@@ -21478,7 +21484,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B38" s="276" t="n">
         <f aca="false">SWISS10_H!B37</f>
@@ -21529,7 +21535,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B39" s="280" t="n">
         <f aca="false">SWISS10_H!B38</f>
@@ -21580,7 +21586,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B40" s="284" t="n">
         <f aca="false">SWISS10_H!B39</f>
@@ -21631,7 +21637,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="257" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B43" s="216" t="str">
         <f aca="false">B4</f>
@@ -21672,7 +21678,7 @@
       <c r="K46" s="295"/>
       <c r="L46" s="295"/>
       <c r="M46" s="266" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="N46" s="261"/>
     </row>
@@ -22225,7 +22231,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B73" s="276" t="n">
         <f aca="false">SWISS10_H!B70</f>
@@ -22276,7 +22282,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B74" s="280" t="n">
         <f aca="false">SWISS10_H!B71</f>
@@ -22327,7 +22333,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B75" s="284" t="n">
         <f aca="false">SWISS10_H!B72</f>
@@ -22457,7 +22463,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="54" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B3" s="56" t="str">
         <f aca="false">Data1!A2</f>
@@ -22466,7 +22472,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="54" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B4" s="56" t="str">
         <f aca="false">Data1!G2</f>
@@ -22518,7 +22524,7 @@
     <row r="9" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="257" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B10" s="216" t="str">
         <f aca="false">B3</f>
@@ -22567,11 +22573,11 @@
       <c r="L12" s="289"/>
       <c r="M12" s="289"/>
       <c r="O12" s="260" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P12" s="332"/>
       <c r="R12" s="27" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="S12" s="27"/>
       <c r="T12" s="27"/>
@@ -22580,7 +22586,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="262" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B13" s="290" t="str">
         <f aca="false">FIXED(Data!AO8,0)&amp;" km/h"</f>
@@ -22631,20 +22637,20 @@
         <v>&gt; 130 km/h</v>
       </c>
       <c r="O13" s="342" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="P13" s="5"/>
       <c r="R13" s="343" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="S13" s="344" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="T13" s="345" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="U13" s="346" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24438,7 +24444,7 @@
     </row>
     <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B40" s="358" t="n">
         <f aca="false">SUM(B14:B37)/Data_speed!$O$29</f>
@@ -24512,7 +24518,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B41" s="362" t="n">
         <f aca="false">SUM(B20:B35)/Data_speed!$O$29</f>
@@ -24586,7 +24592,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B42" s="366" t="n">
         <f aca="false">B40-B41</f>
@@ -24678,7 +24684,7 @@
     </row>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="257" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B46" s="216" t="str">
         <f aca="false">B4</f>
@@ -24744,7 +24750,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="262" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B49" s="290" t="str">
         <f aca="false">B13</f>
@@ -26607,7 +26613,7 @@
     </row>
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B76" s="358" t="n">
         <f aca="false">SUM(B50:B73)/Data_speed!$O$57</f>
@@ -26681,7 +26687,7 @@
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B77" s="362" t="n">
         <f aca="false">SUM(B56:B71)/Data_speed!$O$57</f>
@@ -26755,7 +26761,7 @@
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B78" s="366" t="n">
         <f aca="false">B76-B77</f>
@@ -26918,7 +26924,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="54" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B3" s="56" t="str">
         <f aca="false">Data1!A2</f>
@@ -26927,7 +26933,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="54" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B4" s="56" t="str">
         <f aca="false">Data1!G2</f>
@@ -26981,7 +26987,7 @@
     <row r="9" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="257" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B10" s="216" t="str">
         <f aca="false">B3</f>
@@ -27032,11 +27038,11 @@
       <c r="M12" s="289"/>
       <c r="N12" s="374"/>
       <c r="P12" s="260" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="Q12" s="332"/>
       <c r="S12" s="27" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="T12" s="27"/>
       <c r="U12" s="27"/>
@@ -27044,7 +27050,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="262" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B13" s="290" t="str">
         <f aca="false">FIXED(Data!AO8,0)&amp;" km/h"</f>
@@ -27096,20 +27102,20 @@
       </c>
       <c r="N13" s="293"/>
       <c r="P13" s="342" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="Q13" s="5"/>
       <c r="S13" s="343" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="T13" s="344" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="U13" s="345" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="V13" s="346" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29000,7 +29006,7 @@
     </row>
     <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B40" s="358" t="n">
         <f aca="false">SUM(B14:B37)/Data_speed!$O$29</f>
@@ -29078,7 +29084,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B41" s="362" t="n">
         <f aca="false">SUM(B20:B35)/Data_speed!$O$29</f>
@@ -29156,7 +29162,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B42" s="366" t="n">
         <f aca="false">B40-B41</f>
@@ -29252,7 +29258,7 @@
     </row>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="257" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B46" s="216" t="str">
         <f aca="false">B4</f>
@@ -29320,7 +29326,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="262" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B49" s="290" t="str">
         <f aca="false">B13</f>
@@ -31281,7 +31287,7 @@
     </row>
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="60" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B76" s="358" t="n">
         <f aca="false">SUM(B50:B73)/Data_speed!$O$57</f>
@@ -31359,7 +31365,7 @@
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="279" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B77" s="362" t="n">
         <f aca="false">SUM(B56:B71)/Data_speed!$O$57</f>
@@ -31437,7 +31443,7 @@
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="283" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B78" s="366" t="n">
         <f aca="false">B76-B77</f>
@@ -36955,15 +36961,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="119.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="11.52"/>
   </cols>
@@ -37054,6 +37060,22 @@
       </c>
       <c r="B12" s="49" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -37085,7 +37107,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37095,28 +37117,28 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37841,7 +37863,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B29" s="1" t="n">
         <f aca="false">SUM(B5:B28)</f>
@@ -37879,33 +37901,33 @@
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="50" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38630,7 +38652,7 @@
     </row>
     <row r="57" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B57" s="1" t="n">
         <f aca="false">SUM(B33:B56)</f>
@@ -38668,7 +38690,7 @@
     <row r="58" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B59" s="49" t="n">
         <v>7028</v>
@@ -38694,7 +38716,7 @@
     </row>
     <row r="60" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B60" s="49" t="n">
         <v>85</v>
@@ -38721,33 +38743,33 @@
     <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="50" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -39472,7 +39494,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B88" s="1" t="n">
         <f aca="false">SUM(B64:B87)</f>
@@ -39509,7 +39531,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B90" s="49" t="n">
         <v>7043</v>
@@ -39535,7 +39557,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B91" s="49" t="n">
         <v>115</v>
@@ -39588,12 +39610,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="50" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -40743,7 +40765,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B29" s="1" t="n">
         <f aca="false">SUM(B5:B28)</f>
@@ -40805,7 +40827,7 @@
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="50" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -41955,7 +41977,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B57" s="1" t="n">
         <f aca="false">SUM(B33:B56)</f>
@@ -42043,12 +42065,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="50" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -42925,7 +42947,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B29" s="1" t="n">
         <f aca="false">SUM(B5:B28)</f>
@@ -42975,7 +42997,7 @@
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="50" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43852,7 +43874,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B57" s="1" t="n">
         <f aca="false">SUM(B33:B56)</f>
@@ -43917,7 +43939,7 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -43952,7 +43974,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="54" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B3" s="56" t="str">
         <f aca="false">Data1!A2</f>
@@ -43961,7 +43983,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="54" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B4" s="56" t="str">
         <f aca="false">Data1!G2</f>
@@ -43987,7 +44009,7 @@
     </row>
     <row r="8" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C8" s="59" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D8" s="59"/>
       <c r="E8" s="59"/>
@@ -44000,20 +44022,20 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C9" s="60" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D9" s="60"/>
       <c r="E9" s="60"/>
       <c r="F9" s="60" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G9" s="60"/>
       <c r="H9" s="60" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="I9" s="60"/>
       <c r="J9" s="61" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="K9" s="61"/>
     </row>
@@ -44025,25 +44047,25 @@
         <v>38</v>
       </c>
       <c r="E10" s="64" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F10" s="63" t="s">
         <v>38</v>
       </c>
       <c r="G10" s="64" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H10" s="63" t="s">
         <v>38</v>
       </c>
       <c r="I10" s="64" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="J10" s="65" t="s">
         <v>38</v>
       </c>
       <c r="K10" s="66" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -44341,7 +44363,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="91" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B20" s="92"/>
       <c r="C20" s="93" t="n">
@@ -44383,7 +44405,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="95" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B21" s="96"/>
       <c r="C21" s="97" t="n">
@@ -44425,7 +44447,7 @@
     </row>
     <row r="22" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C22" s="25" t="n">
         <f aca="false">Data1!J2</f>
@@ -44458,7 +44480,7 @@
     </row>
     <row r="26" s="1" customFormat="true" ht="19.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C26" s="103" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D26" s="103"/>
       <c r="E26" s="103"/>
@@ -44468,11 +44490,11 @@
     </row>
     <row r="27" s="1" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C27" s="104" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D27" s="104"/>
       <c r="E27" s="105" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F27" s="105"/>
       <c r="H27" s="51"/>
@@ -44480,7 +44502,7 @@
     </row>
     <row r="28" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="106" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B28" s="107"/>
       <c r="C28" s="108" t="n">
@@ -44497,7 +44519,7 @@
     </row>
     <row r="29" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="110" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B29" s="111"/>
       <c r="C29" s="112" t="n">
@@ -44514,7 +44536,7 @@
     </row>
     <row r="30" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="110" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B30" s="111"/>
       <c r="C30" s="112" t="n">
@@ -44531,7 +44553,7 @@
     </row>
     <row r="31" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="110" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B31" s="111"/>
       <c r="C31" s="112" t="n">
@@ -44548,7 +44570,7 @@
     </row>
     <row r="32" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="114" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B32" s="115"/>
       <c r="C32" s="116" t="n">
@@ -44575,7 +44597,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="106" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B34" s="120"/>
       <c r="C34" s="108" t="n">
@@ -44588,7 +44610,7 @@
       </c>
       <c r="F34" s="109"/>
       <c r="H34" s="121" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="I34" s="121"/>
       <c r="J34" s="121"/>
@@ -44596,7 +44618,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="114" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B35" s="122"/>
       <c r="C35" s="116" t="n">
@@ -44660,7 +44682,7 @@
     </row>
     <row r="41" customFormat="false" ht="18.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C41" s="103" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D41" s="103"/>
       <c r="E41" s="103"/>
@@ -44734,7 +44756,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="133" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B44" s="134"/>
       <c r="C44" s="71" t="n">
@@ -44776,7 +44798,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="137" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B45" s="138"/>
       <c r="C45" s="75" t="n">
@@ -44818,7 +44840,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="137" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B46" s="138"/>
       <c r="C46" s="75" t="n">
@@ -44860,7 +44882,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="137" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B47" s="138"/>
       <c r="C47" s="75" t="n">
@@ -44902,7 +44924,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="144" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B48" s="145"/>
       <c r="C48" s="78" t="n">
@@ -44957,7 +44979,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="106" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B50" s="120"/>
       <c r="C50" s="7" t="n">
@@ -44999,7 +45021,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="114" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B51" s="122"/>
       <c r="C51" s="90" t="n">
@@ -45053,7 +45075,7 @@
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="154"/>
       <c r="B53" s="155" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C53" s="156" t="n">
         <f aca="false">AVERAGE(C44:C48)</f>
@@ -45095,7 +45117,7 @@
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="162"/>
       <c r="B54" s="163" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C54" s="164" t="n">
         <f aca="false">AVERAGE(C44:C48,C50:C51)</f>
@@ -45216,7 +45238,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="54" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B3" s="56" t="str">
         <f aca="false">Data1!A2</f>
@@ -45225,7 +45247,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="54" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B4" s="56" t="str">
         <f aca="false">Data1!G2</f>
@@ -45282,31 +45304,31 @@
         <v>38</v>
       </c>
       <c r="E9" s="64" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F9" s="63" t="s">
         <v>38</v>
       </c>
       <c r="G9" s="64" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H9" s="63" t="s">
         <v>38</v>
       </c>
       <c r="I9" s="64" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="J9" s="63" t="s">
         <v>38</v>
       </c>
       <c r="K9" s="64" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="171"/>
       <c r="B10" s="172" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C10" s="93" t="n">
         <f aca="false">CV_H!C20</f>
@@ -45348,7 +45370,7 @@
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="178"/>
       <c r="B11" s="179" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C11" s="180" t="n">
         <f aca="false">CV_H!C21</f>
@@ -45389,19 +45411,19 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="52" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="186" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B32" s="186"/>
       <c r="C32" s="186"/>
       <c r="D32" s="186"/>
       <c r="E32" s="80"/>
       <c r="F32" s="186" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="G32" s="186"/>
       <c r="H32" s="186"/>
@@ -45409,19 +45431,19 @@
     </row>
     <row r="33" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="186" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B33" s="186" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C33" s="186" t="s">
         <v>81</v>
       </c>
       <c r="D33" s="187" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F33" s="186" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G33" s="186"/>
       <c r="H33" s="186" t="str">
@@ -45429,7 +45451,7 @@
         <v>% de TJMO</v>
       </c>
       <c r="I33" s="187" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -45470,7 +45492,7 @@
         <v>21.6</v>
       </c>
       <c r="F35" s="192" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G35" s="192"/>
       <c r="H35" s="193"/>
@@ -45493,7 +45515,7 @@
         <v>18.2</v>
       </c>
       <c r="F36" s="192" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="G36" s="192"/>
       <c r="H36" s="193" t="n">
@@ -45543,7 +45565,7 @@
         <v>75.4</v>
       </c>
       <c r="F38" s="192" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="G38" s="192"/>
       <c r="H38" s="193"/>
@@ -45566,7 +45588,7 @@
         <v>160.6</v>
       </c>
       <c r="F39" s="192" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G39" s="192"/>
       <c r="H39" s="193" t="n">
@@ -45616,7 +45638,7 @@
         <v>1138.6</v>
       </c>
       <c r="F41" s="192" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="G41" s="192"/>
       <c r="H41" s="193"/>
@@ -45639,7 +45661,7 @@
         <v>887.4</v>
       </c>
       <c r="F42" s="192" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G42" s="192"/>
       <c r="H42" s="193" t="n">
@@ -45689,7 +45711,7 @@
         <v>737</v>
       </c>
       <c r="F44" s="192" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G44" s="192"/>
       <c r="H44" s="193"/>
@@ -45712,7 +45734,7 @@
         <v>924.2</v>
       </c>
       <c r="F45" s="192" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="G45" s="192"/>
       <c r="H45" s="193" t="n">
@@ -45762,7 +45784,7 @@
         <v>987.6</v>
       </c>
       <c r="F47" s="192" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="G47" s="192"/>
       <c r="H47" s="193"/>
@@ -45785,7 +45807,7 @@
         <v>826.8</v>
       </c>
       <c r="F48" s="192" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="G48" s="192"/>
       <c r="H48" s="193" t="n">
@@ -45835,7 +45857,7 @@
         <v>1224.2</v>
       </c>
       <c r="F50" s="203" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="G50" s="203"/>
       <c r="H50" s="203"/>
@@ -45893,10 +45915,10 @@
         <v>% de TJMO</v>
       </c>
       <c r="I52" s="186" t="s">
+        <v>254</v>
+      </c>
+      <c r="J52" s="186" t="s">
         <v>252</v>
-      </c>
-      <c r="J52" s="186" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -45938,7 +45960,7 @@
         <v>485.4</v>
       </c>
       <c r="F54" s="192" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="G54" s="192"/>
       <c r="H54" s="207" t="n">
@@ -45993,7 +46015,7 @@
         <v>389.4</v>
       </c>
       <c r="F56" s="192" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="G56" s="192"/>
       <c r="H56" s="207" t="n">

</xml_diff>

<commit_message>
Remove char. speeds from Vit_H
</commit_message>
<xml_diff>
--- a/comptages/report/template.xlsx
+++ b/comptages/report/template.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="191">
   <si>
     <t xml:space="preserve">Data of the count</t>
   </si>
@@ -555,9 +555,6 @@
     <t xml:space="preserve">Véhicules légers : MR (2) + PW (3) + PW+AH(4) + LIE (5) + LIE+AH(6) + LIE+AL(7)</t>
   </si>
   <si>
-    <t xml:space="preserve">Vitesses caractéristiques</t>
-  </si>
-  <si>
     <t xml:space="preserve">30 km/h</t>
   </si>
   <si>
@@ -597,6 +594,18 @@
     <t xml:space="preserve">Véh/h</t>
   </si>
   <si>
+    <t xml:space="preserve">Vitesses caractéristiques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 120 km/h</t>
+  </si>
+  <si>
     <t xml:space="preserve">V15</t>
   </si>
   <si>
@@ -607,15 +616,6 @@
   </si>
   <si>
     <t xml:space="preserve">Vmt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 km/h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 km/h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt; 120 km/h</t>
   </si>
 </sst>
 </file>
@@ -2873,12 +2873,40 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2905,24 +2933,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="175" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2933,10 +2949,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2945,20 +2957,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3085,7 +3085,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="1" sqref="J7 K5"/>
+      <selection pane="topLeft" activeCell="K5" activeCellId="1" sqref="H7 K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3215,7 +3215,7 @@
   <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P55" activeCellId="1" sqref="J7 P55"/>
+      <selection pane="topLeft" activeCell="P55" activeCellId="1" sqref="H7 P55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6515,7 +6515,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -6529,7 +6529,7 @@
   <dimension ref="A1:N76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="1" sqref="J7 K9"/>
+      <selection pane="topLeft" activeCell="K9" activeCellId="1" sqref="H7 K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8158,7 +8158,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -8172,7 +8172,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8207,15 +8207,17 @@
         <v>Periode de comptage du 8/5/2017 au 15/5/2017</v>
       </c>
       <c r="G2" s="0"/>
-      <c r="J2" s="15" t="str">
+      <c r="H2" s="15" t="str">
         <f aca="false">Data_count!B5</f>
         <v>Comptage 2017</v>
       </c>
-      <c r="P2" s="0"/>
-      <c r="U2" s="13" t="str">
+      <c r="J2" s="0"/>
+      <c r="O2" s="13" t="str">
         <f aca="false">Data_count!B6</f>
         <v>Type de capteur : Boucle</v>
       </c>
+      <c r="P2" s="0"/>
+      <c r="U2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="str">
@@ -8224,11 +8226,12 @@
       </c>
       <c r="G3" s="15"/>
       <c r="J3" s="11"/>
-      <c r="P3" s="0"/>
-      <c r="U3" s="16" t="str">
+      <c r="O3" s="16" t="str">
         <f aca="false">Data_count!B7</f>
         <v>Modèle : M660_LT</v>
       </c>
+      <c r="P3" s="0"/>
+      <c r="U3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
@@ -8239,11 +8242,12 @@
         <v>Peseux Gir. de la Maison de Commune</v>
       </c>
       <c r="J4" s="11"/>
-      <c r="P4" s="0"/>
-      <c r="U4" s="16" t="str">
+      <c r="O4" s="16" t="str">
         <f aca="false">Data_count!B8</f>
         <v>Classification : SWISS10</v>
       </c>
+      <c r="P4" s="0"/>
+      <c r="U4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
@@ -8254,11 +8258,12 @@
         <v>Auvernier Gir. de Brena</v>
       </c>
       <c r="J5" s="11"/>
-      <c r="P5" s="0"/>
-      <c r="U5" s="16" t="str">
+      <c r="O5" s="16" t="str">
         <f aca="false">Data_count!B9</f>
         <v>Comptage véhicule par véhicule</v>
       </c>
+      <c r="P5" s="0"/>
+      <c r="U5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="14"/>
@@ -8271,10 +8276,11 @@
       <c r="C7" s="18"/>
       <c r="F7" s="0"/>
       <c r="G7" s="20"/>
-      <c r="J7" s="19" t="str">
+      <c r="H7" s="19" t="str">
         <f aca="false">Data_count!B11</f>
         <v>Rte de la Gare</v>
       </c>
+      <c r="J7" s="0"/>
       <c r="K7" s="11"/>
       <c r="N7" s="118"/>
     </row>
@@ -8309,6 +8315,10 @@
       <c r="O11" s="293"/>
       <c r="P11" s="293"/>
       <c r="Q11" s="294"/>
+      <c r="R11" s="0"/>
+      <c r="S11" s="0"/>
+      <c r="T11" s="0"/>
+      <c r="U11" s="0"/>
     </row>
     <row r="12" s="186" customFormat="true" ht="18.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="247" t="str">
@@ -8330,12 +8340,10 @@
         <v>135</v>
       </c>
       <c r="P12" s="285"/>
-      <c r="R12" s="295" t="s">
-        <v>170</v>
-      </c>
-      <c r="S12" s="295"/>
-      <c r="T12" s="295"/>
-      <c r="U12" s="295"/>
+      <c r="R12" s="0"/>
+      <c r="S12" s="0"/>
+      <c r="T12" s="0"/>
+      <c r="U12" s="0"/>
       <c r="AMF12" s="1"/>
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
@@ -8347,57 +8355,49 @@
         <v>110</v>
       </c>
       <c r="B13" s="248" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="150" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="150" t="s">
+      <c r="D13" s="150" t="s">
         <v>172</v>
       </c>
-      <c r="D13" s="150" t="s">
+      <c r="E13" s="150" t="s">
         <v>173</v>
       </c>
-      <c r="E13" s="150" t="s">
+      <c r="F13" s="150" t="s">
         <v>174</v>
       </c>
-      <c r="F13" s="150" t="s">
+      <c r="G13" s="150" t="s">
         <v>175</v>
       </c>
-      <c r="G13" s="150" t="s">
+      <c r="H13" s="150" t="s">
         <v>176</v>
       </c>
-      <c r="H13" s="150" t="s">
+      <c r="I13" s="150" t="s">
         <v>177</v>
       </c>
-      <c r="I13" s="150" t="s">
+      <c r="J13" s="150" t="s">
         <v>178</v>
       </c>
-      <c r="J13" s="150" t="s">
+      <c r="K13" s="150" t="s">
         <v>179</v>
       </c>
-      <c r="K13" s="150" t="s">
+      <c r="L13" s="150" t="s">
         <v>180</v>
       </c>
-      <c r="L13" s="150" t="s">
+      <c r="M13" s="251" t="s">
         <v>181</v>
       </c>
-      <c r="M13" s="251" t="s">
+      <c r="O13" s="295" t="s">
         <v>182</v>
       </c>
-      <c r="O13" s="296" t="s">
-        <v>183</v>
-      </c>
       <c r="P13" s="118"/>
-      <c r="R13" s="297" t="s">
-        <v>184</v>
-      </c>
-      <c r="S13" s="298" t="s">
-        <v>185</v>
-      </c>
-      <c r="T13" s="299" t="s">
-        <v>186</v>
-      </c>
-      <c r="U13" s="300" t="s">
-        <v>187</v>
-      </c>
+      <c r="R13" s="0"/>
+      <c r="S13" s="0"/>
+      <c r="T13" s="0"/>
+      <c r="U13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="226" t="s">
@@ -8456,22 +8456,10 @@
         <v>54</v>
       </c>
       <c r="P14" s="177"/>
-      <c r="R14" s="301" t="n">
-        <f aca="false">Data_speed!P5</f>
-        <v>45</v>
-      </c>
-      <c r="S14" s="301" t="n">
-        <f aca="false">Data_speed!Q5</f>
-        <v>55</v>
-      </c>
-      <c r="T14" s="301" t="n">
-        <f aca="false">Data_speed!R5</f>
-        <v>55</v>
-      </c>
-      <c r="U14" s="302" t="n">
-        <f aca="false">Data_speed!S5</f>
-        <v>51.65</v>
-      </c>
+      <c r="R14" s="0"/>
+      <c r="S14" s="0"/>
+      <c r="T14" s="0"/>
+      <c r="U14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="229" t="s">
@@ -8530,22 +8518,10 @@
         <v>22.2857142857143</v>
       </c>
       <c r="P15" s="177"/>
-      <c r="R15" s="301" t="n">
-        <f aca="false">Data_speed!P6</f>
-        <v>45</v>
-      </c>
-      <c r="S15" s="301" t="n">
-        <f aca="false">Data_speed!Q6</f>
-        <v>55</v>
-      </c>
-      <c r="T15" s="301" t="n">
-        <f aca="false">Data_speed!R6</f>
-        <v>55</v>
-      </c>
-      <c r="U15" s="302" t="n">
-        <f aca="false">Data_speed!S6</f>
-        <v>51.96</v>
-      </c>
+      <c r="R15" s="0"/>
+      <c r="S15" s="0"/>
+      <c r="T15" s="0"/>
+      <c r="U15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="229" t="s">
@@ -8604,22 +8580,10 @@
         <v>15.5714285714286</v>
       </c>
       <c r="P16" s="177"/>
-      <c r="R16" s="301" t="n">
-        <f aca="false">Data_speed!P7</f>
-        <v>45</v>
-      </c>
-      <c r="S16" s="301" t="n">
-        <f aca="false">Data_speed!Q7</f>
-        <v>55</v>
-      </c>
-      <c r="T16" s="301" t="n">
-        <f aca="false">Data_speed!R7</f>
-        <v>55</v>
-      </c>
-      <c r="U16" s="302" t="n">
-        <f aca="false">Data_speed!S7</f>
-        <v>52.22</v>
-      </c>
+      <c r="R16" s="0"/>
+      <c r="S16" s="0"/>
+      <c r="T16" s="0"/>
+      <c r="U16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="229" t="s">
@@ -8678,22 +8642,10 @@
         <v>13.8571428571429</v>
       </c>
       <c r="P17" s="177"/>
-      <c r="R17" s="301" t="n">
-        <f aca="false">Data_speed!P8</f>
-        <v>45</v>
-      </c>
-      <c r="S17" s="301" t="n">
-        <f aca="false">Data_speed!Q8</f>
-        <v>55</v>
-      </c>
-      <c r="T17" s="301" t="n">
-        <f aca="false">Data_speed!R8</f>
-        <v>65</v>
-      </c>
-      <c r="U17" s="302" t="n">
-        <f aca="false">Data_speed!S8</f>
-        <v>53.66</v>
-      </c>
+      <c r="R17" s="0"/>
+      <c r="S17" s="0"/>
+      <c r="T17" s="0"/>
+      <c r="U17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="229" t="s">
@@ -8752,22 +8704,10 @@
         <v>19.2857142857143</v>
       </c>
       <c r="P18" s="177"/>
-      <c r="R18" s="301" t="n">
-        <f aca="false">Data_speed!P9</f>
-        <v>45</v>
-      </c>
-      <c r="S18" s="301" t="n">
-        <f aca="false">Data_speed!Q9</f>
-        <v>55</v>
-      </c>
-      <c r="T18" s="301" t="n">
-        <f aca="false">Data_speed!R9</f>
-        <v>65</v>
-      </c>
-      <c r="U18" s="302" t="n">
-        <f aca="false">Data_speed!S9</f>
-        <v>54.76</v>
-      </c>
+      <c r="R18" s="0"/>
+      <c r="S18" s="0"/>
+      <c r="T18" s="0"/>
+      <c r="U18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="229" t="s">
@@ -8826,22 +8766,10 @@
         <v>43.4285714285714</v>
       </c>
       <c r="P19" s="177"/>
-      <c r="R19" s="301" t="n">
-        <f aca="false">Data_speed!P10</f>
-        <v>45</v>
-      </c>
-      <c r="S19" s="301" t="n">
-        <f aca="false">Data_speed!Q10</f>
-        <v>55</v>
-      </c>
-      <c r="T19" s="301" t="n">
-        <f aca="false">Data_speed!R10</f>
-        <v>55</v>
-      </c>
-      <c r="U19" s="302" t="n">
-        <f aca="false">Data_speed!S10</f>
-        <v>51.38</v>
-      </c>
+      <c r="R19" s="0"/>
+      <c r="S19" s="0"/>
+      <c r="T19" s="0"/>
+      <c r="U19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="222" t="s">
@@ -8900,22 +8828,10 @@
         <v>172.714285714286</v>
       </c>
       <c r="P20" s="177"/>
-      <c r="R20" s="301" t="n">
-        <f aca="false">Data_speed!P11</f>
-        <v>45</v>
-      </c>
-      <c r="S20" s="301" t="n">
-        <f aca="false">Data_speed!Q11</f>
-        <v>45</v>
-      </c>
-      <c r="T20" s="301" t="n">
-        <f aca="false">Data_speed!R11</f>
-        <v>55</v>
-      </c>
-      <c r="U20" s="302" t="n">
-        <f aca="false">Data_speed!S11</f>
-        <v>49.76</v>
-      </c>
+      <c r="R20" s="0"/>
+      <c r="S20" s="0"/>
+      <c r="T20" s="0"/>
+      <c r="U20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="226" t="s">
@@ -8974,22 +8890,10 @@
         <v>363</v>
       </c>
       <c r="P21" s="177"/>
-      <c r="R21" s="301" t="n">
-        <f aca="false">Data_speed!P12</f>
-        <v>45</v>
-      </c>
-      <c r="S21" s="301" t="n">
-        <f aca="false">Data_speed!Q12</f>
-        <v>45</v>
-      </c>
-      <c r="T21" s="301" t="n">
-        <f aca="false">Data_speed!R12</f>
-        <v>55</v>
-      </c>
-      <c r="U21" s="302" t="n">
-        <f aca="false">Data_speed!S12</f>
-        <v>48.05</v>
-      </c>
+      <c r="R21" s="0"/>
+      <c r="S21" s="0"/>
+      <c r="T21" s="0"/>
+      <c r="U21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="226" t="s">
@@ -9048,22 +8952,10 @@
         <v>333.714285714286</v>
       </c>
       <c r="P22" s="177"/>
-      <c r="R22" s="301" t="n">
-        <f aca="false">Data_speed!P13</f>
-        <v>45</v>
-      </c>
-      <c r="S22" s="301" t="n">
-        <f aca="false">Data_speed!Q13</f>
-        <v>45</v>
-      </c>
-      <c r="T22" s="301" t="n">
-        <f aca="false">Data_speed!R13</f>
-        <v>55</v>
-      </c>
-      <c r="U22" s="302" t="n">
-        <f aca="false">Data_speed!S13</f>
-        <v>49.24</v>
-      </c>
+      <c r="R22" s="0"/>
+      <c r="S22" s="0"/>
+      <c r="T22" s="0"/>
+      <c r="U22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="229" t="s">
@@ -9122,22 +9014,10 @@
         <v>317.285714285714</v>
       </c>
       <c r="P23" s="177"/>
-      <c r="R23" s="301" t="n">
-        <f aca="false">Data_speed!P14</f>
-        <v>45</v>
-      </c>
-      <c r="S23" s="301" t="n">
-        <f aca="false">Data_speed!Q14</f>
-        <v>45</v>
-      </c>
-      <c r="T23" s="301" t="n">
-        <f aca="false">Data_speed!R14</f>
-        <v>55</v>
-      </c>
-      <c r="U23" s="302" t="n">
-        <f aca="false">Data_speed!S14</f>
-        <v>49.03</v>
-      </c>
+      <c r="R23" s="0"/>
+      <c r="S23" s="0"/>
+      <c r="T23" s="0"/>
+      <c r="U23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="229" t="s">
@@ -9196,22 +9076,10 @@
         <v>340.857142857143</v>
       </c>
       <c r="P24" s="177"/>
-      <c r="R24" s="301" t="n">
-        <f aca="false">Data_speed!P15</f>
-        <v>45</v>
-      </c>
-      <c r="S24" s="301" t="n">
-        <f aca="false">Data_speed!Q15</f>
-        <v>45</v>
-      </c>
-      <c r="T24" s="301" t="n">
-        <f aca="false">Data_speed!R15</f>
-        <v>55</v>
-      </c>
-      <c r="U24" s="302" t="n">
-        <f aca="false">Data_speed!S15</f>
-        <v>48.33</v>
-      </c>
+      <c r="R24" s="0"/>
+      <c r="S24" s="0"/>
+      <c r="T24" s="0"/>
+      <c r="U24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="229" t="s">
@@ -9270,22 +9138,10 @@
         <v>445.857142857143</v>
       </c>
       <c r="P25" s="177"/>
-      <c r="R25" s="301" t="n">
-        <f aca="false">Data_speed!P16</f>
-        <v>45</v>
-      </c>
-      <c r="S25" s="301" t="n">
-        <f aca="false">Data_speed!Q16</f>
-        <v>45</v>
-      </c>
-      <c r="T25" s="301" t="n">
-        <f aca="false">Data_speed!R16</f>
-        <v>55</v>
-      </c>
-      <c r="U25" s="302" t="n">
-        <f aca="false">Data_speed!S16</f>
-        <v>48.52</v>
-      </c>
+      <c r="R25" s="0"/>
+      <c r="S25" s="0"/>
+      <c r="T25" s="0"/>
+      <c r="U25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="256" t="s">
@@ -9344,22 +9200,10 @@
         <v>413.285714285714</v>
       </c>
       <c r="P26" s="177"/>
-      <c r="R26" s="301" t="n">
-        <f aca="false">Data_speed!P17</f>
-        <v>45</v>
-      </c>
-      <c r="S26" s="301" t="n">
-        <f aca="false">Data_speed!Q17</f>
-        <v>45</v>
-      </c>
-      <c r="T26" s="301" t="n">
-        <f aca="false">Data_speed!R17</f>
-        <v>55</v>
-      </c>
-      <c r="U26" s="302" t="n">
-        <f aca="false">Data_speed!S17</f>
-        <v>49.07</v>
-      </c>
+      <c r="R26" s="0"/>
+      <c r="S26" s="0"/>
+      <c r="T26" s="0"/>
+      <c r="U26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="229" t="s">
@@ -9418,22 +9262,10 @@
         <v>420.285714285714</v>
       </c>
       <c r="P27" s="177"/>
-      <c r="R27" s="301" t="n">
-        <f aca="false">Data_speed!P18</f>
-        <v>45</v>
-      </c>
-      <c r="S27" s="301" t="n">
-        <f aca="false">Data_speed!Q18</f>
-        <v>45</v>
-      </c>
-      <c r="T27" s="301" t="n">
-        <f aca="false">Data_speed!R18</f>
-        <v>55</v>
-      </c>
-      <c r="U27" s="302" t="n">
-        <f aca="false">Data_speed!S18</f>
-        <v>48.72</v>
-      </c>
+      <c r="R27" s="0"/>
+      <c r="S27" s="0"/>
+      <c r="T27" s="0"/>
+      <c r="U27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="229" t="s">
@@ -9492,22 +9324,10 @@
         <v>382.142857142857</v>
       </c>
       <c r="P28" s="177"/>
-      <c r="R28" s="301" t="n">
-        <f aca="false">Data_speed!P19</f>
-        <v>45</v>
-      </c>
-      <c r="S28" s="301" t="n">
-        <f aca="false">Data_speed!Q19</f>
-        <v>45</v>
-      </c>
-      <c r="T28" s="301" t="n">
-        <f aca="false">Data_speed!R19</f>
-        <v>55</v>
-      </c>
-      <c r="U28" s="302" t="n">
-        <f aca="false">Data_speed!S19</f>
-        <v>49.16</v>
-      </c>
+      <c r="R28" s="0"/>
+      <c r="S28" s="0"/>
+      <c r="T28" s="0"/>
+      <c r="U28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="229" t="s">
@@ -9566,22 +9386,10 @@
         <v>440</v>
       </c>
       <c r="P29" s="177"/>
-      <c r="R29" s="301" t="n">
-        <f aca="false">Data_speed!P20</f>
-        <v>45</v>
-      </c>
-      <c r="S29" s="301" t="n">
-        <f aca="false">Data_speed!Q20</f>
-        <v>45</v>
-      </c>
-      <c r="T29" s="301" t="n">
-        <f aca="false">Data_speed!R20</f>
-        <v>55</v>
-      </c>
-      <c r="U29" s="302" t="n">
-        <f aca="false">Data_speed!S20</f>
-        <v>48.93</v>
-      </c>
+      <c r="R29" s="0"/>
+      <c r="S29" s="0"/>
+      <c r="T29" s="0"/>
+      <c r="U29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="222" t="s">
@@ -9640,22 +9448,10 @@
         <v>588.857142857143</v>
       </c>
       <c r="P30" s="177"/>
-      <c r="R30" s="301" t="n">
-        <f aca="false">Data_speed!P21</f>
-        <v>45</v>
-      </c>
-      <c r="S30" s="301" t="n">
-        <f aca="false">Data_speed!Q21</f>
-        <v>45</v>
-      </c>
-      <c r="T30" s="301" t="n">
-        <f aca="false">Data_speed!R21</f>
-        <v>55</v>
-      </c>
-      <c r="U30" s="302" t="n">
-        <f aca="false">Data_speed!S21</f>
-        <v>48.25</v>
-      </c>
+      <c r="R30" s="0"/>
+      <c r="S30" s="0"/>
+      <c r="T30" s="0"/>
+      <c r="U30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="226" t="s">
@@ -9714,22 +9510,10 @@
         <v>823.428571428572</v>
       </c>
       <c r="P31" s="177"/>
-      <c r="R31" s="301" t="n">
-        <f aca="false">Data_speed!P22</f>
-        <v>45</v>
-      </c>
-      <c r="S31" s="301" t="n">
-        <f aca="false">Data_speed!Q22</f>
-        <v>45</v>
-      </c>
-      <c r="T31" s="301" t="n">
-        <f aca="false">Data_speed!R22</f>
-        <v>55</v>
-      </c>
-      <c r="U31" s="302" t="n">
-        <f aca="false">Data_speed!S22</f>
-        <v>46.72</v>
-      </c>
+      <c r="R31" s="0"/>
+      <c r="S31" s="0"/>
+      <c r="T31" s="0"/>
+      <c r="U31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="226" t="s">
@@ -9788,22 +9572,10 @@
         <v>620</v>
       </c>
       <c r="P32" s="177"/>
-      <c r="R32" s="301" t="n">
-        <f aca="false">Data_speed!P23</f>
-        <v>45</v>
-      </c>
-      <c r="S32" s="301" t="n">
-        <f aca="false">Data_speed!Q23</f>
-        <v>45</v>
-      </c>
-      <c r="T32" s="301" t="n">
-        <f aca="false">Data_speed!R23</f>
-        <v>55</v>
-      </c>
-      <c r="U32" s="302" t="n">
-        <f aca="false">Data_speed!S23</f>
-        <v>48.2</v>
-      </c>
+      <c r="R32" s="0"/>
+      <c r="S32" s="0"/>
+      <c r="T32" s="0"/>
+      <c r="U32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="229" t="s">
@@ -9862,22 +9634,10 @@
         <v>344.857142857143</v>
       </c>
       <c r="P33" s="177"/>
-      <c r="R33" s="301" t="n">
-        <f aca="false">Data_speed!P24</f>
-        <v>45</v>
-      </c>
-      <c r="S33" s="301" t="n">
-        <f aca="false">Data_speed!Q24</f>
-        <v>45</v>
-      </c>
-      <c r="T33" s="301" t="n">
-        <f aca="false">Data_speed!R24</f>
-        <v>55</v>
-      </c>
-      <c r="U33" s="302" t="n">
-        <f aca="false">Data_speed!S24</f>
-        <v>50.28</v>
-      </c>
+      <c r="R33" s="0"/>
+      <c r="S33" s="0"/>
+      <c r="T33" s="0"/>
+      <c r="U33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="229" t="s">
@@ -9936,22 +9696,10 @@
         <v>244.428571428571</v>
       </c>
       <c r="P34" s="177"/>
-      <c r="R34" s="301" t="n">
-        <f aca="false">Data_speed!P25</f>
-        <v>45</v>
-      </c>
-      <c r="S34" s="301" t="n">
-        <f aca="false">Data_speed!Q25</f>
-        <v>45</v>
-      </c>
-      <c r="T34" s="301" t="n">
-        <f aca="false">Data_speed!R25</f>
-        <v>55</v>
-      </c>
-      <c r="U34" s="302" t="n">
-        <f aca="false">Data_speed!S25</f>
-        <v>50.03</v>
-      </c>
+      <c r="R34" s="0"/>
+      <c r="S34" s="0"/>
+      <c r="T34" s="0"/>
+      <c r="U34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="229" t="s">
@@ -10010,22 +9758,10 @@
         <v>224.285714285714</v>
       </c>
       <c r="P35" s="177"/>
-      <c r="R35" s="301" t="n">
-        <f aca="false">Data_speed!P26</f>
-        <v>45</v>
-      </c>
-      <c r="S35" s="301" t="n">
-        <f aca="false">Data_speed!Q26</f>
-        <v>45</v>
-      </c>
-      <c r="T35" s="301" t="n">
-        <f aca="false">Data_speed!R26</f>
-        <v>55</v>
-      </c>
-      <c r="U35" s="302" t="n">
-        <f aca="false">Data_speed!S26</f>
-        <v>48.9</v>
-      </c>
+      <c r="R35" s="0"/>
+      <c r="S35" s="0"/>
+      <c r="T35" s="0"/>
+      <c r="U35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="229" t="s">
@@ -10084,22 +9820,10 @@
         <v>194.428571428571</v>
       </c>
       <c r="P36" s="177"/>
-      <c r="R36" s="301" t="n">
-        <f aca="false">Data_speed!P27</f>
-        <v>45</v>
-      </c>
-      <c r="S36" s="301" t="n">
-        <f aca="false">Data_speed!Q27</f>
-        <v>45</v>
-      </c>
-      <c r="T36" s="301" t="n">
-        <f aca="false">Data_speed!R27</f>
-        <v>55</v>
-      </c>
-      <c r="U36" s="302" t="n">
-        <f aca="false">Data_speed!S27</f>
-        <v>49.09</v>
-      </c>
+      <c r="R36" s="0"/>
+      <c r="S36" s="0"/>
+      <c r="T36" s="0"/>
+      <c r="U36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="231" t="s">
@@ -10158,85 +9882,73 @@
         <v>111.142857142857</v>
       </c>
       <c r="P37" s="177"/>
-      <c r="R37" s="301" t="n">
-        <f aca="false">Data_speed!P28</f>
-        <v>45</v>
-      </c>
-      <c r="S37" s="301" t="n">
-        <f aca="false">Data_speed!Q28</f>
-        <v>55</v>
-      </c>
-      <c r="T37" s="301" t="n">
-        <f aca="false">Data_speed!R28</f>
-        <v>55</v>
-      </c>
-      <c r="U37" s="302" t="n">
-        <f aca="false">Data_speed!S28</f>
-        <v>50.4</v>
-      </c>
+      <c r="R37" s="0"/>
+      <c r="S37" s="0"/>
+      <c r="T37" s="0"/>
+      <c r="U37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="R38" s="179"/>
-      <c r="S38" s="179"/>
-      <c r="T38" s="179"/>
-      <c r="U38" s="179"/>
+      <c r="R38" s="0"/>
+      <c r="S38" s="0"/>
+      <c r="T38" s="0"/>
+      <c r="U38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="M39" s="303"/>
-      <c r="R39" s="179"/>
-      <c r="S39" s="179"/>
-      <c r="T39" s="179"/>
-      <c r="U39" s="179"/>
+      <c r="M39" s="296"/>
+      <c r="R39" s="0"/>
+      <c r="S39" s="0"/>
+      <c r="T39" s="0"/>
+      <c r="U39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="304" t="n">
+      <c r="B40" s="297" t="n">
         <f aca="false">SUM(B14:B37)/Data_speed!$O$29</f>
         <v>0.00125400871638845</v>
       </c>
-      <c r="C40" s="304" t="n">
+      <c r="C40" s="297" t="n">
         <f aca="false">SUM(C14:C37)/Data_speed!$O$29</f>
         <v>0.00696899925992928</v>
       </c>
-      <c r="D40" s="304" t="n">
+      <c r="D40" s="297" t="n">
         <f aca="false">SUM(D14:D37)/Data_speed!$O$29</f>
         <v>0.0324603239865143</v>
       </c>
-      <c r="E40" s="304" t="n">
+      <c r="E40" s="297" t="n">
         <f aca="false">SUM(E14:E37)/Data_speed!$O$29</f>
         <v>0.559637365348244</v>
       </c>
-      <c r="F40" s="304" t="n">
+      <c r="F40" s="297" t="n">
         <f aca="false">SUM(F14:F37)/Data_speed!$O$29</f>
         <v>0.379245127867774</v>
       </c>
-      <c r="G40" s="304" t="n">
+      <c r="G40" s="297" t="n">
         <f aca="false">SUM(G14:G37)/Data_speed!$O$29</f>
         <v>0.0191801661047611</v>
       </c>
-      <c r="H40" s="304" t="n">
+      <c r="H40" s="297" t="n">
         <f aca="false">SUM(H14:H37)/Data_speed!$O$29</f>
         <v>0.000801743277690979</v>
       </c>
-      <c r="I40" s="304" t="n">
+      <c r="I40" s="297" t="n">
         <f aca="false">SUM(I14:I37)/Data_speed!$O$29</f>
         <v>0.000205575199407943</v>
       </c>
-      <c r="J40" s="304" t="n">
+      <c r="J40" s="297" t="n">
         <f aca="false">SUM(J14:J37)/Data_speed!$O$29</f>
         <v>4.11150398815887E-005</v>
       </c>
-      <c r="K40" s="304" t="n">
+      <c r="K40" s="297" t="n">
         <f aca="false">SUM(K14:K37)/Data_speed!$O$29</f>
         <v>2.05575199407943E-005</v>
       </c>
-      <c r="L40" s="304" t="n">
+      <c r="L40" s="297" t="n">
         <f aca="false">SUM(L14:L37)/Data_speed!$O$29</f>
         <v>2.05575199407943E-005</v>
       </c>
-      <c r="M40" s="304" t="n">
+      <c r="M40" s="297" t="n">
         <f aca="false">SUM(M14:M37)/Data_speed!$O$29</f>
         <v>0.000164460159526355</v>
       </c>
@@ -10245,72 +9957,60 @@
         <v>1</v>
       </c>
       <c r="P40" s="287"/>
-      <c r="R40" s="305" t="n">
-        <f aca="false">AVERAGE(R14:R37)</f>
-        <v>45</v>
-      </c>
-      <c r="S40" s="305" t="n">
-        <f aca="false">AVERAGE(S14:S37)</f>
-        <v>47.9166666666667</v>
-      </c>
-      <c r="T40" s="305" t="n">
-        <f aca="false">AVERAGE(T14:T37)</f>
-        <v>55.8333333333333</v>
-      </c>
-      <c r="U40" s="306" t="n">
-        <f aca="false">AVERAGE(U14:U37)</f>
-        <v>49.84625</v>
-      </c>
+      <c r="R40" s="0"/>
+      <c r="S40" s="0"/>
+      <c r="T40" s="0"/>
+      <c r="U40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="237" t="s">
         <v>146</v>
       </c>
-      <c r="B41" s="307" t="n">
+      <c r="B41" s="298" t="n">
         <f aca="false">SUM(B20:B35)/Data_speed!$O$29</f>
         <v>0.00123345119644766</v>
       </c>
-      <c r="C41" s="307" t="n">
+      <c r="C41" s="298" t="n">
         <f aca="false">SUM(C20:C35)/Data_speed!$O$29</f>
         <v>0.00680453910040293</v>
       </c>
-      <c r="D41" s="307" t="n">
+      <c r="D41" s="298" t="n">
         <f aca="false">SUM(D20:D35)/Data_speed!$O$29</f>
         <v>0.0308773949510731</v>
       </c>
-      <c r="E41" s="307" t="n">
+      <c r="E41" s="298" t="n">
         <f aca="false">SUM(E20:E35)/Data_speed!$O$29</f>
         <v>0.527793766959954</v>
       </c>
-      <c r="F41" s="307" t="n">
+      <c r="F41" s="298" t="n">
         <f aca="false">SUM(F20:F35)/Data_speed!$O$29</f>
         <v>0.348778883315517</v>
       </c>
-      <c r="G41" s="307" t="n">
+      <c r="G41" s="298" t="n">
         <f aca="false">SUM(G20:G35)/Data_speed!$O$29</f>
         <v>0.0156237151550037</v>
       </c>
-      <c r="H41" s="307" t="n">
+      <c r="H41" s="298" t="n">
         <f aca="false">SUM(H20:H35)/Data_speed!$O$29</f>
         <v>0.000411150398815887</v>
       </c>
-      <c r="I41" s="307" t="n">
+      <c r="I41" s="298" t="n">
         <f aca="false">SUM(I20:I35)/Data_speed!$O$29</f>
         <v>6.1672559822383E-005</v>
       </c>
-      <c r="J41" s="307" t="n">
+      <c r="J41" s="298" t="n">
         <f aca="false">SUM(J20:J35)/Data_speed!$O$29</f>
         <v>0</v>
       </c>
-      <c r="K41" s="307" t="n">
+      <c r="K41" s="298" t="n">
         <f aca="false">SUM(K20:K35)/Data_speed!$O$29</f>
         <v>2.05575199407943E-005</v>
       </c>
-      <c r="L41" s="307" t="n">
+      <c r="L41" s="298" t="n">
         <f aca="false">SUM(L20:L35)/Data_speed!$O$29</f>
         <v>2.05575199407943E-005</v>
       </c>
-      <c r="M41" s="307" t="n">
+      <c r="M41" s="298" t="n">
         <f aca="false">SUM(M20:M35)/Data_speed!$O$29</f>
         <v>0.000164460159526355</v>
       </c>
@@ -10319,28 +10019,16 @@
         <v>0.931790148836444</v>
       </c>
       <c r="P41" s="287"/>
-      <c r="R41" s="308" t="n">
-        <f aca="false">AVERAGE(R20:R35)</f>
-        <v>45</v>
-      </c>
-      <c r="S41" s="308" t="n">
-        <f aca="false">AVERAGE(S20:S35)</f>
-        <v>45</v>
-      </c>
-      <c r="T41" s="308" t="n">
-        <f aca="false">AVERAGE(T20:T35)</f>
-        <v>55</v>
-      </c>
-      <c r="U41" s="309" t="n">
-        <f aca="false">AVERAGE(U20:U35)</f>
-        <v>48.824375</v>
-      </c>
+      <c r="R41" s="0"/>
+      <c r="S41" s="0"/>
+      <c r="T41" s="0"/>
+      <c r="U41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="B42" s="310" t="n">
+      <c r="B42" s="299" t="n">
         <f aca="false">B40-B41</f>
         <v>2.05575199407942E-005</v>
       </c>
@@ -10394,22 +10082,10 @@
         <v>0.0682098511635557</v>
       </c>
       <c r="P42" s="287"/>
-      <c r="R42" s="311" t="n">
-        <f aca="false">AVERAGE(AVERAGE(R14:R19), AVERAGE(R36:R37))</f>
-        <v>45</v>
-      </c>
-      <c r="S42" s="311" t="n">
-        <f aca="false">AVERAGE(AVERAGE(S14:S19), AVERAGE(S36:S37))</f>
-        <v>52.5</v>
-      </c>
-      <c r="T42" s="311" t="n">
-        <f aca="false">AVERAGE(AVERAGE(T14:T19), AVERAGE(T36:T37))</f>
-        <v>56.6666666666667</v>
-      </c>
-      <c r="U42" s="312" t="n">
-        <f aca="false">AVERAGE(AVERAGE(U14:U19), AVERAGE(U36:U37))</f>
-        <v>51.175</v>
-      </c>
+      <c r="R42" s="0"/>
+      <c r="S42" s="0"/>
+      <c r="T42" s="0"/>
+      <c r="U42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="11"/>
@@ -10453,6 +10129,10 @@
       <c r="O47" s="293"/>
       <c r="P47" s="293"/>
       <c r="Q47" s="294"/>
+      <c r="R47" s="0"/>
+      <c r="S47" s="0"/>
+      <c r="T47" s="0"/>
+      <c r="U47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="247" t="str">
@@ -10476,13 +10156,10 @@
       </c>
       <c r="P48" s="285"/>
       <c r="Q48" s="186"/>
-      <c r="R48" s="295" t="str">
-        <f aca="false">R12</f>
-        <v>Vitesses caractéristiques</v>
-      </c>
-      <c r="S48" s="295"/>
-      <c r="T48" s="295"/>
-      <c r="U48" s="295"/>
+      <c r="R48" s="0"/>
+      <c r="S48" s="0"/>
+      <c r="T48" s="0"/>
+      <c r="U48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="221" t="s">
@@ -10516,7 +10193,7 @@
         <f aca="false">H13</f>
         <v>90 km/h</v>
       </c>
-      <c r="I49" s="313" t="str">
+      <c r="I49" s="300" t="str">
         <f aca="false">I13</f>
         <v>100 km/h</v>
       </c>
@@ -10528,7 +10205,7 @@
         <f aca="false">K13</f>
         <v>120 km/h</v>
       </c>
-      <c r="L49" s="314" t="str">
+      <c r="L49" s="301" t="str">
         <f aca="false">L13</f>
         <v>130 km/h</v>
       </c>
@@ -10536,27 +10213,15 @@
         <f aca="false">M13</f>
         <v>&gt; 130 km/h</v>
       </c>
-      <c r="O49" s="296" t="str">
+      <c r="O49" s="295" t="str">
         <f aca="false">O13</f>
         <v>Véh/h</v>
       </c>
       <c r="P49" s="118"/>
-      <c r="R49" s="297" t="str">
-        <f aca="false">R13</f>
-        <v>V15</v>
-      </c>
-      <c r="S49" s="298" t="str">
-        <f aca="false">S13</f>
-        <v>V50</v>
-      </c>
-      <c r="T49" s="299" t="str">
-        <f aca="false">T13</f>
-        <v>V85</v>
-      </c>
-      <c r="U49" s="315" t="str">
-        <f aca="false">U13</f>
-        <v>Vmt</v>
-      </c>
+      <c r="R49" s="0"/>
+      <c r="S49" s="0"/>
+      <c r="T49" s="0"/>
+      <c r="U49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="226" t="s">
@@ -10615,22 +10280,10 @@
         <v>40.2857142857143</v>
       </c>
       <c r="P50" s="177"/>
-      <c r="R50" s="301" t="n">
-        <f aca="false">Data_speed!P33</f>
-        <v>45</v>
-      </c>
-      <c r="S50" s="301" t="n">
-        <f aca="false">Data_speed!Q33</f>
-        <v>55</v>
-      </c>
-      <c r="T50" s="301" t="n">
-        <f aca="false">Data_speed!R33</f>
-        <v>55</v>
-      </c>
-      <c r="U50" s="302" t="n">
-        <f aca="false">Data_speed!S33</f>
-        <v>50.42</v>
-      </c>
+      <c r="R50" s="0"/>
+      <c r="S50" s="0"/>
+      <c r="T50" s="0"/>
+      <c r="U50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="229" t="s">
@@ -10689,22 +10342,10 @@
         <v>19.8571428571429</v>
       </c>
       <c r="P51" s="177"/>
-      <c r="R51" s="301" t="n">
-        <f aca="false">Data_speed!P34</f>
-        <v>45</v>
-      </c>
-      <c r="S51" s="301" t="n">
-        <f aca="false">Data_speed!Q34</f>
-        <v>55</v>
-      </c>
-      <c r="T51" s="301" t="n">
-        <f aca="false">Data_speed!R34</f>
-        <v>55</v>
-      </c>
-      <c r="U51" s="302" t="n">
-        <f aca="false">Data_speed!S34</f>
-        <v>51.83</v>
-      </c>
+      <c r="R51" s="0"/>
+      <c r="S51" s="0"/>
+      <c r="T51" s="0"/>
+      <c r="U51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="229" t="s">
@@ -10763,22 +10404,10 @@
         <v>13.1428571428571</v>
       </c>
       <c r="P52" s="177"/>
-      <c r="R52" s="301" t="n">
-        <f aca="false">Data_speed!P35</f>
-        <v>45</v>
-      </c>
-      <c r="S52" s="301" t="n">
-        <f aca="false">Data_speed!Q35</f>
-        <v>55</v>
-      </c>
-      <c r="T52" s="301" t="n">
-        <f aca="false">Data_speed!R35</f>
-        <v>65</v>
-      </c>
-      <c r="U52" s="302" t="n">
-        <f aca="false">Data_speed!S35</f>
-        <v>52.39</v>
-      </c>
+      <c r="R52" s="0"/>
+      <c r="S52" s="0"/>
+      <c r="T52" s="0"/>
+      <c r="U52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="229" t="s">
@@ -10837,22 +10466,10 @@
         <v>14.8571428571429</v>
       </c>
       <c r="P53" s="177"/>
-      <c r="R53" s="301" t="n">
-        <f aca="false">Data_speed!P36</f>
-        <v>45</v>
-      </c>
-      <c r="S53" s="301" t="n">
-        <f aca="false">Data_speed!Q36</f>
-        <v>55</v>
-      </c>
-      <c r="T53" s="301" t="n">
-        <f aca="false">Data_speed!R36</f>
-        <v>55</v>
-      </c>
-      <c r="U53" s="302" t="n">
-        <f aca="false">Data_speed!S36</f>
-        <v>52.98</v>
-      </c>
+      <c r="R53" s="0"/>
+      <c r="S53" s="0"/>
+      <c r="T53" s="0"/>
+      <c r="U53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="229" t="s">
@@ -10911,22 +10528,10 @@
         <v>47</v>
       </c>
       <c r="P54" s="177"/>
-      <c r="R54" s="301" t="n">
-        <f aca="false">Data_speed!P37</f>
-        <v>45</v>
-      </c>
-      <c r="S54" s="301" t="n">
-        <f aca="false">Data_speed!Q37</f>
-        <v>55</v>
-      </c>
-      <c r="T54" s="301" t="n">
-        <f aca="false">Data_speed!R37</f>
-        <v>65</v>
-      </c>
-      <c r="U54" s="302" t="n">
-        <f aca="false">Data_speed!S37</f>
-        <v>53.21</v>
-      </c>
+      <c r="R54" s="0"/>
+      <c r="S54" s="0"/>
+      <c r="T54" s="0"/>
+      <c r="U54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="229" t="s">
@@ -10985,22 +10590,10 @@
         <v>85.4285714285714</v>
       </c>
       <c r="P55" s="177"/>
-      <c r="R55" s="301" t="n">
-        <f aca="false">Data_speed!P38</f>
-        <v>45</v>
-      </c>
-      <c r="S55" s="301" t="n">
-        <f aca="false">Data_speed!Q38</f>
-        <v>55</v>
-      </c>
-      <c r="T55" s="301" t="n">
-        <f aca="false">Data_speed!R38</f>
-        <v>55</v>
-      </c>
-      <c r="U55" s="302" t="n">
-        <f aca="false">Data_speed!S38</f>
-        <v>51.49</v>
-      </c>
+      <c r="R55" s="0"/>
+      <c r="S55" s="0"/>
+      <c r="T55" s="0"/>
+      <c r="U55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="222" t="s">
@@ -11059,22 +10652,10 @@
         <v>305.714285714286</v>
       </c>
       <c r="P56" s="177"/>
-      <c r="R56" s="301" t="n">
-        <f aca="false">Data_speed!P39</f>
-        <v>45</v>
-      </c>
-      <c r="S56" s="301" t="n">
-        <f aca="false">Data_speed!Q39</f>
-        <v>45</v>
-      </c>
-      <c r="T56" s="301" t="n">
-        <f aca="false">Data_speed!R39</f>
-        <v>55</v>
-      </c>
-      <c r="U56" s="302" t="n">
-        <f aca="false">Data_speed!S39</f>
-        <v>50.26</v>
-      </c>
+      <c r="R56" s="0"/>
+      <c r="S56" s="0"/>
+      <c r="T56" s="0"/>
+      <c r="U56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="226" t="s">
@@ -11133,22 +10714,10 @@
         <v>512.428571428571</v>
       </c>
       <c r="P57" s="177"/>
-      <c r="R57" s="301" t="n">
-        <f aca="false">Data_speed!P40</f>
-        <v>45</v>
-      </c>
-      <c r="S57" s="301" t="n">
-        <f aca="false">Data_speed!Q40</f>
-        <v>45</v>
-      </c>
-      <c r="T57" s="301" t="n">
-        <f aca="false">Data_speed!R40</f>
-        <v>55</v>
-      </c>
-      <c r="U57" s="302" t="n">
-        <f aca="false">Data_speed!S40</f>
-        <v>49.16</v>
-      </c>
+      <c r="R57" s="0"/>
+      <c r="S57" s="0"/>
+      <c r="T57" s="0"/>
+      <c r="U57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="226" t="s">
@@ -11207,22 +10776,10 @@
         <v>402.571428571429</v>
       </c>
       <c r="P58" s="177"/>
-      <c r="R58" s="301" t="n">
-        <f aca="false">Data_speed!P41</f>
-        <v>45</v>
-      </c>
-      <c r="S58" s="301" t="n">
-        <f aca="false">Data_speed!Q41</f>
-        <v>45</v>
-      </c>
-      <c r="T58" s="301" t="n">
-        <f aca="false">Data_speed!R41</f>
-        <v>55</v>
-      </c>
-      <c r="U58" s="302" t="n">
-        <f aca="false">Data_speed!S41</f>
-        <v>49.43</v>
-      </c>
+      <c r="R58" s="0"/>
+      <c r="S58" s="0"/>
+      <c r="T58" s="0"/>
+      <c r="U58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="229" t="s">
@@ -11281,22 +10838,10 @@
         <v>353.571428571429</v>
       </c>
       <c r="P59" s="177"/>
-      <c r="R59" s="301" t="n">
-        <f aca="false">Data_speed!P42</f>
-        <v>45</v>
-      </c>
-      <c r="S59" s="301" t="n">
-        <f aca="false">Data_speed!Q42</f>
-        <v>45</v>
-      </c>
-      <c r="T59" s="301" t="n">
-        <f aca="false">Data_speed!R42</f>
-        <v>55</v>
-      </c>
-      <c r="U59" s="302" t="n">
-        <f aca="false">Data_speed!S42</f>
-        <v>49.7</v>
-      </c>
+      <c r="R59" s="0"/>
+      <c r="S59" s="0"/>
+      <c r="T59" s="0"/>
+      <c r="U59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="229" t="s">
@@ -11355,22 +10900,10 @@
         <v>387.714285714286</v>
       </c>
       <c r="P60" s="177"/>
-      <c r="R60" s="301" t="n">
-        <f aca="false">Data_speed!P43</f>
-        <v>45</v>
-      </c>
-      <c r="S60" s="301" t="n">
-        <f aca="false">Data_speed!Q43</f>
-        <v>45</v>
-      </c>
-      <c r="T60" s="301" t="n">
-        <f aca="false">Data_speed!R43</f>
-        <v>55</v>
-      </c>
-      <c r="U60" s="302" t="n">
-        <f aca="false">Data_speed!S43</f>
-        <v>48.99</v>
-      </c>
+      <c r="R60" s="0"/>
+      <c r="S60" s="0"/>
+      <c r="T60" s="0"/>
+      <c r="U60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="229" t="s">
@@ -11429,22 +10962,10 @@
         <v>483.857142857143</v>
       </c>
       <c r="P61" s="177"/>
-      <c r="R61" s="301" t="n">
-        <f aca="false">Data_speed!P44</f>
-        <v>45</v>
-      </c>
-      <c r="S61" s="301" t="n">
-        <f aca="false">Data_speed!Q44</f>
-        <v>45</v>
-      </c>
-      <c r="T61" s="301" t="n">
-        <f aca="false">Data_speed!R44</f>
-        <v>55</v>
-      </c>
-      <c r="U61" s="302" t="n">
-        <f aca="false">Data_speed!S44</f>
-        <v>49.33</v>
-      </c>
+      <c r="R61" s="0"/>
+      <c r="S61" s="0"/>
+      <c r="T61" s="0"/>
+      <c r="U61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="256" t="s">
@@ -11503,22 +11024,10 @@
         <v>407.714285714286</v>
       </c>
       <c r="P62" s="177"/>
-      <c r="R62" s="301" t="n">
-        <f aca="false">Data_speed!P45</f>
-        <v>45</v>
-      </c>
-      <c r="S62" s="301" t="n">
-        <f aca="false">Data_speed!Q45</f>
-        <v>55</v>
-      </c>
-      <c r="T62" s="301" t="n">
-        <f aca="false">Data_speed!R45</f>
-        <v>55</v>
-      </c>
-      <c r="U62" s="302" t="n">
-        <f aca="false">Data_speed!S45</f>
-        <v>50.05</v>
-      </c>
+      <c r="R62" s="0"/>
+      <c r="S62" s="0"/>
+      <c r="T62" s="0"/>
+      <c r="U62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="229" t="s">
@@ -11577,22 +11086,10 @@
         <v>454.285714285714</v>
       </c>
       <c r="P63" s="177"/>
-      <c r="R63" s="301" t="n">
-        <f aca="false">Data_speed!P46</f>
-        <v>45</v>
-      </c>
-      <c r="S63" s="301" t="n">
-        <f aca="false">Data_speed!Q46</f>
-        <v>45</v>
-      </c>
-      <c r="T63" s="301" t="n">
-        <f aca="false">Data_speed!R46</f>
-        <v>55</v>
-      </c>
-      <c r="U63" s="302" t="n">
-        <f aca="false">Data_speed!S46</f>
-        <v>49.89</v>
-      </c>
+      <c r="R63" s="0"/>
+      <c r="S63" s="0"/>
+      <c r="T63" s="0"/>
+      <c r="U63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="229" t="s">
@@ -11651,22 +11148,10 @@
         <v>400.285714285714</v>
       </c>
       <c r="P64" s="177"/>
-      <c r="R64" s="301" t="n">
-        <f aca="false">Data_speed!P47</f>
-        <v>45</v>
-      </c>
-      <c r="S64" s="301" t="n">
-        <f aca="false">Data_speed!Q47</f>
-        <v>45</v>
-      </c>
-      <c r="T64" s="301" t="n">
-        <f aca="false">Data_speed!R47</f>
-        <v>55</v>
-      </c>
-      <c r="U64" s="302" t="n">
-        <f aca="false">Data_speed!S47</f>
-        <v>49.24</v>
-      </c>
+      <c r="R64" s="0"/>
+      <c r="S64" s="0"/>
+      <c r="T64" s="0"/>
+      <c r="U64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="229" t="s">
@@ -11725,22 +11210,10 @@
         <v>423</v>
       </c>
       <c r="P65" s="177"/>
-      <c r="R65" s="301" t="n">
-        <f aca="false">Data_speed!P48</f>
-        <v>45</v>
-      </c>
-      <c r="S65" s="301" t="n">
-        <f aca="false">Data_speed!Q48</f>
-        <v>45</v>
-      </c>
-      <c r="T65" s="301" t="n">
-        <f aca="false">Data_speed!R48</f>
-        <v>55</v>
-      </c>
-      <c r="U65" s="302" t="n">
-        <f aca="false">Data_speed!S48</f>
-        <v>49.64</v>
-      </c>
+      <c r="R65" s="0"/>
+      <c r="S65" s="0"/>
+      <c r="T65" s="0"/>
+      <c r="U65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="222" t="s">
@@ -11799,22 +11272,10 @@
         <v>512.142857142857</v>
       </c>
       <c r="P66" s="177"/>
-      <c r="R66" s="301" t="n">
-        <f aca="false">Data_speed!P49</f>
-        <v>45</v>
-      </c>
-      <c r="S66" s="301" t="n">
-        <f aca="false">Data_speed!Q49</f>
-        <v>45</v>
-      </c>
-      <c r="T66" s="301" t="n">
-        <f aca="false">Data_speed!R49</f>
-        <v>55</v>
-      </c>
-      <c r="U66" s="302" t="n">
-        <f aca="false">Data_speed!S49</f>
-        <v>49.31</v>
-      </c>
+      <c r="R66" s="0"/>
+      <c r="S66" s="0"/>
+      <c r="T66" s="0"/>
+      <c r="U66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="226" t="s">
@@ -11873,22 +11334,10 @@
         <v>554.142857142857</v>
       </c>
       <c r="P67" s="177"/>
-      <c r="R67" s="301" t="n">
-        <f aca="false">Data_speed!P50</f>
-        <v>45</v>
-      </c>
-      <c r="S67" s="301" t="n">
-        <f aca="false">Data_speed!Q50</f>
-        <v>45</v>
-      </c>
-      <c r="T67" s="301" t="n">
-        <f aca="false">Data_speed!R50</f>
-        <v>55</v>
-      </c>
-      <c r="U67" s="302" t="n">
-        <f aca="false">Data_speed!S50</f>
-        <v>49.41</v>
-      </c>
+      <c r="R67" s="0"/>
+      <c r="S67" s="0"/>
+      <c r="T67" s="0"/>
+      <c r="U67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="226" t="s">
@@ -11947,22 +11396,10 @@
         <v>466.285714285714</v>
       </c>
       <c r="P68" s="177"/>
-      <c r="R68" s="301" t="n">
-        <f aca="false">Data_speed!P51</f>
-        <v>45</v>
-      </c>
-      <c r="S68" s="301" t="n">
-        <f aca="false">Data_speed!Q51</f>
-        <v>55</v>
-      </c>
-      <c r="T68" s="301" t="n">
-        <f aca="false">Data_speed!R51</f>
-        <v>55</v>
-      </c>
-      <c r="U68" s="302" t="n">
-        <f aca="false">Data_speed!S51</f>
-        <v>50.19</v>
-      </c>
+      <c r="R68" s="0"/>
+      <c r="S68" s="0"/>
+      <c r="T68" s="0"/>
+      <c r="U68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="229" t="s">
@@ -12021,22 +11458,10 @@
         <v>329.285714285714</v>
       </c>
       <c r="P69" s="177"/>
-      <c r="R69" s="301" t="n">
-        <f aca="false">Data_speed!P52</f>
-        <v>45</v>
-      </c>
-      <c r="S69" s="301" t="n">
-        <f aca="false">Data_speed!Q52</f>
-        <v>55</v>
-      </c>
-      <c r="T69" s="301" t="n">
-        <f aca="false">Data_speed!R52</f>
-        <v>55</v>
-      </c>
-      <c r="U69" s="302" t="n">
-        <f aca="false">Data_speed!S52</f>
-        <v>50.54</v>
-      </c>
+      <c r="R69" s="0"/>
+      <c r="S69" s="0"/>
+      <c r="T69" s="0"/>
+      <c r="U69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="229" t="s">
@@ -12095,22 +11520,10 @@
         <v>215.428571428571</v>
       </c>
       <c r="P70" s="177"/>
-      <c r="R70" s="301" t="n">
-        <f aca="false">Data_speed!P53</f>
-        <v>45</v>
-      </c>
-      <c r="S70" s="301" t="n">
-        <f aca="false">Data_speed!Q53</f>
-        <v>55</v>
-      </c>
-      <c r="T70" s="301" t="n">
-        <f aca="false">Data_speed!R53</f>
-        <v>55</v>
-      </c>
-      <c r="U70" s="302" t="n">
-        <f aca="false">Data_speed!S53</f>
-        <v>50.52</v>
-      </c>
+      <c r="R70" s="0"/>
+      <c r="S70" s="0"/>
+      <c r="T70" s="0"/>
+      <c r="U70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="229" t="s">
@@ -12169,22 +11582,10 @@
         <v>174.714285714286</v>
       </c>
       <c r="P71" s="177"/>
-      <c r="R71" s="301" t="n">
-        <f aca="false">Data_speed!P54</f>
-        <v>45</v>
-      </c>
-      <c r="S71" s="301" t="n">
-        <f aca="false">Data_speed!Q54</f>
-        <v>45</v>
-      </c>
-      <c r="T71" s="301" t="n">
-        <f aca="false">Data_speed!R54</f>
-        <v>55</v>
-      </c>
-      <c r="U71" s="302" t="n">
-        <f aca="false">Data_speed!S54</f>
-        <v>49.57</v>
-      </c>
+      <c r="R71" s="0"/>
+      <c r="S71" s="0"/>
+      <c r="T71" s="0"/>
+      <c r="U71" s="0"/>
     </row>
     <row r="72" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="229" t="s">
@@ -12243,22 +11644,10 @@
         <v>157.428571428571</v>
       </c>
       <c r="P72" s="177"/>
-      <c r="R72" s="301" t="n">
-        <f aca="false">Data_speed!P55</f>
-        <v>45</v>
-      </c>
-      <c r="S72" s="301" t="n">
-        <f aca="false">Data_speed!Q55</f>
-        <v>55</v>
-      </c>
-      <c r="T72" s="301" t="n">
-        <f aca="false">Data_speed!R55</f>
-        <v>55</v>
-      </c>
-      <c r="U72" s="302" t="n">
-        <f aca="false">Data_speed!S55</f>
-        <v>50.42</v>
-      </c>
+      <c r="R72" s="0"/>
+      <c r="S72" s="0"/>
+      <c r="T72" s="0"/>
+      <c r="U72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="231" t="s">
@@ -12317,85 +11706,73 @@
         <v>91.7142857142857</v>
       </c>
       <c r="P73" s="177"/>
-      <c r="R73" s="301" t="n">
-        <f aca="false">Data_speed!P56</f>
-        <v>45</v>
-      </c>
-      <c r="S73" s="301" t="n">
-        <f aca="false">Data_speed!Q56</f>
-        <v>55</v>
-      </c>
-      <c r="T73" s="301" t="n">
-        <f aca="false">Data_speed!R56</f>
-        <v>55</v>
-      </c>
-      <c r="U73" s="302" t="n">
-        <f aca="false">Data_speed!S56</f>
-        <v>50.85</v>
-      </c>
+      <c r="R73" s="0"/>
+      <c r="S73" s="0"/>
+      <c r="T73" s="0"/>
+      <c r="U73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="R74" s="179"/>
-      <c r="S74" s="179"/>
-      <c r="T74" s="179"/>
-      <c r="U74" s="179"/>
+      <c r="R74" s="0"/>
+      <c r="S74" s="0"/>
+      <c r="T74" s="0"/>
+      <c r="U74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="M75" s="303"/>
-      <c r="R75" s="179"/>
-      <c r="S75" s="179"/>
-      <c r="T75" s="179"/>
-      <c r="U75" s="179"/>
+      <c r="M75" s="296"/>
+      <c r="R75" s="0"/>
+      <c r="S75" s="0"/>
+      <c r="T75" s="0"/>
+      <c r="U75" s="0"/>
     </row>
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B76" s="304" t="n">
+      <c r="B76" s="297" t="n">
         <f aca="false">SUM(B50:B73)/Data_speed!$O$57</f>
         <v>0.000646183349314212</v>
       </c>
-      <c r="C76" s="304" t="n">
+      <c r="C76" s="297" t="n">
         <f aca="false">SUM(C50:C73)/Data_speed!$O$57</f>
         <v>0.00323091674657106</v>
       </c>
-      <c r="D76" s="304" t="n">
+      <c r="D76" s="297" t="n">
         <f aca="false">SUM(D50:D73)/Data_speed!$O$57</f>
         <v>0.0208029349230833</v>
       </c>
-      <c r="E76" s="304" t="n">
+      <c r="E76" s="297" t="n">
         <f aca="false">SUM(E50:E73)/Data_speed!$O$57</f>
         <v>0.506044941009714</v>
       </c>
-      <c r="F76" s="304" t="n">
+      <c r="F76" s="297" t="n">
         <f aca="false">SUM(F50:F73)/Data_speed!$O$57</f>
         <v>0.435881936048693</v>
       </c>
-      <c r="G76" s="304" t="n">
+      <c r="G76" s="297" t="n">
         <f aca="false">SUM(G50:G73)/Data_speed!$O$57</f>
         <v>0.0318088964855964</v>
       </c>
-      <c r="H76" s="304" t="n">
+      <c r="H76" s="297" t="n">
         <f aca="false">SUM(H50:H73)/Data_speed!$O$57</f>
         <v>0.00122983282611415</v>
       </c>
-      <c r="I76" s="304" t="n">
+      <c r="I76" s="297" t="n">
         <f aca="false">SUM(I50:I73)/Data_speed!$O$57</f>
         <v>0.000187601617542836</v>
       </c>
-      <c r="J76" s="304" t="n">
+      <c r="J76" s="297" t="n">
         <f aca="false">SUM(J50:J73)/Data_speed!$O$57</f>
         <v>2.08446241714262E-005</v>
       </c>
-      <c r="K76" s="304" t="n">
+      <c r="K76" s="297" t="n">
         <f aca="false">SUM(K50:K73)/Data_speed!$O$57</f>
         <v>0</v>
       </c>
-      <c r="L76" s="304" t="n">
+      <c r="L76" s="297" t="n">
         <f aca="false">SUM(L50:L73)/Data_speed!$O$57</f>
         <v>4.16892483428524E-005</v>
       </c>
-      <c r="M76" s="304" t="n">
+      <c r="M76" s="297" t="n">
         <f aca="false">SUM(M50:M73)/Data_speed!$O$57</f>
         <v>0.000104223120857131</v>
       </c>
@@ -12404,72 +11781,60 @@
         <v>1</v>
       </c>
       <c r="P76" s="287"/>
-      <c r="R76" s="305" t="n">
-        <f aca="false">AVERAGE(R50:R73)</f>
-        <v>45</v>
-      </c>
-      <c r="S76" s="305" t="n">
-        <f aca="false">AVERAGE(S50:S73)</f>
-        <v>50</v>
-      </c>
-      <c r="T76" s="305" t="n">
-        <f aca="false">AVERAGE(T50:T73)</f>
-        <v>55.8333333333333</v>
-      </c>
-      <c r="U76" s="306" t="n">
-        <f aca="false">AVERAGE(U50:U73)</f>
-        <v>50.3675</v>
-      </c>
+      <c r="R76" s="0"/>
+      <c r="S76" s="0"/>
+      <c r="T76" s="0"/>
+      <c r="U76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="237" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="307" t="n">
+      <c r="B77" s="298" t="n">
         <f aca="false">SUM(B56:B71)/Data_speed!$O$57</f>
         <v>0.000646183349314212</v>
       </c>
-      <c r="C77" s="307" t="n">
+      <c r="C77" s="298" t="n">
         <f aca="false">SUM(C56:C71)/Data_speed!$O$57</f>
         <v>0.00318922749822821</v>
       </c>
-      <c r="D77" s="307" t="n">
+      <c r="D77" s="298" t="n">
         <f aca="false">SUM(D56:D71)/Data_speed!$O$57</f>
         <v>0.019760703714512</v>
       </c>
-      <c r="E77" s="307" t="n">
+      <c r="E77" s="298" t="n">
         <f aca="false">SUM(E56:E71)/Data_speed!$O$57</f>
         <v>0.475986992954517</v>
       </c>
-      <c r="F77" s="307" t="n">
+      <c r="F77" s="298" t="n">
         <f aca="false">SUM(F56:F71)/Data_speed!$O$57</f>
         <v>0.404073039563097</v>
       </c>
-      <c r="G77" s="307" t="n">
+      <c r="G77" s="298" t="n">
         <f aca="false">SUM(G56:G71)/Data_speed!$O$57</f>
         <v>0.0266394296910827</v>
       </c>
-      <c r="H77" s="307" t="n">
+      <c r="H77" s="298" t="n">
         <f aca="false">SUM(H56:H71)/Data_speed!$O$57</f>
         <v>0.000854629591028474</v>
       </c>
-      <c r="I77" s="307" t="n">
+      <c r="I77" s="298" t="n">
         <f aca="false">SUM(I56:I71)/Data_speed!$O$57</f>
         <v>0.000145912369199983</v>
       </c>
-      <c r="J77" s="307" t="n">
+      <c r="J77" s="298" t="n">
         <f aca="false">SUM(J56:J71)/Data_speed!$O$57</f>
         <v>2.08446241714262E-005</v>
       </c>
-      <c r="K77" s="307" t="n">
+      <c r="K77" s="298" t="n">
         <f aca="false">SUM(K56:K71)/Data_speed!$O$57</f>
         <v>0</v>
       </c>
-      <c r="L77" s="307" t="n">
+      <c r="L77" s="298" t="n">
         <f aca="false">SUM(L56:L71)/Data_speed!$O$57</f>
         <v>4.16892483428524E-005</v>
       </c>
-      <c r="M77" s="307" t="n">
+      <c r="M77" s="298" t="n">
         <f aca="false">SUM(M56:M71)/Data_speed!$O$57</f>
         <v>0.000104223120857131</v>
       </c>
@@ -12478,28 +11843,16 @@
         <v>0.931462875724351</v>
       </c>
       <c r="P77" s="287"/>
-      <c r="R77" s="308" t="n">
-        <f aca="false">AVERAGE(R56:R71)</f>
-        <v>45</v>
-      </c>
-      <c r="S77" s="308" t="n">
-        <f aca="false">AVERAGE(S56:S71)</f>
-        <v>47.5</v>
-      </c>
-      <c r="T77" s="308" t="n">
-        <f aca="false">AVERAGE(T56:T71)</f>
-        <v>55</v>
-      </c>
-      <c r="U77" s="309" t="n">
-        <f aca="false">AVERAGE(U56:U71)</f>
-        <v>49.701875</v>
-      </c>
+      <c r="R77" s="0"/>
+      <c r="S77" s="0"/>
+      <c r="T77" s="0"/>
+      <c r="U77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="B78" s="310" t="n">
+      <c r="B78" s="299" t="n">
         <f aca="false">B76-B77</f>
         <v>0</v>
       </c>
@@ -12553,50 +11906,41 @@
         <v>0.0685371242756494</v>
       </c>
       <c r="P78" s="287"/>
-      <c r="R78" s="311" t="n">
-        <f aca="false">AVERAGE(AVERAGE(R50:R55), AVERAGE(R72:R73))</f>
-        <v>45</v>
-      </c>
-      <c r="S78" s="311" t="n">
-        <f aca="false">AVERAGE(AVERAGE(S50:S55), AVERAGE(S72:S73))</f>
-        <v>55</v>
-      </c>
-      <c r="T78" s="311" t="n">
-        <f aca="false">AVERAGE(AVERAGE(T50:T55), AVERAGE(T72:T73))</f>
-        <v>56.6666666666667</v>
-      </c>
-      <c r="U78" s="312" t="n">
-        <f aca="false">AVERAGE(AVERAGE(U50:U55), AVERAGE(U72:U73))</f>
-        <v>51.3441666666667</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="23.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="R78" s="0"/>
+      <c r="S78" s="0"/>
+      <c r="T78" s="0"/>
+      <c r="U78" s="0"/>
+    </row>
+    <row r="79" customFormat="false" ht="23.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="R79" s="0"/>
+      <c r="S79" s="0"/>
+      <c r="T79" s="0"/>
+      <c r="U79" s="0"/>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="4">
     <mergeCell ref="A11:P11"/>
     <mergeCell ref="B12:M12"/>
-    <mergeCell ref="R12:U12"/>
     <mergeCell ref="A47:P47"/>
     <mergeCell ref="B48:M48"/>
-    <mergeCell ref="R48:U48"/>
   </mergeCells>
-  <conditionalFormatting sqref="A14:V25">
+  <conditionalFormatting sqref="V14:V25 A14:Q25">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$O14&gt;=MAX($O$14:$O$25)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A26:V37">
+  <conditionalFormatting sqref="V26:V37 A26:Q37">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$O26&gt;=MAX($O$26:$O$37)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50:V61">
+  <conditionalFormatting sqref="V50:V61 A50:Q61">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$O50&gt;=MAX($O$50:$O$61)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A62:V73">
+  <conditionalFormatting sqref="V62:V73 A62:Q73">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$O62&gt;=MAX($O$62:$O$73)</formula>
     </cfRule>
@@ -12605,7 +11949,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.25972222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -12619,7 +11963,7 @@
   <dimension ref="A1:V79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S48" activeCellId="1" sqref="J7 S48"/>
+      <selection pane="topLeft" activeCell="S48" activeCellId="1" sqref="H7 S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12656,7 +12000,7 @@
         <v>Comptage 2017</v>
       </c>
       <c r="P2" s="0"/>
-      <c r="Q2" s="303"/>
+      <c r="Q2" s="296"/>
       <c r="V2" s="13" t="str">
         <f aca="false">Data_count!B6</f>
         <v>Type de capteur : Boucle</v>
@@ -12775,76 +12119,76 @@
       <c r="K12" s="247"/>
       <c r="L12" s="247"/>
       <c r="M12" s="247"/>
-      <c r="N12" s="316"/>
+      <c r="N12" s="302"/>
       <c r="P12" s="219" t="s">
         <v>135</v>
       </c>
       <c r="Q12" s="285"/>
-      <c r="S12" s="295" t="s">
-        <v>170</v>
-      </c>
-      <c r="T12" s="295"/>
-      <c r="U12" s="295"/>
-      <c r="V12" s="295"/>
+      <c r="S12" s="303" t="s">
+        <v>183</v>
+      </c>
+      <c r="T12" s="303"/>
+      <c r="U12" s="303"/>
+      <c r="V12" s="303"/>
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="221" t="s">
         <v>110</v>
       </c>
       <c r="B13" s="248" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="248" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="150" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" s="150" t="s">
+        <v>171</v>
+      </c>
+      <c r="F13" s="150" t="s">
+        <v>172</v>
+      </c>
+      <c r="G13" s="150" t="s">
+        <v>173</v>
+      </c>
+      <c r="H13" s="150" t="s">
+        <v>174</v>
+      </c>
+      <c r="I13" s="150" t="s">
+        <v>175</v>
+      </c>
+      <c r="J13" s="150" t="s">
+        <v>176</v>
+      </c>
+      <c r="K13" s="150" t="s">
+        <v>177</v>
+      </c>
+      <c r="L13" s="150" t="s">
+        <v>178</v>
+      </c>
+      <c r="M13" s="150" t="s">
+        <v>179</v>
+      </c>
+      <c r="N13" s="251" t="s">
+        <v>186</v>
+      </c>
+      <c r="P13" s="295" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q13" s="118"/>
+      <c r="S13" s="304" t="s">
+        <v>187</v>
+      </c>
+      <c r="T13" s="305" t="s">
         <v>188</v>
       </c>
-      <c r="C13" s="248" t="s">
+      <c r="U13" s="306" t="s">
         <v>189</v>
       </c>
-      <c r="D13" s="150" t="s">
-        <v>171</v>
-      </c>
-      <c r="E13" s="150" t="s">
-        <v>172</v>
-      </c>
-      <c r="F13" s="150" t="s">
-        <v>173</v>
-      </c>
-      <c r="G13" s="150" t="s">
-        <v>174</v>
-      </c>
-      <c r="H13" s="150" t="s">
-        <v>175</v>
-      </c>
-      <c r="I13" s="150" t="s">
-        <v>176</v>
-      </c>
-      <c r="J13" s="150" t="s">
-        <v>177</v>
-      </c>
-      <c r="K13" s="150" t="s">
-        <v>178</v>
-      </c>
-      <c r="L13" s="150" t="s">
-        <v>179</v>
-      </c>
-      <c r="M13" s="150" t="s">
-        <v>180</v>
-      </c>
-      <c r="N13" s="251" t="s">
+      <c r="V13" s="307" t="s">
         <v>190</v>
-      </c>
-      <c r="P13" s="296" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q13" s="118"/>
-      <c r="S13" s="297" t="s">
-        <v>184</v>
-      </c>
-      <c r="T13" s="298" t="s">
-        <v>185</v>
-      </c>
-      <c r="U13" s="299" t="s">
-        <v>186</v>
-      </c>
-      <c r="V13" s="300" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12908,19 +12252,19 @@
         <v>54</v>
       </c>
       <c r="Q14" s="177"/>
-      <c r="S14" s="301" t="n">
+      <c r="S14" s="308" t="n">
         <f aca="false">Data_speed!P5</f>
         <v>45</v>
       </c>
-      <c r="T14" s="301" t="n">
+      <c r="T14" s="308" t="n">
         <f aca="false">Data_speed!Q5</f>
         <v>55</v>
       </c>
-      <c r="U14" s="301" t="n">
+      <c r="U14" s="308" t="n">
         <f aca="false">Data_speed!R5</f>
         <v>55</v>
       </c>
-      <c r="V14" s="302" t="n">
+      <c r="V14" s="309" t="n">
         <f aca="false">Data_speed!S5</f>
         <v>51.65</v>
       </c>
@@ -12986,19 +12330,19 @@
         <v>22.2857142857143</v>
       </c>
       <c r="Q15" s="177"/>
-      <c r="S15" s="301" t="n">
+      <c r="S15" s="308" t="n">
         <f aca="false">Data_speed!P6</f>
         <v>45</v>
       </c>
-      <c r="T15" s="301" t="n">
+      <c r="T15" s="308" t="n">
         <f aca="false">Data_speed!Q6</f>
         <v>55</v>
       </c>
-      <c r="U15" s="301" t="n">
+      <c r="U15" s="308" t="n">
         <f aca="false">Data_speed!R6</f>
         <v>55</v>
       </c>
-      <c r="V15" s="302" t="n">
+      <c r="V15" s="309" t="n">
         <f aca="false">Data_speed!S6</f>
         <v>51.96</v>
       </c>
@@ -13064,19 +12408,19 @@
         <v>15.5714285714286</v>
       </c>
       <c r="Q16" s="177"/>
-      <c r="S16" s="301" t="n">
+      <c r="S16" s="308" t="n">
         <f aca="false">Data_speed!P7</f>
         <v>45</v>
       </c>
-      <c r="T16" s="301" t="n">
+      <c r="T16" s="308" t="n">
         <f aca="false">Data_speed!Q7</f>
         <v>55</v>
       </c>
-      <c r="U16" s="301" t="n">
+      <c r="U16" s="308" t="n">
         <f aca="false">Data_speed!R7</f>
         <v>55</v>
       </c>
-      <c r="V16" s="302" t="n">
+      <c r="V16" s="309" t="n">
         <f aca="false">Data_speed!S7</f>
         <v>52.22</v>
       </c>
@@ -13142,19 +12486,19 @@
         <v>13.8571428571429</v>
       </c>
       <c r="Q17" s="177"/>
-      <c r="S17" s="301" t="n">
+      <c r="S17" s="308" t="n">
         <f aca="false">Data_speed!P8</f>
         <v>45</v>
       </c>
-      <c r="T17" s="301" t="n">
+      <c r="T17" s="308" t="n">
         <f aca="false">Data_speed!Q8</f>
         <v>55</v>
       </c>
-      <c r="U17" s="301" t="n">
+      <c r="U17" s="308" t="n">
         <f aca="false">Data_speed!R8</f>
         <v>65</v>
       </c>
-      <c r="V17" s="302" t="n">
+      <c r="V17" s="309" t="n">
         <f aca="false">Data_speed!S8</f>
         <v>53.66</v>
       </c>
@@ -13220,19 +12564,19 @@
         <v>19.2857142857143</v>
       </c>
       <c r="Q18" s="177"/>
-      <c r="S18" s="301" t="n">
+      <c r="S18" s="308" t="n">
         <f aca="false">Data_speed!P9</f>
         <v>45</v>
       </c>
-      <c r="T18" s="301" t="n">
+      <c r="T18" s="308" t="n">
         <f aca="false">Data_speed!Q9</f>
         <v>55</v>
       </c>
-      <c r="U18" s="301" t="n">
+      <c r="U18" s="308" t="n">
         <f aca="false">Data_speed!R9</f>
         <v>65</v>
       </c>
-      <c r="V18" s="302" t="n">
+      <c r="V18" s="309" t="n">
         <f aca="false">Data_speed!S9</f>
         <v>54.76</v>
       </c>
@@ -13298,19 +12642,19 @@
         <v>43.4285714285714</v>
       </c>
       <c r="Q19" s="177"/>
-      <c r="S19" s="301" t="n">
+      <c r="S19" s="308" t="n">
         <f aca="false">Data_speed!P10</f>
         <v>45</v>
       </c>
-      <c r="T19" s="301" t="n">
+      <c r="T19" s="308" t="n">
         <f aca="false">Data_speed!Q10</f>
         <v>55</v>
       </c>
-      <c r="U19" s="301" t="n">
+      <c r="U19" s="308" t="n">
         <f aca="false">Data_speed!R10</f>
         <v>55</v>
       </c>
-      <c r="V19" s="302" t="n">
+      <c r="V19" s="309" t="n">
         <f aca="false">Data_speed!S10</f>
         <v>51.38</v>
       </c>
@@ -13376,19 +12720,19 @@
         <v>172.714285714286</v>
       </c>
       <c r="Q20" s="177"/>
-      <c r="S20" s="301" t="n">
+      <c r="S20" s="308" t="n">
         <f aca="false">Data_speed!P11</f>
         <v>45</v>
       </c>
-      <c r="T20" s="301" t="n">
+      <c r="T20" s="308" t="n">
         <f aca="false">Data_speed!Q11</f>
         <v>45</v>
       </c>
-      <c r="U20" s="301" t="n">
+      <c r="U20" s="308" t="n">
         <f aca="false">Data_speed!R11</f>
         <v>55</v>
       </c>
-      <c r="V20" s="302" t="n">
+      <c r="V20" s="309" t="n">
         <f aca="false">Data_speed!S11</f>
         <v>49.76</v>
       </c>
@@ -13454,19 +12798,19 @@
         <v>363</v>
       </c>
       <c r="Q21" s="177"/>
-      <c r="S21" s="301" t="n">
+      <c r="S21" s="308" t="n">
         <f aca="false">Data_speed!P12</f>
         <v>45</v>
       </c>
-      <c r="T21" s="301" t="n">
+      <c r="T21" s="308" t="n">
         <f aca="false">Data_speed!Q12</f>
         <v>45</v>
       </c>
-      <c r="U21" s="301" t="n">
+      <c r="U21" s="308" t="n">
         <f aca="false">Data_speed!R12</f>
         <v>55</v>
       </c>
-      <c r="V21" s="302" t="n">
+      <c r="V21" s="309" t="n">
         <f aca="false">Data_speed!S12</f>
         <v>48.05</v>
       </c>
@@ -13532,19 +12876,19 @@
         <v>333.714285714286</v>
       </c>
       <c r="Q22" s="177"/>
-      <c r="S22" s="301" t="n">
+      <c r="S22" s="308" t="n">
         <f aca="false">Data_speed!P13</f>
         <v>45</v>
       </c>
-      <c r="T22" s="301" t="n">
+      <c r="T22" s="308" t="n">
         <f aca="false">Data_speed!Q13</f>
         <v>45</v>
       </c>
-      <c r="U22" s="301" t="n">
+      <c r="U22" s="308" t="n">
         <f aca="false">Data_speed!R13</f>
         <v>55</v>
       </c>
-      <c r="V22" s="302" t="n">
+      <c r="V22" s="309" t="n">
         <f aca="false">Data_speed!S13</f>
         <v>49.24</v>
       </c>
@@ -13610,19 +12954,19 @@
         <v>317.285714285714</v>
       </c>
       <c r="Q23" s="177"/>
-      <c r="S23" s="301" t="n">
+      <c r="S23" s="308" t="n">
         <f aca="false">Data_speed!P14</f>
         <v>45</v>
       </c>
-      <c r="T23" s="301" t="n">
+      <c r="T23" s="308" t="n">
         <f aca="false">Data_speed!Q14</f>
         <v>45</v>
       </c>
-      <c r="U23" s="301" t="n">
+      <c r="U23" s="308" t="n">
         <f aca="false">Data_speed!R14</f>
         <v>55</v>
       </c>
-      <c r="V23" s="302" t="n">
+      <c r="V23" s="309" t="n">
         <f aca="false">Data_speed!S14</f>
         <v>49.03</v>
       </c>
@@ -13688,19 +13032,19 @@
         <v>340.857142857143</v>
       </c>
       <c r="Q24" s="177"/>
-      <c r="S24" s="301" t="n">
+      <c r="S24" s="308" t="n">
         <f aca="false">Data_speed!P15</f>
         <v>45</v>
       </c>
-      <c r="T24" s="301" t="n">
+      <c r="T24" s="308" t="n">
         <f aca="false">Data_speed!Q15</f>
         <v>45</v>
       </c>
-      <c r="U24" s="301" t="n">
+      <c r="U24" s="308" t="n">
         <f aca="false">Data_speed!R15</f>
         <v>55</v>
       </c>
-      <c r="V24" s="302" t="n">
+      <c r="V24" s="309" t="n">
         <f aca="false">Data_speed!S15</f>
         <v>48.33</v>
       </c>
@@ -13766,19 +13110,19 @@
         <v>445.857142857143</v>
       </c>
       <c r="Q25" s="177"/>
-      <c r="S25" s="301" t="n">
+      <c r="S25" s="308" t="n">
         <f aca="false">Data_speed!P16</f>
         <v>45</v>
       </c>
-      <c r="T25" s="301" t="n">
+      <c r="T25" s="308" t="n">
         <f aca="false">Data_speed!Q16</f>
         <v>45</v>
       </c>
-      <c r="U25" s="301" t="n">
+      <c r="U25" s="308" t="n">
         <f aca="false">Data_speed!R16</f>
         <v>55</v>
       </c>
-      <c r="V25" s="302" t="n">
+      <c r="V25" s="309" t="n">
         <f aca="false">Data_speed!S16</f>
         <v>48.52</v>
       </c>
@@ -13844,19 +13188,19 @@
         <v>413.285714285714</v>
       </c>
       <c r="Q26" s="177"/>
-      <c r="S26" s="301" t="n">
+      <c r="S26" s="308" t="n">
         <f aca="false">Data_speed!P17</f>
         <v>45</v>
       </c>
-      <c r="T26" s="301" t="n">
+      <c r="T26" s="308" t="n">
         <f aca="false">Data_speed!Q17</f>
         <v>45</v>
       </c>
-      <c r="U26" s="301" t="n">
+      <c r="U26" s="308" t="n">
         <f aca="false">Data_speed!R17</f>
         <v>55</v>
       </c>
-      <c r="V26" s="302" t="n">
+      <c r="V26" s="309" t="n">
         <f aca="false">Data_speed!S17</f>
         <v>49.07</v>
       </c>
@@ -13922,19 +13266,19 @@
         <v>420.285714285714</v>
       </c>
       <c r="Q27" s="177"/>
-      <c r="S27" s="301" t="n">
+      <c r="S27" s="308" t="n">
         <f aca="false">Data_speed!P18</f>
         <v>45</v>
       </c>
-      <c r="T27" s="301" t="n">
+      <c r="T27" s="308" t="n">
         <f aca="false">Data_speed!Q18</f>
         <v>45</v>
       </c>
-      <c r="U27" s="301" t="n">
+      <c r="U27" s="308" t="n">
         <f aca="false">Data_speed!R18</f>
         <v>55</v>
       </c>
-      <c r="V27" s="302" t="n">
+      <c r="V27" s="309" t="n">
         <f aca="false">Data_speed!S18</f>
         <v>48.72</v>
       </c>
@@ -14000,19 +13344,19 @@
         <v>382.142857142857</v>
       </c>
       <c r="Q28" s="177"/>
-      <c r="S28" s="301" t="n">
+      <c r="S28" s="308" t="n">
         <f aca="false">Data_speed!P19</f>
         <v>45</v>
       </c>
-      <c r="T28" s="301" t="n">
+      <c r="T28" s="308" t="n">
         <f aca="false">Data_speed!Q19</f>
         <v>45</v>
       </c>
-      <c r="U28" s="301" t="n">
+      <c r="U28" s="308" t="n">
         <f aca="false">Data_speed!R19</f>
         <v>55</v>
       </c>
-      <c r="V28" s="302" t="n">
+      <c r="V28" s="309" t="n">
         <f aca="false">Data_speed!S19</f>
         <v>49.16</v>
       </c>
@@ -14078,19 +13422,19 @@
         <v>440</v>
       </c>
       <c r="Q29" s="177"/>
-      <c r="S29" s="301" t="n">
+      <c r="S29" s="308" t="n">
         <f aca="false">Data_speed!P20</f>
         <v>45</v>
       </c>
-      <c r="T29" s="301" t="n">
+      <c r="T29" s="308" t="n">
         <f aca="false">Data_speed!Q20</f>
         <v>45</v>
       </c>
-      <c r="U29" s="301" t="n">
+      <c r="U29" s="308" t="n">
         <f aca="false">Data_speed!R20</f>
         <v>55</v>
       </c>
-      <c r="V29" s="302" t="n">
+      <c r="V29" s="309" t="n">
         <f aca="false">Data_speed!S20</f>
         <v>48.93</v>
       </c>
@@ -14156,19 +13500,19 @@
         <v>588.857142857143</v>
       </c>
       <c r="Q30" s="177"/>
-      <c r="S30" s="301" t="n">
+      <c r="S30" s="308" t="n">
         <f aca="false">Data_speed!P21</f>
         <v>45</v>
       </c>
-      <c r="T30" s="301" t="n">
+      <c r="T30" s="308" t="n">
         <f aca="false">Data_speed!Q21</f>
         <v>45</v>
       </c>
-      <c r="U30" s="301" t="n">
+      <c r="U30" s="308" t="n">
         <f aca="false">Data_speed!R21</f>
         <v>55</v>
       </c>
-      <c r="V30" s="302" t="n">
+      <c r="V30" s="309" t="n">
         <f aca="false">Data_speed!S21</f>
         <v>48.25</v>
       </c>
@@ -14234,19 +13578,19 @@
         <v>823.428571428572</v>
       </c>
       <c r="Q31" s="177"/>
-      <c r="S31" s="301" t="n">
+      <c r="S31" s="308" t="n">
         <f aca="false">Data_speed!P22</f>
         <v>45</v>
       </c>
-      <c r="T31" s="301" t="n">
+      <c r="T31" s="308" t="n">
         <f aca="false">Data_speed!Q22</f>
         <v>45</v>
       </c>
-      <c r="U31" s="301" t="n">
+      <c r="U31" s="308" t="n">
         <f aca="false">Data_speed!R22</f>
         <v>55</v>
       </c>
-      <c r="V31" s="302" t="n">
+      <c r="V31" s="309" t="n">
         <f aca="false">Data_speed!S22</f>
         <v>46.72</v>
       </c>
@@ -14312,19 +13656,19 @@
         <v>620</v>
       </c>
       <c r="Q32" s="177"/>
-      <c r="S32" s="301" t="n">
+      <c r="S32" s="308" t="n">
         <f aca="false">Data_speed!P23</f>
         <v>45</v>
       </c>
-      <c r="T32" s="301" t="n">
+      <c r="T32" s="308" t="n">
         <f aca="false">Data_speed!Q23</f>
         <v>45</v>
       </c>
-      <c r="U32" s="301" t="n">
+      <c r="U32" s="308" t="n">
         <f aca="false">Data_speed!R23</f>
         <v>55</v>
       </c>
-      <c r="V32" s="302" t="n">
+      <c r="V32" s="309" t="n">
         <f aca="false">Data_speed!S23</f>
         <v>48.2</v>
       </c>
@@ -14390,19 +13734,19 @@
         <v>344.857142857143</v>
       </c>
       <c r="Q33" s="177"/>
-      <c r="S33" s="301" t="n">
+      <c r="S33" s="308" t="n">
         <f aca="false">Data_speed!P24</f>
         <v>45</v>
       </c>
-      <c r="T33" s="301" t="n">
+      <c r="T33" s="308" t="n">
         <f aca="false">Data_speed!Q24</f>
         <v>45</v>
       </c>
-      <c r="U33" s="301" t="n">
+      <c r="U33" s="308" t="n">
         <f aca="false">Data_speed!R24</f>
         <v>55</v>
       </c>
-      <c r="V33" s="302" t="n">
+      <c r="V33" s="309" t="n">
         <f aca="false">Data_speed!S24</f>
         <v>50.28</v>
       </c>
@@ -14468,19 +13812,19 @@
         <v>244.428571428571</v>
       </c>
       <c r="Q34" s="177"/>
-      <c r="S34" s="301" t="n">
+      <c r="S34" s="308" t="n">
         <f aca="false">Data_speed!P25</f>
         <v>45</v>
       </c>
-      <c r="T34" s="301" t="n">
+      <c r="T34" s="308" t="n">
         <f aca="false">Data_speed!Q25</f>
         <v>45</v>
       </c>
-      <c r="U34" s="301" t="n">
+      <c r="U34" s="308" t="n">
         <f aca="false">Data_speed!R25</f>
         <v>55</v>
       </c>
-      <c r="V34" s="302" t="n">
+      <c r="V34" s="309" t="n">
         <f aca="false">Data_speed!S25</f>
         <v>50.03</v>
       </c>
@@ -14546,19 +13890,19 @@
         <v>224.285714285714</v>
       </c>
       <c r="Q35" s="177"/>
-      <c r="S35" s="301" t="n">
+      <c r="S35" s="308" t="n">
         <f aca="false">Data_speed!P26</f>
         <v>45</v>
       </c>
-      <c r="T35" s="301" t="n">
+      <c r="T35" s="308" t="n">
         <f aca="false">Data_speed!Q26</f>
         <v>45</v>
       </c>
-      <c r="U35" s="301" t="n">
+      <c r="U35" s="308" t="n">
         <f aca="false">Data_speed!R26</f>
         <v>55</v>
       </c>
-      <c r="V35" s="302" t="n">
+      <c r="V35" s="309" t="n">
         <f aca="false">Data_speed!S26</f>
         <v>48.9</v>
       </c>
@@ -14624,19 +13968,19 @@
         <v>194.428571428571</v>
       </c>
       <c r="Q36" s="177"/>
-      <c r="S36" s="301" t="n">
+      <c r="S36" s="308" t="n">
         <f aca="false">Data_speed!P27</f>
         <v>45</v>
       </c>
-      <c r="T36" s="301" t="n">
+      <c r="T36" s="308" t="n">
         <f aca="false">Data_speed!Q27</f>
         <v>45</v>
       </c>
-      <c r="U36" s="301" t="n">
+      <c r="U36" s="308" t="n">
         <f aca="false">Data_speed!R27</f>
         <v>55</v>
       </c>
-      <c r="V36" s="302" t="n">
+      <c r="V36" s="309" t="n">
         <f aca="false">Data_speed!S27</f>
         <v>49.09</v>
       </c>
@@ -14702,19 +14046,19 @@
         <v>111.142857142857</v>
       </c>
       <c r="Q37" s="177"/>
-      <c r="S37" s="301" t="n">
+      <c r="S37" s="308" t="n">
         <f aca="false">Data_speed!P28</f>
         <v>45</v>
       </c>
-      <c r="T37" s="301" t="n">
+      <c r="T37" s="308" t="n">
         <f aca="false">Data_speed!Q28</f>
         <v>55</v>
       </c>
-      <c r="U37" s="301" t="n">
+      <c r="U37" s="308" t="n">
         <f aca="false">Data_speed!R28</f>
         <v>55</v>
       </c>
-      <c r="V37" s="302" t="n">
+      <c r="V37" s="309" t="n">
         <f aca="false">Data_speed!S28</f>
         <v>50.4</v>
       </c>
@@ -14726,8 +14070,8 @@
       <c r="V38" s="179"/>
     </row>
     <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="M39" s="303"/>
-      <c r="N39" s="303"/>
+      <c r="M39" s="296"/>
+      <c r="N39" s="296"/>
       <c r="S39" s="179"/>
       <c r="T39" s="179"/>
       <c r="U39" s="179"/>
@@ -14737,55 +14081,55 @@
       <c r="A40" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="304" t="n">
+      <c r="B40" s="297" t="n">
         <f aca="false">SUM(B14:B37)/Data_speed!$O$29</f>
         <v>0.00125400871638845</v>
       </c>
-      <c r="C40" s="304" t="n">
+      <c r="C40" s="297" t="n">
         <f aca="false">SUM(C14:C37)/Data_speed!$O$29</f>
         <v>0.00696899925992928</v>
       </c>
-      <c r="D40" s="304" t="n">
+      <c r="D40" s="297" t="n">
         <f aca="false">SUM(D14:D37)/Data_speed!$O$29</f>
         <v>0.0324603239865143</v>
       </c>
-      <c r="E40" s="304" t="n">
+      <c r="E40" s="297" t="n">
         <f aca="false">SUM(E14:E37)/Data_speed!$O$29</f>
         <v>0.559637365348244</v>
       </c>
-      <c r="F40" s="304" t="n">
+      <c r="F40" s="297" t="n">
         <f aca="false">SUM(F14:F37)/Data_speed!$O$29</f>
         <v>0.379245127867774</v>
       </c>
-      <c r="G40" s="304" t="n">
+      <c r="G40" s="297" t="n">
         <f aca="false">SUM(G14:G37)/Data_speed!$O$29</f>
         <v>0.0191801661047611</v>
       </c>
-      <c r="H40" s="304" t="n">
+      <c r="H40" s="297" t="n">
         <f aca="false">SUM(H14:H37)/Data_speed!$O$29</f>
         <v>0.000801743277690979</v>
       </c>
-      <c r="I40" s="304" t="n">
+      <c r="I40" s="297" t="n">
         <f aca="false">SUM(I14:I37)/Data_speed!$O$29</f>
         <v>0.000205575199407943</v>
       </c>
-      <c r="J40" s="304" t="n">
+      <c r="J40" s="297" t="n">
         <f aca="false">SUM(J14:J37)/Data_speed!$O$29</f>
         <v>4.11150398815887E-005</v>
       </c>
-      <c r="K40" s="304" t="n">
+      <c r="K40" s="297" t="n">
         <f aca="false">SUM(K14:K37)/Data_speed!$O$29</f>
         <v>2.05575199407943E-005</v>
       </c>
-      <c r="L40" s="304" t="n">
+      <c r="L40" s="297" t="n">
         <f aca="false">SUM(L14:L37)/Data_speed!$O$29</f>
         <v>2.05575199407943E-005</v>
       </c>
-      <c r="M40" s="304" t="n">
+      <c r="M40" s="297" t="n">
         <f aca="false">SUM(M14:M37)/Data_speed!$O$29</f>
         <v>0.000164460159526355</v>
       </c>
-      <c r="N40" s="304" t="n">
+      <c r="N40" s="297" t="n">
         <f aca="false">SUM(N14:N37)/Data_speed!$O$29</f>
         <v>0</v>
       </c>
@@ -14794,19 +14138,19 @@
         <v>1</v>
       </c>
       <c r="Q40" s="287"/>
-      <c r="S40" s="305" t="n">
+      <c r="S40" s="310" t="n">
         <f aca="false">AVERAGE(S14:S37)</f>
         <v>45</v>
       </c>
-      <c r="T40" s="305" t="n">
+      <c r="T40" s="310" t="n">
         <f aca="false">AVERAGE(T14:T37)</f>
         <v>47.9166666666667</v>
       </c>
-      <c r="U40" s="305" t="n">
+      <c r="U40" s="310" t="n">
         <f aca="false">AVERAGE(U14:U37)</f>
         <v>55.8333333333333</v>
       </c>
-      <c r="V40" s="306" t="n">
+      <c r="V40" s="311" t="n">
         <f aca="false">AVERAGE(V14:V37)</f>
         <v>49.84625</v>
       </c>
@@ -14815,55 +14159,55 @@
       <c r="A41" s="237" t="s">
         <v>146</v>
       </c>
-      <c r="B41" s="307" t="n">
+      <c r="B41" s="298" t="n">
         <f aca="false">SUM(B20:B35)/Data_speed!$O$29</f>
         <v>0.00123345119644766</v>
       </c>
-      <c r="C41" s="307" t="n">
+      <c r="C41" s="298" t="n">
         <f aca="false">SUM(C20:C35)/Data_speed!$O$29</f>
         <v>0.00680453910040293</v>
       </c>
-      <c r="D41" s="307" t="n">
+      <c r="D41" s="298" t="n">
         <f aca="false">SUM(D20:D35)/Data_speed!$O$29</f>
         <v>0.0308773949510731</v>
       </c>
-      <c r="E41" s="307" t="n">
+      <c r="E41" s="298" t="n">
         <f aca="false">SUM(E20:E35)/Data_speed!$O$29</f>
         <v>0.527793766959954</v>
       </c>
-      <c r="F41" s="307" t="n">
+      <c r="F41" s="298" t="n">
         <f aca="false">SUM(F20:F35)/Data_speed!$O$29</f>
         <v>0.348778883315517</v>
       </c>
-      <c r="G41" s="307" t="n">
+      <c r="G41" s="298" t="n">
         <f aca="false">SUM(G20:G35)/Data_speed!$O$29</f>
         <v>0.0156237151550037</v>
       </c>
-      <c r="H41" s="307" t="n">
+      <c r="H41" s="298" t="n">
         <f aca="false">SUM(H20:H35)/Data_speed!$O$29</f>
         <v>0.000411150398815887</v>
       </c>
-      <c r="I41" s="307" t="n">
+      <c r="I41" s="298" t="n">
         <f aca="false">SUM(I20:I35)/Data_speed!$O$29</f>
         <v>6.1672559822383E-005</v>
       </c>
-      <c r="J41" s="307" t="n">
+      <c r="J41" s="298" t="n">
         <f aca="false">SUM(J20:J35)/Data_speed!$O$29</f>
         <v>0</v>
       </c>
-      <c r="K41" s="307" t="n">
+      <c r="K41" s="298" t="n">
         <f aca="false">SUM(K20:K35)/Data_speed!$O$29</f>
         <v>2.05575199407943E-005</v>
       </c>
-      <c r="L41" s="307" t="n">
+      <c r="L41" s="298" t="n">
         <f aca="false">SUM(L20:L35)/Data_speed!$O$29</f>
         <v>2.05575199407943E-005</v>
       </c>
-      <c r="M41" s="307" t="n">
+      <c r="M41" s="298" t="n">
         <f aca="false">SUM(M20:M35)/Data_speed!$O$29</f>
         <v>0.000164460159526355</v>
       </c>
-      <c r="N41" s="307" t="n">
+      <c r="N41" s="298" t="n">
         <f aca="false">SUM(N20:N35)/Data_speed!$O$29</f>
         <v>0</v>
       </c>
@@ -14872,19 +14216,19 @@
         <v>0.931790148836444</v>
       </c>
       <c r="Q41" s="287"/>
-      <c r="S41" s="308" t="n">
+      <c r="S41" s="312" t="n">
         <f aca="false">AVERAGE(S20:S35)</f>
         <v>45</v>
       </c>
-      <c r="T41" s="308" t="n">
+      <c r="T41" s="312" t="n">
         <f aca="false">AVERAGE(T20:T35)</f>
         <v>45</v>
       </c>
-      <c r="U41" s="308" t="n">
+      <c r="U41" s="312" t="n">
         <f aca="false">AVERAGE(U20:U35)</f>
         <v>55</v>
       </c>
-      <c r="V41" s="309" t="n">
+      <c r="V41" s="313" t="n">
         <f aca="false">AVERAGE(V20:V35)</f>
         <v>48.824375</v>
       </c>
@@ -14893,7 +14237,7 @@
       <c r="A42" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="B42" s="310" t="n">
+      <c r="B42" s="299" t="n">
         <f aca="false">B40-B41</f>
         <v>2.05575199407942E-005</v>
       </c>
@@ -14951,19 +14295,19 @@
         <v>0.0682098511635557</v>
       </c>
       <c r="Q42" s="287"/>
-      <c r="S42" s="311" t="n">
+      <c r="S42" s="314" t="n">
         <f aca="false">AVERAGE(AVERAGE(S14:S19), AVERAGE(S36:S37))</f>
         <v>45</v>
       </c>
-      <c r="T42" s="311" t="n">
+      <c r="T42" s="314" t="n">
         <f aca="false">AVERAGE(AVERAGE(T14:T19), AVERAGE(T36:T37))</f>
         <v>52.5</v>
       </c>
-      <c r="U42" s="311" t="n">
+      <c r="U42" s="314" t="n">
         <f aca="false">AVERAGE(AVERAGE(U14:U19), AVERAGE(U36:U37))</f>
         <v>56.6666666666667</v>
       </c>
-      <c r="V42" s="312" t="n">
+      <c r="V42" s="315" t="n">
         <f aca="false">AVERAGE(AVERAGE(V14:V19), AVERAGE(V36:V37))</f>
         <v>51.175</v>
       </c>
@@ -15038,20 +14382,20 @@
       <c r="K48" s="247"/>
       <c r="L48" s="247"/>
       <c r="M48" s="247"/>
-      <c r="N48" s="316"/>
+      <c r="N48" s="302"/>
       <c r="P48" s="219" t="str">
         <f aca="false">P12</f>
         <v>THM</v>
       </c>
       <c r="Q48" s="285"/>
       <c r="R48" s="186"/>
-      <c r="S48" s="295" t="str">
+      <c r="S48" s="303" t="str">
         <f aca="false">S12</f>
         <v>Vitesses caractéristiques</v>
       </c>
-      <c r="T48" s="295"/>
-      <c r="U48" s="295"/>
-      <c r="V48" s="295"/>
+      <c r="T48" s="303"/>
+      <c r="U48" s="303"/>
+      <c r="V48" s="303"/>
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="221" t="s">
@@ -15109,24 +14453,24 @@
         <f aca="false">N13</f>
         <v>&gt; 120 km/h</v>
       </c>
-      <c r="P49" s="296" t="str">
+      <c r="P49" s="295" t="str">
         <f aca="false">P13</f>
         <v>Véh/h</v>
       </c>
       <c r="Q49" s="118"/>
-      <c r="S49" s="297" t="str">
+      <c r="S49" s="304" t="str">
         <f aca="false">S13</f>
         <v>V15</v>
       </c>
-      <c r="T49" s="298" t="str">
+      <c r="T49" s="305" t="str">
         <f aca="false">T13</f>
         <v>V50</v>
       </c>
-      <c r="U49" s="299" t="str">
+      <c r="U49" s="306" t="str">
         <f aca="false">U13</f>
         <v>V85</v>
       </c>
-      <c r="V49" s="315" t="str">
+      <c r="V49" s="316" t="str">
         <f aca="false">V13</f>
         <v>Vmt</v>
       </c>
@@ -15192,19 +14536,19 @@
         <v>40.2857142857143</v>
       </c>
       <c r="Q50" s="177"/>
-      <c r="S50" s="301" t="n">
+      <c r="S50" s="308" t="n">
         <f aca="false">Data_speed!P33</f>
         <v>45</v>
       </c>
-      <c r="T50" s="301" t="n">
+      <c r="T50" s="308" t="n">
         <f aca="false">Data_speed!Q33</f>
         <v>55</v>
       </c>
-      <c r="U50" s="301" t="n">
+      <c r="U50" s="308" t="n">
         <f aca="false">Data_speed!R33</f>
         <v>55</v>
       </c>
-      <c r="V50" s="302" t="n">
+      <c r="V50" s="309" t="n">
         <f aca="false">Data_speed!S33</f>
         <v>50.42</v>
       </c>
@@ -15270,19 +14614,19 @@
         <v>19.8571428571429</v>
       </c>
       <c r="Q51" s="177"/>
-      <c r="S51" s="301" t="n">
+      <c r="S51" s="308" t="n">
         <f aca="false">Data_speed!P34</f>
         <v>45</v>
       </c>
-      <c r="T51" s="301" t="n">
+      <c r="T51" s="308" t="n">
         <f aca="false">Data_speed!Q34</f>
         <v>55</v>
       </c>
-      <c r="U51" s="301" t="n">
+      <c r="U51" s="308" t="n">
         <f aca="false">Data_speed!R34</f>
         <v>55</v>
       </c>
-      <c r="V51" s="302" t="n">
+      <c r="V51" s="309" t="n">
         <f aca="false">Data_speed!S34</f>
         <v>51.83</v>
       </c>
@@ -15348,19 +14692,19 @@
         <v>13.1428571428571</v>
       </c>
       <c r="Q52" s="177"/>
-      <c r="S52" s="301" t="n">
+      <c r="S52" s="308" t="n">
         <f aca="false">Data_speed!P35</f>
         <v>45</v>
       </c>
-      <c r="T52" s="301" t="n">
+      <c r="T52" s="308" t="n">
         <f aca="false">Data_speed!Q35</f>
         <v>55</v>
       </c>
-      <c r="U52" s="301" t="n">
+      <c r="U52" s="308" t="n">
         <f aca="false">Data_speed!R35</f>
         <v>65</v>
       </c>
-      <c r="V52" s="302" t="n">
+      <c r="V52" s="309" t="n">
         <f aca="false">Data_speed!S35</f>
         <v>52.39</v>
       </c>
@@ -15426,19 +14770,19 @@
         <v>14.8571428571429</v>
       </c>
       <c r="Q53" s="177"/>
-      <c r="S53" s="301" t="n">
+      <c r="S53" s="308" t="n">
         <f aca="false">Data_speed!P36</f>
         <v>45</v>
       </c>
-      <c r="T53" s="301" t="n">
+      <c r="T53" s="308" t="n">
         <f aca="false">Data_speed!Q36</f>
         <v>55</v>
       </c>
-      <c r="U53" s="301" t="n">
+      <c r="U53" s="308" t="n">
         <f aca="false">Data_speed!R36</f>
         <v>55</v>
       </c>
-      <c r="V53" s="302" t="n">
+      <c r="V53" s="309" t="n">
         <f aca="false">Data_speed!S36</f>
         <v>52.98</v>
       </c>
@@ -15504,19 +14848,19 @@
         <v>47</v>
       </c>
       <c r="Q54" s="177"/>
-      <c r="S54" s="301" t="n">
+      <c r="S54" s="308" t="n">
         <f aca="false">Data_speed!P37</f>
         <v>45</v>
       </c>
-      <c r="T54" s="301" t="n">
+      <c r="T54" s="308" t="n">
         <f aca="false">Data_speed!Q37</f>
         <v>55</v>
       </c>
-      <c r="U54" s="301" t="n">
+      <c r="U54" s="308" t="n">
         <f aca="false">Data_speed!R37</f>
         <v>65</v>
       </c>
-      <c r="V54" s="302" t="n">
+      <c r="V54" s="309" t="n">
         <f aca="false">Data_speed!S37</f>
         <v>53.21</v>
       </c>
@@ -15582,19 +14926,19 @@
         <v>85.4285714285714</v>
       </c>
       <c r="Q55" s="177"/>
-      <c r="S55" s="301" t="n">
+      <c r="S55" s="308" t="n">
         <f aca="false">Data_speed!P38</f>
         <v>45</v>
       </c>
-      <c r="T55" s="301" t="n">
+      <c r="T55" s="308" t="n">
         <f aca="false">Data_speed!Q38</f>
         <v>55</v>
       </c>
-      <c r="U55" s="301" t="n">
+      <c r="U55" s="308" t="n">
         <f aca="false">Data_speed!R38</f>
         <v>55</v>
       </c>
-      <c r="V55" s="302" t="n">
+      <c r="V55" s="309" t="n">
         <f aca="false">Data_speed!S38</f>
         <v>51.49</v>
       </c>
@@ -15660,19 +15004,19 @@
         <v>305.714285714286</v>
       </c>
       <c r="Q56" s="177"/>
-      <c r="S56" s="301" t="n">
+      <c r="S56" s="308" t="n">
         <f aca="false">Data_speed!P39</f>
         <v>45</v>
       </c>
-      <c r="T56" s="301" t="n">
+      <c r="T56" s="308" t="n">
         <f aca="false">Data_speed!Q39</f>
         <v>45</v>
       </c>
-      <c r="U56" s="301" t="n">
+      <c r="U56" s="308" t="n">
         <f aca="false">Data_speed!R39</f>
         <v>55</v>
       </c>
-      <c r="V56" s="302" t="n">
+      <c r="V56" s="309" t="n">
         <f aca="false">Data_speed!S39</f>
         <v>50.26</v>
       </c>
@@ -15738,19 +15082,19 @@
         <v>512.428571428571</v>
       </c>
       <c r="Q57" s="177"/>
-      <c r="S57" s="301" t="n">
+      <c r="S57" s="308" t="n">
         <f aca="false">Data_speed!P40</f>
         <v>45</v>
       </c>
-      <c r="T57" s="301" t="n">
+      <c r="T57" s="308" t="n">
         <f aca="false">Data_speed!Q40</f>
         <v>45</v>
       </c>
-      <c r="U57" s="301" t="n">
+      <c r="U57" s="308" t="n">
         <f aca="false">Data_speed!R40</f>
         <v>55</v>
       </c>
-      <c r="V57" s="302" t="n">
+      <c r="V57" s="309" t="n">
         <f aca="false">Data_speed!S40</f>
         <v>49.16</v>
       </c>
@@ -15816,19 +15160,19 @@
         <v>402.571428571429</v>
       </c>
       <c r="Q58" s="177"/>
-      <c r="S58" s="301" t="n">
+      <c r="S58" s="308" t="n">
         <f aca="false">Data_speed!P41</f>
         <v>45</v>
       </c>
-      <c r="T58" s="301" t="n">
+      <c r="T58" s="308" t="n">
         <f aca="false">Data_speed!Q41</f>
         <v>45</v>
       </c>
-      <c r="U58" s="301" t="n">
+      <c r="U58" s="308" t="n">
         <f aca="false">Data_speed!R41</f>
         <v>55</v>
       </c>
-      <c r="V58" s="302" t="n">
+      <c r="V58" s="309" t="n">
         <f aca="false">Data_speed!S41</f>
         <v>49.43</v>
       </c>
@@ -15894,19 +15238,19 @@
         <v>353.571428571429</v>
       </c>
       <c r="Q59" s="177"/>
-      <c r="S59" s="301" t="n">
+      <c r="S59" s="308" t="n">
         <f aca="false">Data_speed!P42</f>
         <v>45</v>
       </c>
-      <c r="T59" s="301" t="n">
+      <c r="T59" s="308" t="n">
         <f aca="false">Data_speed!Q42</f>
         <v>45</v>
       </c>
-      <c r="U59" s="301" t="n">
+      <c r="U59" s="308" t="n">
         <f aca="false">Data_speed!R42</f>
         <v>55</v>
       </c>
-      <c r="V59" s="302" t="n">
+      <c r="V59" s="309" t="n">
         <f aca="false">Data_speed!S42</f>
         <v>49.7</v>
       </c>
@@ -15972,19 +15316,19 @@
         <v>387.714285714286</v>
       </c>
       <c r="Q60" s="177"/>
-      <c r="S60" s="301" t="n">
+      <c r="S60" s="308" t="n">
         <f aca="false">Data_speed!P43</f>
         <v>45</v>
       </c>
-      <c r="T60" s="301" t="n">
+      <c r="T60" s="308" t="n">
         <f aca="false">Data_speed!Q43</f>
         <v>45</v>
       </c>
-      <c r="U60" s="301" t="n">
+      <c r="U60" s="308" t="n">
         <f aca="false">Data_speed!R43</f>
         <v>55</v>
       </c>
-      <c r="V60" s="302" t="n">
+      <c r="V60" s="309" t="n">
         <f aca="false">Data_speed!S43</f>
         <v>48.99</v>
       </c>
@@ -16050,19 +15394,19 @@
         <v>483.857142857143</v>
       </c>
       <c r="Q61" s="177"/>
-      <c r="S61" s="301" t="n">
+      <c r="S61" s="308" t="n">
         <f aca="false">Data_speed!P44</f>
         <v>45</v>
       </c>
-      <c r="T61" s="301" t="n">
+      <c r="T61" s="308" t="n">
         <f aca="false">Data_speed!Q44</f>
         <v>45</v>
       </c>
-      <c r="U61" s="301" t="n">
+      <c r="U61" s="308" t="n">
         <f aca="false">Data_speed!R44</f>
         <v>55</v>
       </c>
-      <c r="V61" s="302" t="n">
+      <c r="V61" s="309" t="n">
         <f aca="false">Data_speed!S44</f>
         <v>49.33</v>
       </c>
@@ -16128,19 +15472,19 @@
         <v>407.714285714286</v>
       </c>
       <c r="Q62" s="177"/>
-      <c r="S62" s="301" t="n">
+      <c r="S62" s="308" t="n">
         <f aca="false">Data_speed!P45</f>
         <v>45</v>
       </c>
-      <c r="T62" s="301" t="n">
+      <c r="T62" s="308" t="n">
         <f aca="false">Data_speed!Q45</f>
         <v>55</v>
       </c>
-      <c r="U62" s="301" t="n">
+      <c r="U62" s="308" t="n">
         <f aca="false">Data_speed!R45</f>
         <v>55</v>
       </c>
-      <c r="V62" s="302" t="n">
+      <c r="V62" s="309" t="n">
         <f aca="false">Data_speed!S45</f>
         <v>50.05</v>
       </c>
@@ -16206,19 +15550,19 @@
         <v>454.285714285714</v>
       </c>
       <c r="Q63" s="177"/>
-      <c r="S63" s="301" t="n">
+      <c r="S63" s="308" t="n">
         <f aca="false">Data_speed!P46</f>
         <v>45</v>
       </c>
-      <c r="T63" s="301" t="n">
+      <c r="T63" s="308" t="n">
         <f aca="false">Data_speed!Q46</f>
         <v>45</v>
       </c>
-      <c r="U63" s="301" t="n">
+      <c r="U63" s="308" t="n">
         <f aca="false">Data_speed!R46</f>
         <v>55</v>
       </c>
-      <c r="V63" s="302" t="n">
+      <c r="V63" s="309" t="n">
         <f aca="false">Data_speed!S46</f>
         <v>49.89</v>
       </c>
@@ -16284,19 +15628,19 @@
         <v>400.285714285714</v>
       </c>
       <c r="Q64" s="177"/>
-      <c r="S64" s="301" t="n">
+      <c r="S64" s="308" t="n">
         <f aca="false">Data_speed!P47</f>
         <v>45</v>
       </c>
-      <c r="T64" s="301" t="n">
+      <c r="T64" s="308" t="n">
         <f aca="false">Data_speed!Q47</f>
         <v>45</v>
       </c>
-      <c r="U64" s="301" t="n">
+      <c r="U64" s="308" t="n">
         <f aca="false">Data_speed!R47</f>
         <v>55</v>
       </c>
-      <c r="V64" s="302" t="n">
+      <c r="V64" s="309" t="n">
         <f aca="false">Data_speed!S47</f>
         <v>49.24</v>
       </c>
@@ -16362,19 +15706,19 @@
         <v>423</v>
       </c>
       <c r="Q65" s="177"/>
-      <c r="S65" s="301" t="n">
+      <c r="S65" s="308" t="n">
         <f aca="false">Data_speed!P48</f>
         <v>45</v>
       </c>
-      <c r="T65" s="301" t="n">
+      <c r="T65" s="308" t="n">
         <f aca="false">Data_speed!Q48</f>
         <v>45</v>
       </c>
-      <c r="U65" s="301" t="n">
+      <c r="U65" s="308" t="n">
         <f aca="false">Data_speed!R48</f>
         <v>55</v>
       </c>
-      <c r="V65" s="302" t="n">
+      <c r="V65" s="309" t="n">
         <f aca="false">Data_speed!S48</f>
         <v>49.64</v>
       </c>
@@ -16440,19 +15784,19 @@
         <v>512.142857142857</v>
       </c>
       <c r="Q66" s="177"/>
-      <c r="S66" s="301" t="n">
+      <c r="S66" s="308" t="n">
         <f aca="false">Data_speed!P49</f>
         <v>45</v>
       </c>
-      <c r="T66" s="301" t="n">
+      <c r="T66" s="308" t="n">
         <f aca="false">Data_speed!Q49</f>
         <v>45</v>
       </c>
-      <c r="U66" s="301" t="n">
+      <c r="U66" s="308" t="n">
         <f aca="false">Data_speed!R49</f>
         <v>55</v>
       </c>
-      <c r="V66" s="302" t="n">
+      <c r="V66" s="309" t="n">
         <f aca="false">Data_speed!S49</f>
         <v>49.31</v>
       </c>
@@ -16518,19 +15862,19 @@
         <v>554.142857142857</v>
       </c>
       <c r="Q67" s="177"/>
-      <c r="S67" s="301" t="n">
+      <c r="S67" s="308" t="n">
         <f aca="false">Data_speed!P50</f>
         <v>45</v>
       </c>
-      <c r="T67" s="301" t="n">
+      <c r="T67" s="308" t="n">
         <f aca="false">Data_speed!Q50</f>
         <v>45</v>
       </c>
-      <c r="U67" s="301" t="n">
+      <c r="U67" s="308" t="n">
         <f aca="false">Data_speed!R50</f>
         <v>55</v>
       </c>
-      <c r="V67" s="302" t="n">
+      <c r="V67" s="309" t="n">
         <f aca="false">Data_speed!S50</f>
         <v>49.41</v>
       </c>
@@ -16596,19 +15940,19 @@
         <v>466.285714285714</v>
       </c>
       <c r="Q68" s="177"/>
-      <c r="S68" s="301" t="n">
+      <c r="S68" s="308" t="n">
         <f aca="false">Data_speed!P51</f>
         <v>45</v>
       </c>
-      <c r="T68" s="301" t="n">
+      <c r="T68" s="308" t="n">
         <f aca="false">Data_speed!Q51</f>
         <v>55</v>
       </c>
-      <c r="U68" s="301" t="n">
+      <c r="U68" s="308" t="n">
         <f aca="false">Data_speed!R51</f>
         <v>55</v>
       </c>
-      <c r="V68" s="302" t="n">
+      <c r="V68" s="309" t="n">
         <f aca="false">Data_speed!S51</f>
         <v>50.19</v>
       </c>
@@ -16674,19 +16018,19 @@
         <v>329.285714285714</v>
       </c>
       <c r="Q69" s="177"/>
-      <c r="S69" s="301" t="n">
+      <c r="S69" s="308" t="n">
         <f aca="false">Data_speed!P52</f>
         <v>45</v>
       </c>
-      <c r="T69" s="301" t="n">
+      <c r="T69" s="308" t="n">
         <f aca="false">Data_speed!Q52</f>
         <v>55</v>
       </c>
-      <c r="U69" s="301" t="n">
+      <c r="U69" s="308" t="n">
         <f aca="false">Data_speed!R52</f>
         <v>55</v>
       </c>
-      <c r="V69" s="302" t="n">
+      <c r="V69" s="309" t="n">
         <f aca="false">Data_speed!S52</f>
         <v>50.54</v>
       </c>
@@ -16752,19 +16096,19 @@
         <v>215.428571428571</v>
       </c>
       <c r="Q70" s="177"/>
-      <c r="S70" s="301" t="n">
+      <c r="S70" s="308" t="n">
         <f aca="false">Data_speed!P53</f>
         <v>45</v>
       </c>
-      <c r="T70" s="301" t="n">
+      <c r="T70" s="308" t="n">
         <f aca="false">Data_speed!Q53</f>
         <v>55</v>
       </c>
-      <c r="U70" s="301" t="n">
+      <c r="U70" s="308" t="n">
         <f aca="false">Data_speed!R53</f>
         <v>55</v>
       </c>
-      <c r="V70" s="302" t="n">
+      <c r="V70" s="309" t="n">
         <f aca="false">Data_speed!S53</f>
         <v>50.52</v>
       </c>
@@ -16830,19 +16174,19 @@
         <v>174.714285714286</v>
       </c>
       <c r="Q71" s="177"/>
-      <c r="S71" s="301" t="n">
+      <c r="S71" s="308" t="n">
         <f aca="false">Data_speed!P54</f>
         <v>45</v>
       </c>
-      <c r="T71" s="301" t="n">
+      <c r="T71" s="308" t="n">
         <f aca="false">Data_speed!Q54</f>
         <v>45</v>
       </c>
-      <c r="U71" s="301" t="n">
+      <c r="U71" s="308" t="n">
         <f aca="false">Data_speed!R54</f>
         <v>55</v>
       </c>
-      <c r="V71" s="302" t="n">
+      <c r="V71" s="309" t="n">
         <f aca="false">Data_speed!S54</f>
         <v>49.57</v>
       </c>
@@ -16908,19 +16252,19 @@
         <v>157.428571428571</v>
       </c>
       <c r="Q72" s="177"/>
-      <c r="S72" s="301" t="n">
+      <c r="S72" s="308" t="n">
         <f aca="false">Data_speed!P55</f>
         <v>45</v>
       </c>
-      <c r="T72" s="301" t="n">
+      <c r="T72" s="308" t="n">
         <f aca="false">Data_speed!Q55</f>
         <v>55</v>
       </c>
-      <c r="U72" s="301" t="n">
+      <c r="U72" s="308" t="n">
         <f aca="false">Data_speed!R55</f>
         <v>55</v>
       </c>
-      <c r="V72" s="302" t="n">
+      <c r="V72" s="309" t="n">
         <f aca="false">Data_speed!S55</f>
         <v>50.42</v>
       </c>
@@ -16986,19 +16330,19 @@
         <v>91.7142857142857</v>
       </c>
       <c r="Q73" s="177"/>
-      <c r="S73" s="301" t="n">
+      <c r="S73" s="308" t="n">
         <f aca="false">Data_speed!P56</f>
         <v>45</v>
       </c>
-      <c r="T73" s="301" t="n">
+      <c r="T73" s="308" t="n">
         <f aca="false">Data_speed!Q56</f>
         <v>55</v>
       </c>
-      <c r="U73" s="301" t="n">
+      <c r="U73" s="308" t="n">
         <f aca="false">Data_speed!R56</f>
         <v>55</v>
       </c>
-      <c r="V73" s="302" t="n">
+      <c r="V73" s="309" t="n">
         <f aca="false">Data_speed!S56</f>
         <v>50.85</v>
       </c>
@@ -17010,8 +16354,8 @@
       <c r="V74" s="179"/>
     </row>
     <row r="75" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="M75" s="303"/>
-      <c r="N75" s="303"/>
+      <c r="M75" s="296"/>
+      <c r="N75" s="296"/>
       <c r="S75" s="179"/>
       <c r="T75" s="179"/>
       <c r="U75" s="179"/>
@@ -17021,55 +16365,55 @@
       <c r="A76" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B76" s="304" t="n">
+      <c r="B76" s="297" t="n">
         <f aca="false">SUM(B50:B73)/Data_speed!$O$57</f>
         <v>0.000646183349314212</v>
       </c>
-      <c r="C76" s="304" t="n">
+      <c r="C76" s="297" t="n">
         <f aca="false">SUM(C50:C73)/Data_speed!$O$57</f>
         <v>0.00323091674657106</v>
       </c>
-      <c r="D76" s="304" t="n">
+      <c r="D76" s="297" t="n">
         <f aca="false">SUM(D50:D73)/Data_speed!$O$57</f>
         <v>0.0208029349230833</v>
       </c>
-      <c r="E76" s="304" t="n">
+      <c r="E76" s="297" t="n">
         <f aca="false">SUM(E50:E73)/Data_speed!$O$57</f>
         <v>0.506044941009714</v>
       </c>
-      <c r="F76" s="304" t="n">
+      <c r="F76" s="297" t="n">
         <f aca="false">SUM(F50:F73)/Data_speed!$O$57</f>
         <v>0.435881936048693</v>
       </c>
-      <c r="G76" s="304" t="n">
+      <c r="G76" s="297" t="n">
         <f aca="false">SUM(G50:G73)/Data_speed!$O$57</f>
         <v>0.0318088964855964</v>
       </c>
-      <c r="H76" s="304" t="n">
+      <c r="H76" s="297" t="n">
         <f aca="false">SUM(H50:H73)/Data_speed!$O$57</f>
         <v>0.00122983282611415</v>
       </c>
-      <c r="I76" s="304" t="n">
+      <c r="I76" s="297" t="n">
         <f aca="false">SUM(I50:I73)/Data_speed!$O$57</f>
         <v>0.000187601617542836</v>
       </c>
-      <c r="J76" s="304" t="n">
+      <c r="J76" s="297" t="n">
         <f aca="false">SUM(J50:J73)/Data_speed!$O$57</f>
         <v>2.08446241714262E-005</v>
       </c>
-      <c r="K76" s="304" t="n">
+      <c r="K76" s="297" t="n">
         <f aca="false">SUM(K50:K73)/Data_speed!$O$57</f>
         <v>0</v>
       </c>
-      <c r="L76" s="304" t="n">
+      <c r="L76" s="297" t="n">
         <f aca="false">SUM(L50:L73)/Data_speed!$O$57</f>
         <v>4.16892483428524E-005</v>
       </c>
-      <c r="M76" s="304" t="n">
+      <c r="M76" s="297" t="n">
         <f aca="false">SUM(M50:M73)/Data_speed!$O$57</f>
         <v>0.000104223120857131</v>
       </c>
-      <c r="N76" s="304" t="n">
+      <c r="N76" s="297" t="n">
         <f aca="false">SUM(N50:N73)/Data_speed!$O$57</f>
         <v>0</v>
       </c>
@@ -17078,19 +16422,19 @@
         <v>1</v>
       </c>
       <c r="Q76" s="287"/>
-      <c r="S76" s="305" t="n">
+      <c r="S76" s="310" t="n">
         <f aca="false">AVERAGE(S50:S73)</f>
         <v>45</v>
       </c>
-      <c r="T76" s="305" t="n">
+      <c r="T76" s="310" t="n">
         <f aca="false">AVERAGE(T50:T73)</f>
         <v>50</v>
       </c>
-      <c r="U76" s="305" t="n">
+      <c r="U76" s="310" t="n">
         <f aca="false">AVERAGE(U50:U73)</f>
         <v>55.8333333333333</v>
       </c>
-      <c r="V76" s="306" t="n">
+      <c r="V76" s="311" t="n">
         <f aca="false">AVERAGE(V50:V73)</f>
         <v>50.3675</v>
       </c>
@@ -17099,55 +16443,55 @@
       <c r="A77" s="237" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="307" t="n">
+      <c r="B77" s="298" t="n">
         <f aca="false">SUM(B56:B71)/Data_speed!$O$57</f>
         <v>0.000646183349314212</v>
       </c>
-      <c r="C77" s="307" t="n">
+      <c r="C77" s="298" t="n">
         <f aca="false">SUM(C56:C71)/Data_speed!$O$57</f>
         <v>0.00318922749822821</v>
       </c>
-      <c r="D77" s="307" t="n">
+      <c r="D77" s="298" t="n">
         <f aca="false">SUM(D56:D71)/Data_speed!$O$57</f>
         <v>0.019760703714512</v>
       </c>
-      <c r="E77" s="307" t="n">
+      <c r="E77" s="298" t="n">
         <f aca="false">SUM(E56:E71)/Data_speed!$O$57</f>
         <v>0.475986992954517</v>
       </c>
-      <c r="F77" s="307" t="n">
+      <c r="F77" s="298" t="n">
         <f aca="false">SUM(F56:F71)/Data_speed!$O$57</f>
         <v>0.404073039563097</v>
       </c>
-      <c r="G77" s="307" t="n">
+      <c r="G77" s="298" t="n">
         <f aca="false">SUM(G56:G71)/Data_speed!$O$57</f>
         <v>0.0266394296910827</v>
       </c>
-      <c r="H77" s="307" t="n">
+      <c r="H77" s="298" t="n">
         <f aca="false">SUM(H56:H71)/Data_speed!$O$57</f>
         <v>0.000854629591028474</v>
       </c>
-      <c r="I77" s="307" t="n">
+      <c r="I77" s="298" t="n">
         <f aca="false">SUM(I56:I71)/Data_speed!$O$57</f>
         <v>0.000145912369199983</v>
       </c>
-      <c r="J77" s="307" t="n">
+      <c r="J77" s="298" t="n">
         <f aca="false">SUM(J56:J71)/Data_speed!$O$57</f>
         <v>2.08446241714262E-005</v>
       </c>
-      <c r="K77" s="307" t="n">
+      <c r="K77" s="298" t="n">
         <f aca="false">SUM(K56:K71)/Data_speed!$O$57</f>
         <v>0</v>
       </c>
-      <c r="L77" s="307" t="n">
+      <c r="L77" s="298" t="n">
         <f aca="false">SUM(L56:L71)/Data_speed!$O$57</f>
         <v>4.16892483428524E-005</v>
       </c>
-      <c r="M77" s="307" t="n">
+      <c r="M77" s="298" t="n">
         <f aca="false">SUM(M56:M71)/Data_speed!$O$57</f>
         <v>0.000104223120857131</v>
       </c>
-      <c r="N77" s="307" t="n">
+      <c r="N77" s="298" t="n">
         <f aca="false">SUM(N56:N71)/Data_speed!$O$57</f>
         <v>0</v>
       </c>
@@ -17156,19 +16500,19 @@
         <v>0.931462875724351</v>
       </c>
       <c r="Q77" s="287"/>
-      <c r="S77" s="308" t="n">
+      <c r="S77" s="312" t="n">
         <f aca="false">AVERAGE(S56:S71)</f>
         <v>45</v>
       </c>
-      <c r="T77" s="308" t="n">
+      <c r="T77" s="312" t="n">
         <f aca="false">AVERAGE(T56:T71)</f>
         <v>47.5</v>
       </c>
-      <c r="U77" s="308" t="n">
+      <c r="U77" s="312" t="n">
         <f aca="false">AVERAGE(U56:U71)</f>
         <v>55</v>
       </c>
-      <c r="V77" s="309" t="n">
+      <c r="V77" s="313" t="n">
         <f aca="false">AVERAGE(V56:V71)</f>
         <v>49.701875</v>
       </c>
@@ -17177,7 +16521,7 @@
       <c r="A78" s="241" t="s">
         <v>147</v>
       </c>
-      <c r="B78" s="310" t="n">
+      <c r="B78" s="299" t="n">
         <f aca="false">B76-B77</f>
         <v>0</v>
       </c>
@@ -17235,19 +16579,19 @@
         <v>0.0685371242756494</v>
       </c>
       <c r="Q78" s="287"/>
-      <c r="S78" s="311" t="n">
+      <c r="S78" s="314" t="n">
         <f aca="false">AVERAGE(AVERAGE(S50:S55), AVERAGE(S72:S73))</f>
         <v>45</v>
       </c>
-      <c r="T78" s="311" t="n">
+      <c r="T78" s="314" t="n">
         <f aca="false">AVERAGE(AVERAGE(T50:T55), AVERAGE(T72:T73))</f>
         <v>55</v>
       </c>
-      <c r="U78" s="311" t="n">
+      <c r="U78" s="314" t="n">
         <f aca="false">AVERAGE(AVERAGE(U50:U55), AVERAGE(U72:U73))</f>
         <v>56.6666666666667</v>
       </c>
-      <c r="V78" s="312" t="n">
+      <c r="V78" s="315" t="n">
         <f aca="false">AVERAGE(AVERAGE(V50:V55), AVERAGE(V72:V73))</f>
         <v>51.3441666666667</v>
       </c>
@@ -17288,7 +16632,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.25972222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -17302,7 +16646,7 @@
   <dimension ref="A1:T93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="1" sqref="J7 K5"/>
+      <selection pane="topLeft" activeCell="K5" activeCellId="1" sqref="H7 K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20664,7 +20008,7 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S34" activeCellId="1" sqref="J7 S34"/>
+      <selection pane="topLeft" activeCell="S34" activeCellId="1" sqref="H7 S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23725,7 +23069,7 @@
   <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N66" activeCellId="1" sqref="J7 N66"/>
+      <selection pane="topLeft" activeCell="N66" activeCellId="1" sqref="H7 N66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26014,7 +25358,7 @@
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27283,7 +26627,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.65347222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -27297,7 +26641,7 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L42" activeCellId="1" sqref="J7 L42"/>
+      <selection pane="topLeft" activeCell="L42" activeCellId="1" sqref="H7 L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28558,7 +27902,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.65347222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -28572,7 +27916,7 @@
   <dimension ref="A1:AE1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="J7 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="H7 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31856,7 +31200,7 @@
   <pageMargins left="0.39375" right="0.39375" top="0.7875" bottom="0.39375" header="0.39375" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -31870,7 +31214,7 @@
   <dimension ref="A1:K78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="J7 A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="H7 A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34427,7 +33771,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -34441,7 +33785,7 @@
   <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="1" sqref="J7 H10"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="1" sqref="H7 H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35815,7 +35159,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>

<commit_message>
Add average speed in Vit_Hd
</commit_message>
<xml_diff>
--- a/comptages/report/template.xlsx
+++ b/comptages/report/template.xlsx
@@ -2865,7 +2865,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3085,7 +3085,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="1" sqref="H7 K5"/>
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3215,7 +3215,7 @@
   <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P55" activeCellId="1" sqref="H7 P55"/>
+      <selection pane="topLeft" activeCell="P55" activeCellId="0" sqref="P55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6515,7 +6515,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -6529,7 +6529,7 @@
   <dimension ref="A1:N76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="1" sqref="H7 K9"/>
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8158,7 +8158,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -8172,7 +8172,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="V47" activeCellId="0" sqref="V47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8295,10 +8295,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="293" t="e">
-        <f aca="false">#REF!&amp;" =&gt; avec un usage de "&amp;TEXT(#REF!,0)&amp;" voie(s) : "&amp;#REF!&amp;"  "&amp;#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A11" s="293"/>
       <c r="B11" s="293"/>
       <c r="C11" s="293"/>
       <c r="D11" s="293"/>
@@ -10109,10 +10106,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="293" t="e">
-        <f aca="false">#REF!&amp;" =&gt; avec un usage de "&amp;TEXT(#REF!,0)&amp;" voie(s) : "&amp;#REF!&amp;"  "&amp;#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A47" s="293"/>
       <c r="B47" s="293"/>
       <c r="C47" s="293"/>
       <c r="D47" s="293"/>
@@ -11949,7 +11943,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.25972222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -11962,8 +11956,8 @@
   </sheetPr>
   <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S48" activeCellId="1" sqref="H7 S48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12078,9 +12072,9 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="293" t="e">
-        <f aca="false">#REF!&amp;" =&gt; avec un usage de "&amp;TEXT(#REF!,0)&amp;" voie(s) : "&amp;#REF!&amp;"  "&amp;#REF!</f>
-        <v>#REF!</v>
+      <c r="A11" s="293" t="str">
+        <f aca="false">_xlfn.CONCAT("Vitesse moyenne = ", INT(V40), " km/h")</f>
+        <v>Vitesse moyenne = 49 km/h</v>
       </c>
       <c r="B11" s="293"/>
       <c r="C11" s="293"/>
@@ -14340,9 +14334,9 @@
       <c r="V46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="293" t="e">
-        <f aca="false">#REF!&amp;" =&gt; avec un usage de "&amp;TEXT(#REF!,0)&amp;" voie(s) : "&amp;#REF!&amp;"  "&amp;#REF!</f>
-        <v>#REF!</v>
+      <c r="A47" s="293" t="str">
+        <f aca="false">_xlfn.CONCAT("Vitesse moyenne = ", INT(V76), " km/h")</f>
+        <v>Vitesse moyenne = 50 km/h</v>
       </c>
       <c r="B47" s="293"/>
       <c r="C47" s="293"/>
@@ -16632,7 +16626,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.25972222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -16646,7 +16640,7 @@
   <dimension ref="A1:T93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="1" sqref="H7 K5"/>
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20008,7 +20002,7 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S34" activeCellId="1" sqref="H7 S34"/>
+      <selection pane="topLeft" activeCell="S34" activeCellId="0" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23069,7 +23063,7 @@
   <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N66" activeCellId="1" sqref="H7 N66"/>
+      <selection pane="topLeft" activeCell="N66" activeCellId="0" sqref="N66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25358,7 +25352,7 @@
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26627,7 +26621,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.65347222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -26641,7 +26635,7 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L42" activeCellId="1" sqref="H7 L42"/>
+      <selection pane="topLeft" activeCell="L42" activeCellId="0" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27902,7 +27896,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.65347222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -27916,7 +27910,7 @@
   <dimension ref="A1:AE1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="H7 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31200,7 +31194,7 @@
   <pageMargins left="0.39375" right="0.39375" top="0.7875" bottom="0.39375" header="0.39375" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -31214,7 +31208,7 @@
   <dimension ref="A1:K78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="H7 A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33771,7 +33765,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -33785,7 +33779,7 @@
   <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="1" sqref="H7 H10"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35159,7 +35153,7 @@
   <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>

<commit_message>
Fix headers and footers
Closes #78
</commit_message>
<xml_diff>
--- a/comptages/report/template.xlsx
+++ b/comptages/report/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Data_count" sheetId="1" state="visible" r:id="rId2"/>
@@ -6545,10 +6545,14 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
+  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.72222222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
+Département du développement
+territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+Bureau signalisation et circulation
+Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -8188,10 +8192,14 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
+  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.72222222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8 épublique et canton de Neuchâtel
+Département du développement
+territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+Bureau signalisation et circulation
+Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -11973,10 +11981,13 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.25972222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
+  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.67638888888889" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
+Département du développement territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+Bureau signalisation et circulation
+Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -11989,7 +12000,7 @@
   </sheetPr>
   <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
     </sheetView>
   </sheetViews>
@@ -16656,10 +16667,13 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.25972222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
+  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.67638888888889" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
+Département du développement territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+Bureau signalisation et circulation
+Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -21810,7 +21824,7 @@
   </sheetPr>
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -23077,10 +23091,14 @@
     <mergeCell ref="J43:K43"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.65347222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
+  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.95902777777778" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
+Département du développement
+territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+Bureau signalisation et circulation
+Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -24352,10 +24370,14 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.65347222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
+  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.95902777777778" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
+Département du développement
+territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+Bureau signalisation et circulation
+Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -27650,10 +27672,14 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.39375" right="0.39375" top="0.7875" bottom="0.39375" header="0.39375" footer="0.236111111111111"/>
+  <pageMargins left="0.39375" right="0.39375" top="1.09305555555556" bottom="0.39375" header="0.39375" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
+Département du développement
+territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+Bureau signalisation et circulation
+Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -30221,10 +30247,14 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
+  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.72222222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
+Département du développement
+territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+Bureau signalisation et circulation
+Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -31609,10 +31639,14 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.41666666666667" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
+  <pageMargins left="0.669444444444444" right="0.669444444444444" top="1.72222222222222" bottom="0.472222222222222" header="0.708333333333333" footer="0.236111111111111"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;8 République et canton de Neuchâtel_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Département du développement_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8 Service des ponts et chaussées_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Bureau signalisation et circulation_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x005F_x000a_Neuchâtel, le &amp;D</oddHeader>
+    <oddHeader>&amp;L&amp;8République et canton de Neuchâtel
+Département du développement
+territorial et de l'environnement&amp;CComptage hebdomadaire&amp;R&amp;8Service des ponts et chaussées
+Bureau signalisation et circulation
+Neuchâtel, le &amp;D</oddHeader>
     <oddFooter>&amp;L&amp;6 &amp;F&amp;R&amp;8 Page: &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>

<commit_message>
Fix titles in sheets
Closes #85
</commit_message>
<xml_diff>
--- a/comptages/report/template.xlsx
+++ b/comptages/report/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Data_count" sheetId="1" state="visible" r:id="rId2"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="181">
   <si>
     <t xml:space="preserve">Data of the count</t>
   </si>
@@ -417,6 +417,9 @@
     <t xml:space="preserve">24 heures</t>
   </si>
   <si>
+    <t xml:space="preserve">Classification SWISS7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dir 1 : </t>
   </si>
   <si>
@@ -480,6 +483,9 @@
     <t xml:space="preserve">Véhicules lourds : CAR (1) + LW (8) + LZ (9) + SZ (10)</t>
   </si>
   <si>
+    <t xml:space="preserve">Classification SWISS10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Part du TJM</t>
   </si>
   <si>
@@ -514,6 +520,9 @@
   </si>
   <si>
     <t xml:space="preserve">Véhicules légers : MR (2) + PW (3) + PW+AH(4) + LIE (5) + LIE+AH(6) + LIE+AL(7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyse des vitesses</t>
   </si>
   <si>
     <t xml:space="preserve">30 km/h</t>
@@ -3142,7 +3151,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="J8 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3248,7 +3257,7 @@
   <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P55" activeCellId="0" sqref="P55"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="1" sqref="J8 G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3289,7 +3298,9 @@
         <f aca="false">Data_count!B10</f>
         <v>0</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>146</v>
+      </c>
       <c r="J3" s="11"/>
       <c r="N3" s="16" t="n">
         <f aca="false">Data_count!B7</f>
@@ -3350,7 +3361,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="216" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B9" s="217" t="n">
         <f aca="false">B4</f>
@@ -3377,7 +3388,7 @@
         <v>122</v>
       </c>
       <c r="N11" s="220" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3385,38 +3396,38 @@
         <v>97</v>
       </c>
       <c r="B12" s="248" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C12" s="150" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D12" s="249" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E12" s="150" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F12" s="249" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G12" s="150" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H12" s="249" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I12" s="150" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J12" s="249" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K12" s="291" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L12" s="64"/>
       <c r="M12" s="225" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N12" s="220"/>
     </row>
@@ -4773,7 +4784,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B39" s="238" t="e">
         <f aca="false">SUM(B19:B34)/Data_category!$L$29</f>
@@ -4827,7 +4838,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B40" s="242" t="e">
         <f aca="false">B38-B39</f>
@@ -4891,7 +4902,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="216" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B42" s="4" t="n">
         <f aca="false">B5</f>
@@ -4968,7 +4979,7 @@
       </c>
       <c r="L45" s="64"/>
       <c r="M45" s="225" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N45" s="220"/>
     </row>
@@ -6325,7 +6336,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B72" s="238" t="e">
         <f aca="false">SUM(B52:B67)/Data_category!$L$57</f>
@@ -6379,7 +6390,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B73" s="242" t="e">
         <f aca="false">B71-B72</f>
@@ -6433,23 +6444,23 @@
     </row>
     <row r="75" s="42" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="82" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B75" s="82"/>
       <c r="C75" s="82" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D75" s="155"/>
       <c r="E75" s="82"/>
       <c r="F75" s="82"/>
       <c r="G75" s="82" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H75" s="82"/>
       <c r="I75" s="82"/>
       <c r="J75" s="294"/>
       <c r="K75" s="82" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L75" s="82"/>
       <c r="M75" s="1"/>
@@ -6457,16 +6468,16 @@
     </row>
     <row r="76" s="42" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="82" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B76" s="82"/>
       <c r="C76" s="82" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E76" s="82"/>
       <c r="F76" s="82"/>
       <c r="G76" s="82" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H76" s="82"/>
       <c r="I76" s="82"/>
@@ -6478,16 +6489,16 @@
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="82" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B77" s="82"/>
       <c r="C77" s="82" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E77" s="82"/>
       <c r="F77" s="82"/>
       <c r="G77" s="82" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H77" s="82"/>
       <c r="I77" s="82"/>
@@ -6497,7 +6508,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="252" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B78" s="252"/>
       <c r="C78" s="252"/>
@@ -6506,7 +6517,7 @@
       <c r="F78" s="252"/>
       <c r="G78" s="252"/>
       <c r="H78" s="252" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I78" s="252"/>
       <c r="J78" s="252"/>
@@ -6566,7 +6577,7 @@
   <dimension ref="A1:N76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S60" activeCellId="0" sqref="S60"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="1" sqref="J8 G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6637,6 +6648,10 @@
         <f aca="false">Data_count!B14</f>
         <v>0</v>
       </c>
+      <c r="G5" s="15" t="n">
+        <f aca="false">Data_count!B8</f>
+        <v>0</v>
+      </c>
       <c r="J5" s="11"/>
       <c r="N5" s="16" t="n">
         <f aca="false">Data_count!B9</f>
@@ -6646,16 +6661,16 @@
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="14"/>
       <c r="C6" s="18"/>
+      <c r="G6" s="15" t="s">
+        <v>146</v>
+      </c>
       <c r="J6" s="11"/>
       <c r="N6" s="118"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="14"/>
       <c r="C7" s="18"/>
-      <c r="F7" s="19" t="n">
-        <f aca="false">Data_count!B11</f>
-        <v>0</v>
-      </c>
+      <c r="F7" s="0"/>
       <c r="G7" s="20"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -6665,14 +6680,17 @@
       <c r="A8" s="14"/>
       <c r="C8" s="18"/>
       <c r="F8" s="19"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="19" t="n">
+        <f aca="false">Data_count!B11</f>
+        <v>0</v>
+      </c>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="N8" s="118"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="216" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B9" s="4" t="n">
         <f aca="false">B4</f>
@@ -6698,7 +6716,7 @@
       <c r="L11" s="256"/>
       <c r="M11" s="257"/>
       <c r="N11" s="220" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7319,7 +7337,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B40" s="238" t="e">
         <f aca="false">SWISS10_H!B39</f>
@@ -7370,7 +7388,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B41" s="242" t="e">
         <f aca="false">SWISS10_H!B40</f>
@@ -7421,7 +7439,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="216" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B44" s="4" t="n">
         <f aca="false">B5</f>
@@ -8066,7 +8084,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B75" s="238" t="e">
         <f aca="false">SWISS10_H!B72</f>
@@ -8117,7 +8135,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B76" s="242" t="e">
         <f aca="false">SWISS10_H!B73</f>
@@ -8213,7 +8231,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V47" activeCellId="0" sqref="V47"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="1" sqref="J8 H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8325,10 +8343,15 @@
       <c r="K7" s="11"/>
       <c r="N7" s="118"/>
     </row>
+    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="216" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B10" s="4" t="n">
         <f aca="false">B4</f>
@@ -8393,43 +8416,43 @@
         <v>97</v>
       </c>
       <c r="B13" s="248" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C13" s="150" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D13" s="150" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E13" s="150" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F13" s="150" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G13" s="150" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H13" s="150" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="I13" s="150" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="J13" s="150" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="K13" s="150" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="L13" s="150" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="M13" s="251" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="O13" s="303" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="P13" s="118"/>
       <c r="R13" s="0"/>
@@ -10002,7 +10025,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B41" s="306" t="e">
         <f aca="false">SUM(B20:B35)/Data_speed!$O$29</f>
@@ -10064,7 +10087,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B42" s="307" t="e">
         <f aca="false">B40-B41</f>
@@ -10139,7 +10162,7 @@
     <row r="45" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="216" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B46" s="4" t="n">
         <f aca="false">B5</f>
@@ -11823,7 +11846,7 @@
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B77" s="306" t="e">
         <f aca="false">SUM(B56:B71)/Data_speed!$O$57</f>
@@ -11885,7 +11908,7 @@
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B78" s="307" t="e">
         <f aca="false">B76-B77</f>
@@ -12000,8 +12023,8 @@
   </sheetPr>
   <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12105,10 +12128,15 @@
       <c r="K7" s="11"/>
       <c r="N7" s="118"/>
     </row>
+    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J8" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="216" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B10" s="4" t="n">
         <f aca="false">B4</f>
@@ -12163,7 +12191,7 @@
       </c>
       <c r="Q12" s="290"/>
       <c r="S12" s="312" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="T12" s="312"/>
       <c r="U12" s="312"/>
@@ -12174,59 +12202,59 @@
         <v>97</v>
       </c>
       <c r="B13" s="248" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C13" s="248" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" s="150" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="150" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" s="150" t="s">
+        <v>162</v>
+      </c>
+      <c r="G13" s="150" t="s">
+        <v>163</v>
+      </c>
+      <c r="H13" s="150" t="s">
+        <v>164</v>
+      </c>
+      <c r="I13" s="150" t="s">
+        <v>165</v>
+      </c>
+      <c r="J13" s="150" t="s">
+        <v>166</v>
+      </c>
+      <c r="K13" s="150" t="s">
+        <v>167</v>
+      </c>
+      <c r="L13" s="150" t="s">
+        <v>168</v>
+      </c>
+      <c r="M13" s="150" t="s">
+        <v>169</v>
+      </c>
+      <c r="N13" s="251" t="s">
+        <v>176</v>
+      </c>
+      <c r="P13" s="303" t="s">
         <v>172</v>
-      </c>
-      <c r="D13" s="150" t="s">
-        <v>157</v>
-      </c>
-      <c r="E13" s="150" t="s">
-        <v>158</v>
-      </c>
-      <c r="F13" s="150" t="s">
-        <v>159</v>
-      </c>
-      <c r="G13" s="150" t="s">
-        <v>160</v>
-      </c>
-      <c r="H13" s="150" t="s">
-        <v>161</v>
-      </c>
-      <c r="I13" s="150" t="s">
-        <v>162</v>
-      </c>
-      <c r="J13" s="150" t="s">
-        <v>163</v>
-      </c>
-      <c r="K13" s="150" t="s">
-        <v>164</v>
-      </c>
-      <c r="L13" s="150" t="s">
-        <v>165</v>
-      </c>
-      <c r="M13" s="150" t="s">
-        <v>166</v>
-      </c>
-      <c r="N13" s="251" t="s">
-        <v>173</v>
-      </c>
-      <c r="P13" s="303" t="s">
-        <v>169</v>
       </c>
       <c r="Q13" s="118"/>
       <c r="S13" s="313" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="T13" s="314" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="U13" s="315" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="V13" s="316" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14195,7 +14223,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B41" s="306" t="e">
         <f aca="false">SUM(B20:B35)/Data_speed!$O$29</f>
@@ -14273,7 +14301,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B42" s="307" t="e">
         <f aca="false">B40-B41</f>
@@ -14369,7 +14397,7 @@
     </row>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="216" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B46" s="4" t="n">
         <f aca="false">B5</f>
@@ -16479,7 +16507,7 @@
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B77" s="306" t="e">
         <f aca="false">SUM(B56:B71)/Data_speed!$O$57</f>
@@ -16557,7 +16585,7 @@
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B78" s="307" t="e">
         <f aca="false">B76-B77</f>
@@ -16687,7 +16715,7 @@
   <dimension ref="A1:T93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B92" activeCellId="0" sqref="B92"/>
+      <selection pane="topLeft" activeCell="B92" activeCellId="1" sqref="J8 B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18971,7 +18999,7 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
+      <selection pane="topLeft" activeCell="P33" activeCellId="1" sqref="J8 P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20496,7 +20524,7 @@
   <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="1" sqref="J8 B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21824,8 +21852,8 @@
   </sheetPr>
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J8 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23112,7 +23140,7 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L42" activeCellId="0" sqref="L42"/>
+      <selection pane="topLeft" activeCell="L42" activeCellId="1" sqref="J8 L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24391,7 +24419,7 @@
   <dimension ref="A1:AE1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="J8 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27693,7 +27721,7 @@
   <dimension ref="A1:K78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="1" sqref="J8 G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27734,7 +27762,9 @@
         <f aca="false">Data_count!B10</f>
         <v>0</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>124</v>
+      </c>
       <c r="J3" s="11"/>
       <c r="K3" s="16" t="n">
         <f aca="false">Data_count!B7</f>
@@ -27795,7 +27825,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="216" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B9" s="217" t="n">
         <f aca="false">B4</f>
@@ -27828,29 +27858,29 @@
         <v>97</v>
       </c>
       <c r="B12" s="222" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C12" s="151" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D12" s="223" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E12" s="151" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F12" s="223" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G12" s="151" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H12" s="224" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I12" s="42"/>
       <c r="J12" s="225" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K12" s="220"/>
     </row>
@@ -28884,7 +28914,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B39" s="238" t="e">
         <f aca="false">SUM(B19:B34)/Data_category!$L$29</f>
@@ -28925,7 +28955,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B40" s="242" t="e">
         <f aca="false">B38-B39</f>
@@ -28975,7 +29005,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="216" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B42" s="4" t="n">
         <f aca="false">B5</f>
@@ -29037,7 +29067,7 @@
       </c>
       <c r="I45" s="42"/>
       <c r="J45" s="225" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K45" s="220"/>
     </row>
@@ -30071,7 +30101,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B72" s="238" t="e">
         <f aca="false">SUM(B52:B67)/Data_category!$L$57</f>
@@ -30112,7 +30142,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B73" s="242" t="e">
         <f aca="false">B71-B72</f>
@@ -30153,17 +30183,17 @@
     </row>
     <row r="75" s="42" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="82" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B75" s="82"/>
       <c r="C75" s="82" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D75" s="155"/>
       <c r="E75" s="82"/>
       <c r="F75" s="82"/>
       <c r="G75" s="82" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H75" s="82"/>
       <c r="I75" s="1"/>
@@ -30172,16 +30202,16 @@
     </row>
     <row r="76" s="42" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="82" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B76" s="82"/>
       <c r="C76" s="82" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E76" s="82"/>
       <c r="F76" s="82"/>
       <c r="G76" s="82" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H76" s="82"/>
       <c r="I76" s="1"/>
@@ -30196,20 +30226,20 @@
       <c r="E77" s="82"/>
       <c r="F77" s="82"/>
       <c r="G77" s="82" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H77" s="82"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="252" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B78" s="252"/>
       <c r="C78" s="252"/>
       <c r="D78" s="252"/>
       <c r="E78" s="252"/>
       <c r="F78" s="252" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G78" s="252"/>
       <c r="H78" s="252"/>
@@ -30268,7 +30298,7 @@
   <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I73" activeCellId="0" sqref="I73"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="J8 G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30309,7 +30339,9 @@
         <f aca="false">Data_count!B10</f>
         <v>0</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>124</v>
+      </c>
       <c r="J3" s="11"/>
       <c r="K3" s="16" t="n">
         <f aca="false">Data_count!B7</f>
@@ -30370,7 +30402,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="216" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B9" s="4" t="n">
         <f aca="false">B4</f>
@@ -30916,7 +30948,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B40" s="238" t="e">
         <f aca="false">SWISS7_H!B39</f>
@@ -30955,7 +30987,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B41" s="242" t="e">
         <f aca="false">SWISS7_H!B40</f>
@@ -30994,7 +31026,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="216" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B44" s="4" t="n">
         <f aca="false">B5</f>
@@ -31537,7 +31569,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="237" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B75" s="238" t="e">
         <f aca="false">SWISS7_H!B72</f>
@@ -31576,7 +31608,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="241" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B76" s="242" t="e">
         <f aca="false">SWISS7_H!B73</f>

</xml_diff>

<commit_message>
Improve legend readability in the SWISSX_G pages
Closes #87
</commit_message>
<xml_diff>
--- a/comptages/report/template.xlsx
+++ b/comptages/report/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Data_count" sheetId="1" state="visible" r:id="rId2"/>
@@ -2795,31 +2795,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="5" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="5" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="6" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="6" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="7" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="7" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="8" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="8" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="9" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="9" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="10" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="10" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="11" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="11" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2871,7 +2871,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="11" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="11" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2915,15 +2915,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="12" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="12" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="13" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="13" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="14" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="14" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3151,7 +3151,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="J8 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3257,7 +3257,7 @@
   <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="1" sqref="J8 G3"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6576,8 +6576,8 @@
   </sheetPr>
   <dimension ref="A1:N76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="1" sqref="J8 G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P59" activeCellId="0" sqref="P59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8231,7 +8231,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="1" sqref="J8 H8"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12023,7 +12023,7 @@
   </sheetPr>
   <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -16715,7 +16715,7 @@
   <dimension ref="A1:T93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B92" activeCellId="1" sqref="J8 B92"/>
+      <selection pane="topLeft" activeCell="B92" activeCellId="0" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18999,7 +18999,7 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P33" activeCellId="1" sqref="J8 P33"/>
+      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20524,7 +20524,7 @@
   <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="1" sqref="J8 B33"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21853,7 +21853,7 @@
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23140,7 +23140,7 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L42" activeCellId="1" sqref="J8 L42"/>
+      <selection pane="topLeft" activeCell="L42" activeCellId="0" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24419,7 +24419,7 @@
   <dimension ref="A1:AE1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="J8 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27721,7 +27721,7 @@
   <dimension ref="A1:K78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="1" sqref="J8 G3"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30298,7 +30298,7 @@
   <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="J8 G2"/>
+      <selection pane="topLeft" activeCell="B73" activeCellId="0" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Replace 'CONCAT' with '&'
Closes #80
</commit_message>
<xml_diff>
--- a/comptages/report/template.xlsx
+++ b/comptages/report/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Data_count" sheetId="1" state="visible" r:id="rId2"/>
@@ -2970,7 +2970,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3161,7 +3161,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="119.13"/>
@@ -3267,14 +3267,14 @@
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="9.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="1.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="119" width="9.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="11.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6587,14 +6587,14 @@
       <selection pane="topLeft" activeCell="B73" activeCellId="0" sqref="B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="9.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="1.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="11.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8241,7 +8241,7 @@
       <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="6.98"/>
@@ -8253,9 +8253,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="6.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="7.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="22" style="1" width="11.04"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="1020" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1019" min="22" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1020" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12030,11 +12030,11 @@
   </sheetPr>
   <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="6.98"/>
@@ -12045,7 +12045,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="1" width="1.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="19" style="1" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="7.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="1" width="11.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12152,7 +12152,7 @@
     </row>
     <row r="11" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="311" t="str">
-        <f aca="false">_xlfn.CONCAT("Vitesse moyenne = ", INT(V40), " km/h")</f>
+        <f aca="false">"Vitesse moyenne = "&amp;INT(V40)&amp;" km/h"</f>
         <v>Vitesse moyenne = 0 km/h</v>
       </c>
       <c r="B11" s="311"/>
@@ -14414,7 +14414,7 @@
     </row>
     <row r="47" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="311" t="str">
-        <f aca="false">_xlfn.CONCAT("Vitesse moyenne = ", INT(V76), " km/h")</f>
+        <f aca="false">"Vitesse moyenne = "&amp;INT(V76)&amp;" km/h"</f>
         <v>Vitesse moyenne = 0 km/h</v>
       </c>
       <c r="B47" s="311"/>
@@ -16725,7 +16725,7 @@
       <selection pane="topLeft" activeCell="B92" activeCellId="0" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.19"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="11.52"/>
@@ -19009,7 +19009,7 @@
       <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="11.52"/>
   </cols>
@@ -20530,11 +20530,11 @@
   </sheetPr>
   <dimension ref="A1:W57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Y29" activeCellId="0" sqref="Y29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="11.52"/>
   </cols>
@@ -23849,12 +23849,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="12" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25136,11 +25136,11 @@
       <selection pane="topLeft" activeCell="L42" activeCellId="0" sqref="L42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26415,7 +26415,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.84"/>
@@ -26424,7 +26424,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="13" style="1" width="8.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="23" style="1" width="8.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="32" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="32" style="1" width="11.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29717,14 +29717,14 @@
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="12.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="1.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="119" width="11.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32294,14 +32294,14 @@
       <selection pane="topLeft" activeCell="D73" activeCellId="0" sqref="D73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="13.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="1.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add average speed on report speed pages
Closes #84
</commit_message>
<xml_diff>
--- a/comptages/report/template.xlsx
+++ b/comptages/report/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Data_count" sheetId="1" state="visible" r:id="rId2"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="183">
   <si>
     <t xml:space="preserve">Data of the count</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t xml:space="preserve">average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average by class</t>
   </si>
   <si>
     <t xml:space="preserve">Data category</t>
@@ -1725,7 +1728,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="327">
+  <cellXfs count="326">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2934,8 +2937,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2968,10 +2971,6 @@
     </xf>
     <xf numFmtId="169" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3306,7 +3305,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J3" s="12"/>
       <c r="N3" s="17" t="n">
@@ -3316,7 +3315,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -3330,7 +3329,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -3368,7 +3367,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="217" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B9" s="218" t="n">
         <f aca="false">B4</f>
@@ -3392,49 +3391,49 @@
       <c r="K11" s="248"/>
       <c r="L11" s="291"/>
       <c r="M11" s="220" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N11" s="221" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="222" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B12" s="249" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C12" s="151" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D12" s="250" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E12" s="151" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F12" s="250" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G12" s="151" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H12" s="250" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I12" s="151" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J12" s="250" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K12" s="292" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L12" s="65"/>
       <c r="M12" s="226" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N12" s="221"/>
     </row>
@@ -4737,7 +4736,7 @@
     <row r="37" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B38" s="235" t="e">
         <f aca="false">SUM(B13:B36)/Data_category!$L$29</f>
@@ -4791,7 +4790,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B39" s="239" t="e">
         <f aca="false">SUM(B19:B34)/Data_category!$L$29</f>
@@ -4845,7 +4844,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B40" s="243" t="e">
         <f aca="false">B38-B39</f>
@@ -4909,7 +4908,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="217" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B42" s="4" t="n">
         <f aca="false">B5</f>
@@ -4933,7 +4932,7 @@
       <c r="K44" s="248"/>
       <c r="L44" s="291"/>
       <c r="M44" s="220" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N44" s="221" t="str">
         <f aca="false">N11</f>
@@ -4942,7 +4941,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="222" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B45" s="249" t="str">
         <f aca="false">B12</f>
@@ -4986,7 +4985,7 @@
       </c>
       <c r="L45" s="65"/>
       <c r="M45" s="226" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N45" s="221"/>
     </row>
@@ -6289,7 +6288,7 @@
     <row r="70" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B71" s="235" t="e">
         <f aca="false">SUM(B46:B69)/Data_category!$L$57</f>
@@ -6343,7 +6342,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B72" s="239" t="e">
         <f aca="false">SUM(B52:B67)/Data_category!$L$57</f>
@@ -6397,7 +6396,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B73" s="243" t="e">
         <f aca="false">B71-B72</f>
@@ -6451,23 +6450,23 @@
     </row>
     <row r="75" s="43" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="83" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B75" s="83"/>
       <c r="C75" s="83" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D75" s="156"/>
       <c r="E75" s="83"/>
       <c r="F75" s="83"/>
       <c r="G75" s="83" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H75" s="83"/>
       <c r="I75" s="83"/>
       <c r="J75" s="295"/>
       <c r="K75" s="83" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L75" s="83"/>
       <c r="M75" s="1"/>
@@ -6475,16 +6474,16 @@
     </row>
     <row r="76" s="43" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="83" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B76" s="83"/>
       <c r="C76" s="83" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E76" s="83"/>
       <c r="F76" s="83"/>
       <c r="G76" s="83" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H76" s="83"/>
       <c r="I76" s="83"/>
@@ -6496,16 +6495,16 @@
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="83" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B77" s="83"/>
       <c r="C77" s="83" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E77" s="83"/>
       <c r="F77" s="83"/>
       <c r="G77" s="83" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H77" s="83"/>
       <c r="I77" s="83"/>
@@ -6515,7 +6514,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="253" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B78" s="253"/>
       <c r="C78" s="253"/>
@@ -6524,7 +6523,7 @@
       <c r="F78" s="253"/>
       <c r="G78" s="253"/>
       <c r="H78" s="253" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I78" s="253"/>
       <c r="J78" s="253"/>
@@ -6635,7 +6634,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -6649,7 +6648,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -6669,7 +6668,7 @@
       <c r="A6" s="15"/>
       <c r="C6" s="19"/>
       <c r="G6" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J6" s="12"/>
       <c r="N6" s="119"/>
@@ -6697,7 +6696,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="217" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B9" s="4" t="n">
         <f aca="false">B4</f>
@@ -6723,7 +6722,7 @@
       <c r="L11" s="257"/>
       <c r="M11" s="258"/>
       <c r="N11" s="221" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6740,7 +6739,7 @@
       <c r="K12" s="178"/>
       <c r="L12" s="259"/>
       <c r="M12" s="260" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N12" s="221"/>
     </row>
@@ -7293,7 +7292,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B39" s="235" t="e">
         <f aca="false">SWISS10_H!B38</f>
@@ -7344,7 +7343,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B40" s="239" t="e">
         <f aca="false">SWISS10_H!B39</f>
@@ -7395,7 +7394,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B41" s="243" t="e">
         <f aca="false">SWISS10_H!B40</f>
@@ -7446,7 +7445,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="217" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B44" s="4" t="n">
         <f aca="false">B5</f>
@@ -7487,7 +7486,7 @@
       <c r="K47" s="284"/>
       <c r="L47" s="284"/>
       <c r="M47" s="226" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N47" s="221"/>
     </row>
@@ -8040,7 +8039,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B74" s="235" t="e">
         <f aca="false">SWISS10_H!B71</f>
@@ -8091,7 +8090,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B75" s="239" t="e">
         <f aca="false">SWISS10_H!B72</f>
@@ -8142,7 +8141,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B76" s="243" t="e">
         <f aca="false">SWISS10_H!B73</f>
@@ -8237,8 +8236,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8301,7 +8300,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -8317,7 +8316,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -8352,13 +8351,13 @@
     </row>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H8" s="20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="217" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B10" s="4" t="n">
         <f aca="false">B4</f>
@@ -8366,7 +8365,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="302"/>
+      <c r="A11" s="302" t="e">
+        <f aca="false">"Vitesse moyenne = " &amp; ROUND(Data_speed!S29,1) &amp; " km/h"</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="B11" s="302"/>
       <c r="C11" s="302"/>
       <c r="D11" s="302"/>
@@ -8405,7 +8407,7 @@
       <c r="L12" s="248"/>
       <c r="M12" s="248"/>
       <c r="O12" s="220" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P12" s="291"/>
       <c r="R12" s="0"/>
@@ -8420,46 +8422,46 @@
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="222" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B13" s="249" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C13" s="151" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D13" s="151" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E13" s="151" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F13" s="151" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G13" s="151" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H13" s="151" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I13" s="151" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J13" s="151" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K13" s="151" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L13" s="151" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M13" s="252" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="O13" s="304" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="P13" s="119"/>
       <c r="R13" s="0"/>
@@ -9970,7 +9972,7 @@
     </row>
     <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B40" s="306" t="e">
         <f aca="false">SUM(B14:B37)/Data_speed!$O$29</f>
@@ -10032,7 +10034,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B41" s="307" t="e">
         <f aca="false">SUM(B20:B35)/Data_speed!$O$29</f>
@@ -10094,7 +10096,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B42" s="308" t="e">
         <f aca="false">B40-B41</f>
@@ -10169,7 +10171,7 @@
     <row r="45" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="217" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B46" s="4" t="n">
         <f aca="false">B5</f>
@@ -10177,7 +10179,10 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="302"/>
+      <c r="A47" s="302" t="e">
+        <f aca="false">"Vitesse moyenne = " &amp; ROUND(Data_speed!S57,1) &amp; " km/h"</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="B47" s="302"/>
       <c r="C47" s="302"/>
       <c r="D47" s="302"/>
@@ -10228,7 +10233,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="222" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B49" s="249" t="str">
         <f aca="false">B13</f>
@@ -11791,7 +11796,7 @@
     </row>
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B76" s="306" t="e">
         <f aca="false">SUM(B50:B73)/Data_speed!$O$57</f>
@@ -11853,7 +11858,7 @@
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B77" s="307" t="e">
         <f aca="false">SUM(B56:B71)/Data_speed!$O$57</f>
@@ -11915,7 +11920,7 @@
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B78" s="308" t="e">
         <f aca="false">B76-B77</f>
@@ -12030,8 +12035,8 @@
   </sheetPr>
   <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12089,7 +12094,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -12104,7 +12109,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -12137,13 +12142,13 @@
     </row>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J8" s="20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="217" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B10" s="4" t="n">
         <f aca="false">B4</f>
@@ -12151,26 +12156,26 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="311" t="str">
+      <c r="A11" s="302" t="str">
         <f aca="false">"Vitesse moyenne = "&amp;INT(V40)&amp;" km/h"</f>
         <v>Vitesse moyenne = 0 km/h</v>
       </c>
-      <c r="B11" s="311"/>
-      <c r="C11" s="311"/>
-      <c r="D11" s="311"/>
-      <c r="E11" s="311"/>
-      <c r="F11" s="311"/>
-      <c r="G11" s="311"/>
-      <c r="H11" s="311"/>
-      <c r="I11" s="311"/>
-      <c r="J11" s="311"/>
-      <c r="K11" s="311"/>
-      <c r="L11" s="311"/>
-      <c r="M11" s="311"/>
-      <c r="N11" s="311"/>
-      <c r="O11" s="311"/>
-      <c r="P11" s="311"/>
-      <c r="Q11" s="311"/>
+      <c r="B11" s="302"/>
+      <c r="C11" s="302"/>
+      <c r="D11" s="302"/>
+      <c r="E11" s="302"/>
+      <c r="F11" s="302"/>
+      <c r="G11" s="302"/>
+      <c r="H11" s="302"/>
+      <c r="I11" s="302"/>
+      <c r="J11" s="302"/>
+      <c r="K11" s="302"/>
+      <c r="L11" s="302"/>
+      <c r="M11" s="302"/>
+      <c r="N11" s="302"/>
+      <c r="O11" s="302"/>
+      <c r="P11" s="302"/>
+      <c r="Q11" s="302"/>
       <c r="R11" s="303"/>
       <c r="S11" s="303"/>
       <c r="T11" s="303"/>
@@ -12192,76 +12197,76 @@
       <c r="K12" s="248"/>
       <c r="L12" s="248"/>
       <c r="M12" s="248"/>
-      <c r="N12" s="312"/>
+      <c r="N12" s="311"/>
       <c r="P12" s="220" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="Q12" s="291"/>
-      <c r="S12" s="313" t="s">
-        <v>174</v>
-      </c>
-      <c r="T12" s="313"/>
-      <c r="U12" s="313"/>
-      <c r="V12" s="313"/>
+      <c r="S12" s="312" t="s">
+        <v>175</v>
+      </c>
+      <c r="T12" s="312"/>
+      <c r="U12" s="312"/>
+      <c r="V12" s="312"/>
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="222" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B13" s="249" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C13" s="249" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D13" s="151" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E13" s="151" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F13" s="151" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G13" s="151" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H13" s="151" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I13" s="151" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J13" s="151" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K13" s="151" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="L13" s="151" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M13" s="151" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="N13" s="252" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="P13" s="304" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="Q13" s="119"/>
-      <c r="S13" s="314" t="s">
-        <v>178</v>
-      </c>
-      <c r="T13" s="315" t="s">
+      <c r="S13" s="313" t="s">
         <v>179</v>
       </c>
-      <c r="U13" s="316" t="s">
+      <c r="T13" s="314" t="s">
         <v>180</v>
       </c>
-      <c r="V13" s="317" t="s">
+      <c r="U13" s="315" t="s">
         <v>181</v>
+      </c>
+      <c r="V13" s="316" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12325,19 +12330,19 @@
         <v>0</v>
       </c>
       <c r="Q14" s="178"/>
-      <c r="S14" s="318" t="n">
+      <c r="S14" s="317" t="n">
         <f aca="false">Data_speed!P5</f>
         <v>0</v>
       </c>
-      <c r="T14" s="318" t="n">
+      <c r="T14" s="317" t="n">
         <f aca="false">Data_speed!Q5</f>
         <v>0</v>
       </c>
-      <c r="U14" s="318" t="n">
+      <c r="U14" s="317" t="n">
         <f aca="false">Data_speed!R5</f>
         <v>0</v>
       </c>
-      <c r="V14" s="319" t="n">
+      <c r="V14" s="318" t="n">
         <f aca="false">Data_speed!S5</f>
         <v>0</v>
       </c>
@@ -12403,19 +12408,19 @@
         <v>0</v>
       </c>
       <c r="Q15" s="178"/>
-      <c r="S15" s="318" t="n">
+      <c r="S15" s="317" t="n">
         <f aca="false">Data_speed!P6</f>
         <v>0</v>
       </c>
-      <c r="T15" s="318" t="n">
+      <c r="T15" s="317" t="n">
         <f aca="false">Data_speed!Q6</f>
         <v>0</v>
       </c>
-      <c r="U15" s="318" t="n">
+      <c r="U15" s="317" t="n">
         <f aca="false">Data_speed!R6</f>
         <v>0</v>
       </c>
-      <c r="V15" s="319" t="n">
+      <c r="V15" s="318" t="n">
         <f aca="false">Data_speed!S6</f>
         <v>0</v>
       </c>
@@ -12481,19 +12486,19 @@
         <v>0</v>
       </c>
       <c r="Q16" s="178"/>
-      <c r="S16" s="318" t="n">
+      <c r="S16" s="317" t="n">
         <f aca="false">Data_speed!P7</f>
         <v>0</v>
       </c>
-      <c r="T16" s="318" t="n">
+      <c r="T16" s="317" t="n">
         <f aca="false">Data_speed!Q7</f>
         <v>0</v>
       </c>
-      <c r="U16" s="318" t="n">
+      <c r="U16" s="317" t="n">
         <f aca="false">Data_speed!R7</f>
         <v>0</v>
       </c>
-      <c r="V16" s="319" t="n">
+      <c r="V16" s="318" t="n">
         <f aca="false">Data_speed!S7</f>
         <v>0</v>
       </c>
@@ -12559,19 +12564,19 @@
         <v>0</v>
       </c>
       <c r="Q17" s="178"/>
-      <c r="S17" s="318" t="n">
+      <c r="S17" s="317" t="n">
         <f aca="false">Data_speed!P8</f>
         <v>0</v>
       </c>
-      <c r="T17" s="318" t="n">
+      <c r="T17" s="317" t="n">
         <f aca="false">Data_speed!Q8</f>
         <v>0</v>
       </c>
-      <c r="U17" s="318" t="n">
+      <c r="U17" s="317" t="n">
         <f aca="false">Data_speed!R8</f>
         <v>0</v>
       </c>
-      <c r="V17" s="319" t="n">
+      <c r="V17" s="318" t="n">
         <f aca="false">Data_speed!S8</f>
         <v>0</v>
       </c>
@@ -12637,19 +12642,19 @@
         <v>0</v>
       </c>
       <c r="Q18" s="178"/>
-      <c r="S18" s="318" t="n">
+      <c r="S18" s="317" t="n">
         <f aca="false">Data_speed!P9</f>
         <v>0</v>
       </c>
-      <c r="T18" s="318" t="n">
+      <c r="T18" s="317" t="n">
         <f aca="false">Data_speed!Q9</f>
         <v>0</v>
       </c>
-      <c r="U18" s="318" t="n">
+      <c r="U18" s="317" t="n">
         <f aca="false">Data_speed!R9</f>
         <v>0</v>
       </c>
-      <c r="V18" s="319" t="n">
+      <c r="V18" s="318" t="n">
         <f aca="false">Data_speed!S9</f>
         <v>0</v>
       </c>
@@ -12715,19 +12720,19 @@
         <v>0</v>
       </c>
       <c r="Q19" s="178"/>
-      <c r="S19" s="318" t="n">
+      <c r="S19" s="317" t="n">
         <f aca="false">Data_speed!P10</f>
         <v>0</v>
       </c>
-      <c r="T19" s="318" t="n">
+      <c r="T19" s="317" t="n">
         <f aca="false">Data_speed!Q10</f>
         <v>0</v>
       </c>
-      <c r="U19" s="318" t="n">
+      <c r="U19" s="317" t="n">
         <f aca="false">Data_speed!R10</f>
         <v>0</v>
       </c>
-      <c r="V19" s="319" t="n">
+      <c r="V19" s="318" t="n">
         <f aca="false">Data_speed!S10</f>
         <v>0</v>
       </c>
@@ -12793,19 +12798,19 @@
         <v>0</v>
       </c>
       <c r="Q20" s="178"/>
-      <c r="S20" s="318" t="n">
+      <c r="S20" s="317" t="n">
         <f aca="false">Data_speed!P11</f>
         <v>0</v>
       </c>
-      <c r="T20" s="318" t="n">
+      <c r="T20" s="317" t="n">
         <f aca="false">Data_speed!Q11</f>
         <v>0</v>
       </c>
-      <c r="U20" s="318" t="n">
+      <c r="U20" s="317" t="n">
         <f aca="false">Data_speed!R11</f>
         <v>0</v>
       </c>
-      <c r="V20" s="319" t="n">
+      <c r="V20" s="318" t="n">
         <f aca="false">Data_speed!S11</f>
         <v>0</v>
       </c>
@@ -12871,19 +12876,19 @@
         <v>0</v>
       </c>
       <c r="Q21" s="178"/>
-      <c r="S21" s="318" t="n">
+      <c r="S21" s="317" t="n">
         <f aca="false">Data_speed!P12</f>
         <v>0</v>
       </c>
-      <c r="T21" s="318" t="n">
+      <c r="T21" s="317" t="n">
         <f aca="false">Data_speed!Q12</f>
         <v>0</v>
       </c>
-      <c r="U21" s="318" t="n">
+      <c r="U21" s="317" t="n">
         <f aca="false">Data_speed!R12</f>
         <v>0</v>
       </c>
-      <c r="V21" s="319" t="n">
+      <c r="V21" s="318" t="n">
         <f aca="false">Data_speed!S12</f>
         <v>0</v>
       </c>
@@ -12949,19 +12954,19 @@
         <v>0</v>
       </c>
       <c r="Q22" s="178"/>
-      <c r="S22" s="318" t="n">
+      <c r="S22" s="317" t="n">
         <f aca="false">Data_speed!P13</f>
         <v>0</v>
       </c>
-      <c r="T22" s="318" t="n">
+      <c r="T22" s="317" t="n">
         <f aca="false">Data_speed!Q13</f>
         <v>0</v>
       </c>
-      <c r="U22" s="318" t="n">
+      <c r="U22" s="317" t="n">
         <f aca="false">Data_speed!R13</f>
         <v>0</v>
       </c>
-      <c r="V22" s="319" t="n">
+      <c r="V22" s="318" t="n">
         <f aca="false">Data_speed!S13</f>
         <v>0</v>
       </c>
@@ -13027,19 +13032,19 @@
         <v>0</v>
       </c>
       <c r="Q23" s="178"/>
-      <c r="S23" s="318" t="n">
+      <c r="S23" s="317" t="n">
         <f aca="false">Data_speed!P14</f>
         <v>0</v>
       </c>
-      <c r="T23" s="318" t="n">
+      <c r="T23" s="317" t="n">
         <f aca="false">Data_speed!Q14</f>
         <v>0</v>
       </c>
-      <c r="U23" s="318" t="n">
+      <c r="U23" s="317" t="n">
         <f aca="false">Data_speed!R14</f>
         <v>0</v>
       </c>
-      <c r="V23" s="319" t="n">
+      <c r="V23" s="318" t="n">
         <f aca="false">Data_speed!S14</f>
         <v>0</v>
       </c>
@@ -13105,19 +13110,19 @@
         <v>0</v>
       </c>
       <c r="Q24" s="178"/>
-      <c r="S24" s="318" t="n">
+      <c r="S24" s="317" t="n">
         <f aca="false">Data_speed!P15</f>
         <v>0</v>
       </c>
-      <c r="T24" s="318" t="n">
+      <c r="T24" s="317" t="n">
         <f aca="false">Data_speed!Q15</f>
         <v>0</v>
       </c>
-      <c r="U24" s="318" t="n">
+      <c r="U24" s="317" t="n">
         <f aca="false">Data_speed!R15</f>
         <v>0</v>
       </c>
-      <c r="V24" s="319" t="n">
+      <c r="V24" s="318" t="n">
         <f aca="false">Data_speed!S15</f>
         <v>0</v>
       </c>
@@ -13183,19 +13188,19 @@
         <v>0</v>
       </c>
       <c r="Q25" s="178"/>
-      <c r="S25" s="318" t="n">
+      <c r="S25" s="317" t="n">
         <f aca="false">Data_speed!P16</f>
         <v>0</v>
       </c>
-      <c r="T25" s="318" t="n">
+      <c r="T25" s="317" t="n">
         <f aca="false">Data_speed!Q16</f>
         <v>0</v>
       </c>
-      <c r="U25" s="318" t="n">
+      <c r="U25" s="317" t="n">
         <f aca="false">Data_speed!R16</f>
         <v>0</v>
       </c>
-      <c r="V25" s="319" t="n">
+      <c r="V25" s="318" t="n">
         <f aca="false">Data_speed!S16</f>
         <v>0</v>
       </c>
@@ -13261,19 +13266,19 @@
         <v>0</v>
       </c>
       <c r="Q26" s="178"/>
-      <c r="S26" s="318" t="n">
+      <c r="S26" s="317" t="n">
         <f aca="false">Data_speed!P17</f>
         <v>0</v>
       </c>
-      <c r="T26" s="318" t="n">
+      <c r="T26" s="317" t="n">
         <f aca="false">Data_speed!Q17</f>
         <v>0</v>
       </c>
-      <c r="U26" s="318" t="n">
+      <c r="U26" s="317" t="n">
         <f aca="false">Data_speed!R17</f>
         <v>0</v>
       </c>
-      <c r="V26" s="319" t="n">
+      <c r="V26" s="318" t="n">
         <f aca="false">Data_speed!S17</f>
         <v>0</v>
       </c>
@@ -13339,19 +13344,19 @@
         <v>0</v>
       </c>
       <c r="Q27" s="178"/>
-      <c r="S27" s="318" t="n">
+      <c r="S27" s="317" t="n">
         <f aca="false">Data_speed!P18</f>
         <v>0</v>
       </c>
-      <c r="T27" s="318" t="n">
+      <c r="T27" s="317" t="n">
         <f aca="false">Data_speed!Q18</f>
         <v>0</v>
       </c>
-      <c r="U27" s="318" t="n">
+      <c r="U27" s="317" t="n">
         <f aca="false">Data_speed!R18</f>
         <v>0</v>
       </c>
-      <c r="V27" s="319" t="n">
+      <c r="V27" s="318" t="n">
         <f aca="false">Data_speed!S18</f>
         <v>0</v>
       </c>
@@ -13417,19 +13422,19 @@
         <v>0</v>
       </c>
       <c r="Q28" s="178"/>
-      <c r="S28" s="318" t="n">
+      <c r="S28" s="317" t="n">
         <f aca="false">Data_speed!P19</f>
         <v>0</v>
       </c>
-      <c r="T28" s="318" t="n">
+      <c r="T28" s="317" t="n">
         <f aca="false">Data_speed!Q19</f>
         <v>0</v>
       </c>
-      <c r="U28" s="318" t="n">
+      <c r="U28" s="317" t="n">
         <f aca="false">Data_speed!R19</f>
         <v>0</v>
       </c>
-      <c r="V28" s="319" t="n">
+      <c r="V28" s="318" t="n">
         <f aca="false">Data_speed!S19</f>
         <v>0</v>
       </c>
@@ -13495,19 +13500,19 @@
         <v>0</v>
       </c>
       <c r="Q29" s="178"/>
-      <c r="S29" s="318" t="n">
+      <c r="S29" s="317" t="n">
         <f aca="false">Data_speed!P20</f>
         <v>0</v>
       </c>
-      <c r="T29" s="318" t="n">
+      <c r="T29" s="317" t="n">
         <f aca="false">Data_speed!Q20</f>
         <v>0</v>
       </c>
-      <c r="U29" s="318" t="n">
+      <c r="U29" s="317" t="n">
         <f aca="false">Data_speed!R20</f>
         <v>0</v>
       </c>
-      <c r="V29" s="319" t="n">
+      <c r="V29" s="318" t="n">
         <f aca="false">Data_speed!S20</f>
         <v>0</v>
       </c>
@@ -13573,19 +13578,19 @@
         <v>0</v>
       </c>
       <c r="Q30" s="178"/>
-      <c r="S30" s="318" t="n">
+      <c r="S30" s="317" t="n">
         <f aca="false">Data_speed!P21</f>
         <v>0</v>
       </c>
-      <c r="T30" s="318" t="n">
+      <c r="T30" s="317" t="n">
         <f aca="false">Data_speed!Q21</f>
         <v>0</v>
       </c>
-      <c r="U30" s="318" t="n">
+      <c r="U30" s="317" t="n">
         <f aca="false">Data_speed!R21</f>
         <v>0</v>
       </c>
-      <c r="V30" s="319" t="n">
+      <c r="V30" s="318" t="n">
         <f aca="false">Data_speed!S21</f>
         <v>0</v>
       </c>
@@ -13651,19 +13656,19 @@
         <v>0</v>
       </c>
       <c r="Q31" s="178"/>
-      <c r="S31" s="318" t="n">
+      <c r="S31" s="317" t="n">
         <f aca="false">Data_speed!P22</f>
         <v>0</v>
       </c>
-      <c r="T31" s="318" t="n">
+      <c r="T31" s="317" t="n">
         <f aca="false">Data_speed!Q22</f>
         <v>0</v>
       </c>
-      <c r="U31" s="318" t="n">
+      <c r="U31" s="317" t="n">
         <f aca="false">Data_speed!R22</f>
         <v>0</v>
       </c>
-      <c r="V31" s="319" t="n">
+      <c r="V31" s="318" t="n">
         <f aca="false">Data_speed!S22</f>
         <v>0</v>
       </c>
@@ -13729,19 +13734,19 @@
         <v>0</v>
       </c>
       <c r="Q32" s="178"/>
-      <c r="S32" s="318" t="n">
+      <c r="S32" s="317" t="n">
         <f aca="false">Data_speed!P23</f>
         <v>0</v>
       </c>
-      <c r="T32" s="318" t="n">
+      <c r="T32" s="317" t="n">
         <f aca="false">Data_speed!Q23</f>
         <v>0</v>
       </c>
-      <c r="U32" s="318" t="n">
+      <c r="U32" s="317" t="n">
         <f aca="false">Data_speed!R23</f>
         <v>0</v>
       </c>
-      <c r="V32" s="319" t="n">
+      <c r="V32" s="318" t="n">
         <f aca="false">Data_speed!S23</f>
         <v>0</v>
       </c>
@@ -13807,19 +13812,19 @@
         <v>0</v>
       </c>
       <c r="Q33" s="178"/>
-      <c r="S33" s="318" t="n">
+      <c r="S33" s="317" t="n">
         <f aca="false">Data_speed!P24</f>
         <v>0</v>
       </c>
-      <c r="T33" s="318" t="n">
+      <c r="T33" s="317" t="n">
         <f aca="false">Data_speed!Q24</f>
         <v>0</v>
       </c>
-      <c r="U33" s="318" t="n">
+      <c r="U33" s="317" t="n">
         <f aca="false">Data_speed!R24</f>
         <v>0</v>
       </c>
-      <c r="V33" s="319" t="n">
+      <c r="V33" s="318" t="n">
         <f aca="false">Data_speed!S24</f>
         <v>0</v>
       </c>
@@ -13885,19 +13890,19 @@
         <v>0</v>
       </c>
       <c r="Q34" s="178"/>
-      <c r="S34" s="318" t="n">
+      <c r="S34" s="317" t="n">
         <f aca="false">Data_speed!P25</f>
         <v>0</v>
       </c>
-      <c r="T34" s="318" t="n">
+      <c r="T34" s="317" t="n">
         <f aca="false">Data_speed!Q25</f>
         <v>0</v>
       </c>
-      <c r="U34" s="318" t="n">
+      <c r="U34" s="317" t="n">
         <f aca="false">Data_speed!R25</f>
         <v>0</v>
       </c>
-      <c r="V34" s="319" t="n">
+      <c r="V34" s="318" t="n">
         <f aca="false">Data_speed!S25</f>
         <v>0</v>
       </c>
@@ -13963,19 +13968,19 @@
         <v>0</v>
       </c>
       <c r="Q35" s="178"/>
-      <c r="S35" s="318" t="n">
+      <c r="S35" s="317" t="n">
         <f aca="false">Data_speed!P26</f>
         <v>0</v>
       </c>
-      <c r="T35" s="318" t="n">
+      <c r="T35" s="317" t="n">
         <f aca="false">Data_speed!Q26</f>
         <v>0</v>
       </c>
-      <c r="U35" s="318" t="n">
+      <c r="U35" s="317" t="n">
         <f aca="false">Data_speed!R26</f>
         <v>0</v>
       </c>
-      <c r="V35" s="319" t="n">
+      <c r="V35" s="318" t="n">
         <f aca="false">Data_speed!S26</f>
         <v>0</v>
       </c>
@@ -14041,19 +14046,19 @@
         <v>0</v>
       </c>
       <c r="Q36" s="178"/>
-      <c r="S36" s="318" t="n">
+      <c r="S36" s="317" t="n">
         <f aca="false">Data_speed!P27</f>
         <v>0</v>
       </c>
-      <c r="T36" s="318" t="n">
+      <c r="T36" s="317" t="n">
         <f aca="false">Data_speed!Q27</f>
         <v>0</v>
       </c>
-      <c r="U36" s="318" t="n">
+      <c r="U36" s="317" t="n">
         <f aca="false">Data_speed!R27</f>
         <v>0</v>
       </c>
-      <c r="V36" s="319" t="n">
+      <c r="V36" s="318" t="n">
         <f aca="false">Data_speed!S27</f>
         <v>0</v>
       </c>
@@ -14119,19 +14124,19 @@
         <v>0</v>
       </c>
       <c r="Q37" s="178"/>
-      <c r="S37" s="318" t="n">
+      <c r="S37" s="317" t="n">
         <f aca="false">Data_speed!P28</f>
         <v>0</v>
       </c>
-      <c r="T37" s="318" t="n">
+      <c r="T37" s="317" t="n">
         <f aca="false">Data_speed!Q28</f>
         <v>0</v>
       </c>
-      <c r="U37" s="318" t="n">
+      <c r="U37" s="317" t="n">
         <f aca="false">Data_speed!R28</f>
         <v>0</v>
       </c>
-      <c r="V37" s="319" t="n">
+      <c r="V37" s="318" t="n">
         <f aca="false">Data_speed!S28</f>
         <v>0</v>
       </c>
@@ -14152,7 +14157,7 @@
     </row>
     <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B40" s="306" t="e">
         <f aca="false">SUM(B14:B37)/Data_speed!$O$29</f>
@@ -14211,26 +14216,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q40" s="293"/>
-      <c r="S40" s="320" t="n">
+      <c r="S40" s="319" t="n">
         <f aca="false">AVERAGE(S14:S37)</f>
         <v>0</v>
       </c>
-      <c r="T40" s="320" t="n">
+      <c r="T40" s="319" t="n">
         <f aca="false">AVERAGE(T14:T37)</f>
         <v>0</v>
       </c>
-      <c r="U40" s="320" t="n">
+      <c r="U40" s="319" t="n">
         <f aca="false">AVERAGE(U14:U37)</f>
         <v>0</v>
       </c>
-      <c r="V40" s="321" t="n">
+      <c r="V40" s="320" t="n">
         <f aca="false">AVERAGE(V14:V37)</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B41" s="307" t="e">
         <f aca="false">SUM(B20:B35)/Data_speed!$O$29</f>
@@ -14289,26 +14294,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q41" s="293"/>
-      <c r="S41" s="322" t="n">
+      <c r="S41" s="321" t="n">
         <f aca="false">AVERAGE(S20:S35)</f>
         <v>0</v>
       </c>
-      <c r="T41" s="322" t="n">
+      <c r="T41" s="321" t="n">
         <f aca="false">AVERAGE(T20:T35)</f>
         <v>0</v>
       </c>
-      <c r="U41" s="322" t="n">
+      <c r="U41" s="321" t="n">
         <f aca="false">AVERAGE(U20:U35)</f>
         <v>0</v>
       </c>
-      <c r="V41" s="323" t="n">
+      <c r="V41" s="322" t="n">
         <f aca="false">AVERAGE(V20:V35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B42" s="308" t="e">
         <f aca="false">B40-B41</f>
@@ -14368,19 +14373,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q42" s="293"/>
-      <c r="S42" s="324" t="n">
+      <c r="S42" s="323" t="n">
         <f aca="false">AVERAGE(AVERAGE(S14:S19), AVERAGE(S36:S37))</f>
         <v>0</v>
       </c>
-      <c r="T42" s="324" t="n">
+      <c r="T42" s="323" t="n">
         <f aca="false">AVERAGE(AVERAGE(T14:T19), AVERAGE(T36:T37))</f>
         <v>0</v>
       </c>
-      <c r="U42" s="324" t="n">
+      <c r="U42" s="323" t="n">
         <f aca="false">AVERAGE(AVERAGE(U14:U19), AVERAGE(U36:U37))</f>
         <v>0</v>
       </c>
-      <c r="V42" s="325" t="n">
+      <c r="V42" s="324" t="n">
         <f aca="false">AVERAGE(AVERAGE(V14:V19), AVERAGE(V36:V37))</f>
         <v>0</v>
       </c>
@@ -14404,7 +14409,7 @@
     </row>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="217" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B46" s="4" t="n">
         <f aca="false">B5</f>
@@ -14413,26 +14418,26 @@
       <c r="V46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="311" t="str">
+      <c r="A47" s="302" t="str">
         <f aca="false">"Vitesse moyenne = "&amp;INT(V76)&amp;" km/h"</f>
         <v>Vitesse moyenne = 0 km/h</v>
       </c>
-      <c r="B47" s="311"/>
-      <c r="C47" s="311"/>
-      <c r="D47" s="311"/>
-      <c r="E47" s="311"/>
-      <c r="F47" s="311"/>
-      <c r="G47" s="311"/>
-      <c r="H47" s="311"/>
-      <c r="I47" s="311"/>
-      <c r="J47" s="311"/>
-      <c r="K47" s="311"/>
-      <c r="L47" s="311"/>
-      <c r="M47" s="311"/>
-      <c r="N47" s="311"/>
-      <c r="O47" s="311"/>
-      <c r="P47" s="311"/>
-      <c r="Q47" s="311"/>
+      <c r="B47" s="302"/>
+      <c r="C47" s="302"/>
+      <c r="D47" s="302"/>
+      <c r="E47" s="302"/>
+      <c r="F47" s="302"/>
+      <c r="G47" s="302"/>
+      <c r="H47" s="302"/>
+      <c r="I47" s="302"/>
+      <c r="J47" s="302"/>
+      <c r="K47" s="302"/>
+      <c r="L47" s="302"/>
+      <c r="M47" s="302"/>
+      <c r="N47" s="302"/>
+      <c r="O47" s="302"/>
+      <c r="P47" s="302"/>
+      <c r="Q47" s="302"/>
       <c r="R47" s="303"/>
       <c r="S47" s="303"/>
       <c r="T47" s="303"/>
@@ -14455,24 +14460,24 @@
       <c r="K48" s="248"/>
       <c r="L48" s="248"/>
       <c r="M48" s="248"/>
-      <c r="N48" s="312"/>
+      <c r="N48" s="311"/>
       <c r="P48" s="220" t="str">
         <f aca="false">P12</f>
         <v>THM</v>
       </c>
       <c r="Q48" s="291"/>
       <c r="R48" s="187"/>
-      <c r="S48" s="313" t="str">
+      <c r="S48" s="312" t="str">
         <f aca="false">S12</f>
         <v>Vitesses caractéristiques</v>
       </c>
-      <c r="T48" s="313"/>
-      <c r="U48" s="313"/>
-      <c r="V48" s="313"/>
+      <c r="T48" s="312"/>
+      <c r="U48" s="312"/>
+      <c r="V48" s="312"/>
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="222" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B49" s="249" t="str">
         <f aca="false">B13</f>
@@ -14531,19 +14536,19 @@
         <v>Véh/h</v>
       </c>
       <c r="Q49" s="119"/>
-      <c r="S49" s="314" t="str">
+      <c r="S49" s="313" t="str">
         <f aca="false">S13</f>
         <v>V15</v>
       </c>
-      <c r="T49" s="315" t="str">
+      <c r="T49" s="314" t="str">
         <f aca="false">T13</f>
         <v>V50</v>
       </c>
-      <c r="U49" s="316" t="str">
+      <c r="U49" s="315" t="str">
         <f aca="false">U13</f>
         <v>V85</v>
       </c>
-      <c r="V49" s="326" t="str">
+      <c r="V49" s="325" t="str">
         <f aca="false">V13</f>
         <v>Vmt</v>
       </c>
@@ -14609,19 +14614,19 @@
         <v>0</v>
       </c>
       <c r="Q50" s="178"/>
-      <c r="S50" s="318" t="n">
+      <c r="S50" s="317" t="n">
         <f aca="false">Data_speed!P33</f>
         <v>0</v>
       </c>
-      <c r="T50" s="318" t="n">
+      <c r="T50" s="317" t="n">
         <f aca="false">Data_speed!Q33</f>
         <v>0</v>
       </c>
-      <c r="U50" s="318" t="n">
+      <c r="U50" s="317" t="n">
         <f aca="false">Data_speed!R33</f>
         <v>0</v>
       </c>
-      <c r="V50" s="319" t="n">
+      <c r="V50" s="318" t="n">
         <f aca="false">Data_speed!S33</f>
         <v>0</v>
       </c>
@@ -14687,19 +14692,19 @@
         <v>0</v>
       </c>
       <c r="Q51" s="178"/>
-      <c r="S51" s="318" t="n">
+      <c r="S51" s="317" t="n">
         <f aca="false">Data_speed!P34</f>
         <v>0</v>
       </c>
-      <c r="T51" s="318" t="n">
+      <c r="T51" s="317" t="n">
         <f aca="false">Data_speed!Q34</f>
         <v>0</v>
       </c>
-      <c r="U51" s="318" t="n">
+      <c r="U51" s="317" t="n">
         <f aca="false">Data_speed!R34</f>
         <v>0</v>
       </c>
-      <c r="V51" s="319" t="n">
+      <c r="V51" s="318" t="n">
         <f aca="false">Data_speed!S34</f>
         <v>0</v>
       </c>
@@ -14765,19 +14770,19 @@
         <v>0</v>
       </c>
       <c r="Q52" s="178"/>
-      <c r="S52" s="318" t="n">
+      <c r="S52" s="317" t="n">
         <f aca="false">Data_speed!P35</f>
         <v>0</v>
       </c>
-      <c r="T52" s="318" t="n">
+      <c r="T52" s="317" t="n">
         <f aca="false">Data_speed!Q35</f>
         <v>0</v>
       </c>
-      <c r="U52" s="318" t="n">
+      <c r="U52" s="317" t="n">
         <f aca="false">Data_speed!R35</f>
         <v>0</v>
       </c>
-      <c r="V52" s="319" t="n">
+      <c r="V52" s="318" t="n">
         <f aca="false">Data_speed!S35</f>
         <v>0</v>
       </c>
@@ -14843,19 +14848,19 @@
         <v>0</v>
       </c>
       <c r="Q53" s="178"/>
-      <c r="S53" s="318" t="n">
+      <c r="S53" s="317" t="n">
         <f aca="false">Data_speed!P36</f>
         <v>0</v>
       </c>
-      <c r="T53" s="318" t="n">
+      <c r="T53" s="317" t="n">
         <f aca="false">Data_speed!Q36</f>
         <v>0</v>
       </c>
-      <c r="U53" s="318" t="n">
+      <c r="U53" s="317" t="n">
         <f aca="false">Data_speed!R36</f>
         <v>0</v>
       </c>
-      <c r="V53" s="319" t="n">
+      <c r="V53" s="318" t="n">
         <f aca="false">Data_speed!S36</f>
         <v>0</v>
       </c>
@@ -14921,19 +14926,19 @@
         <v>0</v>
       </c>
       <c r="Q54" s="178"/>
-      <c r="S54" s="318" t="n">
+      <c r="S54" s="317" t="n">
         <f aca="false">Data_speed!P37</f>
         <v>0</v>
       </c>
-      <c r="T54" s="318" t="n">
+      <c r="T54" s="317" t="n">
         <f aca="false">Data_speed!Q37</f>
         <v>0</v>
       </c>
-      <c r="U54" s="318" t="n">
+      <c r="U54" s="317" t="n">
         <f aca="false">Data_speed!R37</f>
         <v>0</v>
       </c>
-      <c r="V54" s="319" t="n">
+      <c r="V54" s="318" t="n">
         <f aca="false">Data_speed!S37</f>
         <v>0</v>
       </c>
@@ -14999,19 +15004,19 @@
         <v>0</v>
       </c>
       <c r="Q55" s="178"/>
-      <c r="S55" s="318" t="n">
+      <c r="S55" s="317" t="n">
         <f aca="false">Data_speed!P38</f>
         <v>0</v>
       </c>
-      <c r="T55" s="318" t="n">
+      <c r="T55" s="317" t="n">
         <f aca="false">Data_speed!Q38</f>
         <v>0</v>
       </c>
-      <c r="U55" s="318" t="n">
+      <c r="U55" s="317" t="n">
         <f aca="false">Data_speed!R38</f>
         <v>0</v>
       </c>
-      <c r="V55" s="319" t="n">
+      <c r="V55" s="318" t="n">
         <f aca="false">Data_speed!S38</f>
         <v>0</v>
       </c>
@@ -15077,19 +15082,19 @@
         <v>0</v>
       </c>
       <c r="Q56" s="178"/>
-      <c r="S56" s="318" t="n">
+      <c r="S56" s="317" t="n">
         <f aca="false">Data_speed!P39</f>
         <v>0</v>
       </c>
-      <c r="T56" s="318" t="n">
+      <c r="T56" s="317" t="n">
         <f aca="false">Data_speed!Q39</f>
         <v>0</v>
       </c>
-      <c r="U56" s="318" t="n">
+      <c r="U56" s="317" t="n">
         <f aca="false">Data_speed!R39</f>
         <v>0</v>
       </c>
-      <c r="V56" s="319" t="n">
+      <c r="V56" s="318" t="n">
         <f aca="false">Data_speed!S39</f>
         <v>0</v>
       </c>
@@ -15155,19 +15160,19 @@
         <v>0</v>
       </c>
       <c r="Q57" s="178"/>
-      <c r="S57" s="318" t="n">
+      <c r="S57" s="317" t="n">
         <f aca="false">Data_speed!P40</f>
         <v>0</v>
       </c>
-      <c r="T57" s="318" t="n">
+      <c r="T57" s="317" t="n">
         <f aca="false">Data_speed!Q40</f>
         <v>0</v>
       </c>
-      <c r="U57" s="318" t="n">
+      <c r="U57" s="317" t="n">
         <f aca="false">Data_speed!R40</f>
         <v>0</v>
       </c>
-      <c r="V57" s="319" t="n">
+      <c r="V57" s="318" t="n">
         <f aca="false">Data_speed!S40</f>
         <v>0</v>
       </c>
@@ -15233,19 +15238,19 @@
         <v>0</v>
       </c>
       <c r="Q58" s="178"/>
-      <c r="S58" s="318" t="n">
+      <c r="S58" s="317" t="n">
         <f aca="false">Data_speed!P41</f>
         <v>0</v>
       </c>
-      <c r="T58" s="318" t="n">
+      <c r="T58" s="317" t="n">
         <f aca="false">Data_speed!Q41</f>
         <v>0</v>
       </c>
-      <c r="U58" s="318" t="n">
+      <c r="U58" s="317" t="n">
         <f aca="false">Data_speed!R41</f>
         <v>0</v>
       </c>
-      <c r="V58" s="319" t="n">
+      <c r="V58" s="318" t="n">
         <f aca="false">Data_speed!S41</f>
         <v>0</v>
       </c>
@@ -15311,19 +15316,19 @@
         <v>0</v>
       </c>
       <c r="Q59" s="178"/>
-      <c r="S59" s="318" t="n">
+      <c r="S59" s="317" t="n">
         <f aca="false">Data_speed!P42</f>
         <v>0</v>
       </c>
-      <c r="T59" s="318" t="n">
+      <c r="T59" s="317" t="n">
         <f aca="false">Data_speed!Q42</f>
         <v>0</v>
       </c>
-      <c r="U59" s="318" t="n">
+      <c r="U59" s="317" t="n">
         <f aca="false">Data_speed!R42</f>
         <v>0</v>
       </c>
-      <c r="V59" s="319" t="n">
+      <c r="V59" s="318" t="n">
         <f aca="false">Data_speed!S42</f>
         <v>0</v>
       </c>
@@ -15389,19 +15394,19 @@
         <v>0</v>
       </c>
       <c r="Q60" s="178"/>
-      <c r="S60" s="318" t="n">
+      <c r="S60" s="317" t="n">
         <f aca="false">Data_speed!P43</f>
         <v>0</v>
       </c>
-      <c r="T60" s="318" t="n">
+      <c r="T60" s="317" t="n">
         <f aca="false">Data_speed!Q43</f>
         <v>0</v>
       </c>
-      <c r="U60" s="318" t="n">
+      <c r="U60" s="317" t="n">
         <f aca="false">Data_speed!R43</f>
         <v>0</v>
       </c>
-      <c r="V60" s="319" t="n">
+      <c r="V60" s="318" t="n">
         <f aca="false">Data_speed!S43</f>
         <v>0</v>
       </c>
@@ -15467,19 +15472,19 @@
         <v>0</v>
       </c>
       <c r="Q61" s="178"/>
-      <c r="S61" s="318" t="n">
+      <c r="S61" s="317" t="n">
         <f aca="false">Data_speed!P44</f>
         <v>0</v>
       </c>
-      <c r="T61" s="318" t="n">
+      <c r="T61" s="317" t="n">
         <f aca="false">Data_speed!Q44</f>
         <v>0</v>
       </c>
-      <c r="U61" s="318" t="n">
+      <c r="U61" s="317" t="n">
         <f aca="false">Data_speed!R44</f>
         <v>0</v>
       </c>
-      <c r="V61" s="319" t="n">
+      <c r="V61" s="318" t="n">
         <f aca="false">Data_speed!S44</f>
         <v>0</v>
       </c>
@@ -15545,19 +15550,19 @@
         <v>0</v>
       </c>
       <c r="Q62" s="178"/>
-      <c r="S62" s="318" t="n">
+      <c r="S62" s="317" t="n">
         <f aca="false">Data_speed!P45</f>
         <v>0</v>
       </c>
-      <c r="T62" s="318" t="n">
+      <c r="T62" s="317" t="n">
         <f aca="false">Data_speed!Q45</f>
         <v>0</v>
       </c>
-      <c r="U62" s="318" t="n">
+      <c r="U62" s="317" t="n">
         <f aca="false">Data_speed!R45</f>
         <v>0</v>
       </c>
-      <c r="V62" s="319" t="n">
+      <c r="V62" s="318" t="n">
         <f aca="false">Data_speed!S45</f>
         <v>0</v>
       </c>
@@ -15623,19 +15628,19 @@
         <v>0</v>
       </c>
       <c r="Q63" s="178"/>
-      <c r="S63" s="318" t="n">
+      <c r="S63" s="317" t="n">
         <f aca="false">Data_speed!P46</f>
         <v>0</v>
       </c>
-      <c r="T63" s="318" t="n">
+      <c r="T63" s="317" t="n">
         <f aca="false">Data_speed!Q46</f>
         <v>0</v>
       </c>
-      <c r="U63" s="318" t="n">
+      <c r="U63" s="317" t="n">
         <f aca="false">Data_speed!R46</f>
         <v>0</v>
       </c>
-      <c r="V63" s="319" t="n">
+      <c r="V63" s="318" t="n">
         <f aca="false">Data_speed!S46</f>
         <v>0</v>
       </c>
@@ -15701,19 +15706,19 @@
         <v>0</v>
       </c>
       <c r="Q64" s="178"/>
-      <c r="S64" s="318" t="n">
+      <c r="S64" s="317" t="n">
         <f aca="false">Data_speed!P47</f>
         <v>0</v>
       </c>
-      <c r="T64" s="318" t="n">
+      <c r="T64" s="317" t="n">
         <f aca="false">Data_speed!Q47</f>
         <v>0</v>
       </c>
-      <c r="U64" s="318" t="n">
+      <c r="U64" s="317" t="n">
         <f aca="false">Data_speed!R47</f>
         <v>0</v>
       </c>
-      <c r="V64" s="319" t="n">
+      <c r="V64" s="318" t="n">
         <f aca="false">Data_speed!S47</f>
         <v>0</v>
       </c>
@@ -15779,19 +15784,19 @@
         <v>0</v>
       </c>
       <c r="Q65" s="178"/>
-      <c r="S65" s="318" t="n">
+      <c r="S65" s="317" t="n">
         <f aca="false">Data_speed!P48</f>
         <v>0</v>
       </c>
-      <c r="T65" s="318" t="n">
+      <c r="T65" s="317" t="n">
         <f aca="false">Data_speed!Q48</f>
         <v>0</v>
       </c>
-      <c r="U65" s="318" t="n">
+      <c r="U65" s="317" t="n">
         <f aca="false">Data_speed!R48</f>
         <v>0</v>
       </c>
-      <c r="V65" s="319" t="n">
+      <c r="V65" s="318" t="n">
         <f aca="false">Data_speed!S48</f>
         <v>0</v>
       </c>
@@ -15857,19 +15862,19 @@
         <v>0</v>
       </c>
       <c r="Q66" s="178"/>
-      <c r="S66" s="318" t="n">
+      <c r="S66" s="317" t="n">
         <f aca="false">Data_speed!P49</f>
         <v>0</v>
       </c>
-      <c r="T66" s="318" t="n">
+      <c r="T66" s="317" t="n">
         <f aca="false">Data_speed!Q49</f>
         <v>0</v>
       </c>
-      <c r="U66" s="318" t="n">
+      <c r="U66" s="317" t="n">
         <f aca="false">Data_speed!R49</f>
         <v>0</v>
       </c>
-      <c r="V66" s="319" t="n">
+      <c r="V66" s="318" t="n">
         <f aca="false">Data_speed!S49</f>
         <v>0</v>
       </c>
@@ -15935,19 +15940,19 @@
         <v>0</v>
       </c>
       <c r="Q67" s="178"/>
-      <c r="S67" s="318" t="n">
+      <c r="S67" s="317" t="n">
         <f aca="false">Data_speed!P50</f>
         <v>0</v>
       </c>
-      <c r="T67" s="318" t="n">
+      <c r="T67" s="317" t="n">
         <f aca="false">Data_speed!Q50</f>
         <v>0</v>
       </c>
-      <c r="U67" s="318" t="n">
+      <c r="U67" s="317" t="n">
         <f aca="false">Data_speed!R50</f>
         <v>0</v>
       </c>
-      <c r="V67" s="319" t="n">
+      <c r="V67" s="318" t="n">
         <f aca="false">Data_speed!S50</f>
         <v>0</v>
       </c>
@@ -16013,19 +16018,19 @@
         <v>0</v>
       </c>
       <c r="Q68" s="178"/>
-      <c r="S68" s="318" t="n">
+      <c r="S68" s="317" t="n">
         <f aca="false">Data_speed!P51</f>
         <v>0</v>
       </c>
-      <c r="T68" s="318" t="n">
+      <c r="T68" s="317" t="n">
         <f aca="false">Data_speed!Q51</f>
         <v>0</v>
       </c>
-      <c r="U68" s="318" t="n">
+      <c r="U68" s="317" t="n">
         <f aca="false">Data_speed!R51</f>
         <v>0</v>
       </c>
-      <c r="V68" s="319" t="n">
+      <c r="V68" s="318" t="n">
         <f aca="false">Data_speed!S51</f>
         <v>0</v>
       </c>
@@ -16091,19 +16096,19 @@
         <v>0</v>
       </c>
       <c r="Q69" s="178"/>
-      <c r="S69" s="318" t="n">
+      <c r="S69" s="317" t="n">
         <f aca="false">Data_speed!P52</f>
         <v>0</v>
       </c>
-      <c r="T69" s="318" t="n">
+      <c r="T69" s="317" t="n">
         <f aca="false">Data_speed!Q52</f>
         <v>0</v>
       </c>
-      <c r="U69" s="318" t="n">
+      <c r="U69" s="317" t="n">
         <f aca="false">Data_speed!R52</f>
         <v>0</v>
       </c>
-      <c r="V69" s="319" t="n">
+      <c r="V69" s="318" t="n">
         <f aca="false">Data_speed!S52</f>
         <v>0</v>
       </c>
@@ -16169,19 +16174,19 @@
         <v>0</v>
       </c>
       <c r="Q70" s="178"/>
-      <c r="S70" s="318" t="n">
+      <c r="S70" s="317" t="n">
         <f aca="false">Data_speed!P53</f>
         <v>0</v>
       </c>
-      <c r="T70" s="318" t="n">
+      <c r="T70" s="317" t="n">
         <f aca="false">Data_speed!Q53</f>
         <v>0</v>
       </c>
-      <c r="U70" s="318" t="n">
+      <c r="U70" s="317" t="n">
         <f aca="false">Data_speed!R53</f>
         <v>0</v>
       </c>
-      <c r="V70" s="319" t="n">
+      <c r="V70" s="318" t="n">
         <f aca="false">Data_speed!S53</f>
         <v>0</v>
       </c>
@@ -16247,19 +16252,19 @@
         <v>0</v>
       </c>
       <c r="Q71" s="178"/>
-      <c r="S71" s="318" t="n">
+      <c r="S71" s="317" t="n">
         <f aca="false">Data_speed!P54</f>
         <v>0</v>
       </c>
-      <c r="T71" s="318" t="n">
+      <c r="T71" s="317" t="n">
         <f aca="false">Data_speed!Q54</f>
         <v>0</v>
       </c>
-      <c r="U71" s="318" t="n">
+      <c r="U71" s="317" t="n">
         <f aca="false">Data_speed!R54</f>
         <v>0</v>
       </c>
-      <c r="V71" s="319" t="n">
+      <c r="V71" s="318" t="n">
         <f aca="false">Data_speed!S54</f>
         <v>0</v>
       </c>
@@ -16325,19 +16330,19 @@
         <v>0</v>
       </c>
       <c r="Q72" s="178"/>
-      <c r="S72" s="318" t="n">
+      <c r="S72" s="317" t="n">
         <f aca="false">Data_speed!P55</f>
         <v>0</v>
       </c>
-      <c r="T72" s="318" t="n">
+      <c r="T72" s="317" t="n">
         <f aca="false">Data_speed!Q55</f>
         <v>0</v>
       </c>
-      <c r="U72" s="318" t="n">
+      <c r="U72" s="317" t="n">
         <f aca="false">Data_speed!R55</f>
         <v>0</v>
       </c>
-      <c r="V72" s="319" t="n">
+      <c r="V72" s="318" t="n">
         <f aca="false">Data_speed!S55</f>
         <v>0</v>
       </c>
@@ -16403,19 +16408,19 @@
         <v>0</v>
       </c>
       <c r="Q73" s="178"/>
-      <c r="S73" s="318" t="n">
+      <c r="S73" s="317" t="n">
         <f aca="false">Data_speed!P56</f>
         <v>0</v>
       </c>
-      <c r="T73" s="318" t="n">
+      <c r="T73" s="317" t="n">
         <f aca="false">Data_speed!Q56</f>
         <v>0</v>
       </c>
-      <c r="U73" s="318" t="n">
+      <c r="U73" s="317" t="n">
         <f aca="false">Data_speed!R56</f>
         <v>0</v>
       </c>
-      <c r="V73" s="319" t="n">
+      <c r="V73" s="318" t="n">
         <f aca="false">Data_speed!S56</f>
         <v>0</v>
       </c>
@@ -16436,7 +16441,7 @@
     </row>
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B76" s="306" t="e">
         <f aca="false">SUM(B50:B73)/Data_speed!$O$57</f>
@@ -16495,26 +16500,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q76" s="293"/>
-      <c r="S76" s="320" t="n">
+      <c r="S76" s="319" t="n">
         <f aca="false">AVERAGE(S50:S73)</f>
         <v>0</v>
       </c>
-      <c r="T76" s="320" t="n">
+      <c r="T76" s="319" t="n">
         <f aca="false">AVERAGE(T50:T73)</f>
         <v>0</v>
       </c>
-      <c r="U76" s="320" t="n">
+      <c r="U76" s="319" t="n">
         <f aca="false">AVERAGE(U50:U73)</f>
         <v>0</v>
       </c>
-      <c r="V76" s="321" t="n">
+      <c r="V76" s="320" t="n">
         <f aca="false">AVERAGE(V50:V73)</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B77" s="307" t="e">
         <f aca="false">SUM(B56:B71)/Data_speed!$O$57</f>
@@ -16573,26 +16578,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q77" s="293"/>
-      <c r="S77" s="322" t="n">
+      <c r="S77" s="321" t="n">
         <f aca="false">AVERAGE(S56:S71)</f>
         <v>0</v>
       </c>
-      <c r="T77" s="322" t="n">
+      <c r="T77" s="321" t="n">
         <f aca="false">AVERAGE(T56:T71)</f>
         <v>0</v>
       </c>
-      <c r="U77" s="322" t="n">
+      <c r="U77" s="321" t="n">
         <f aca="false">AVERAGE(U56:U71)</f>
         <v>0</v>
       </c>
-      <c r="V77" s="323" t="n">
+      <c r="V77" s="322" t="n">
         <f aca="false">AVERAGE(V56:V71)</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B78" s="308" t="e">
         <f aca="false">B76-B77</f>
@@ -16652,19 +16657,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q78" s="293"/>
-      <c r="S78" s="324" t="n">
+      <c r="S78" s="323" t="n">
         <f aca="false">AVERAGE(AVERAGE(S50:S55), AVERAGE(S72:S73))</f>
         <v>0</v>
       </c>
-      <c r="T78" s="324" t="n">
+      <c r="T78" s="323" t="n">
         <f aca="false">AVERAGE(AVERAGE(T50:T55), AVERAGE(T72:T73))</f>
         <v>0</v>
       </c>
-      <c r="U78" s="324" t="n">
+      <c r="U78" s="323" t="n">
         <f aca="false">AVERAGE(AVERAGE(U50:U55), AVERAGE(U72:U73))</f>
         <v>0</v>
       </c>
-      <c r="V78" s="325" t="n">
+      <c r="V78" s="324" t="n">
         <f aca="false">AVERAGE(AVERAGE(V50:V55), AVERAGE(V72:V73))</f>
         <v>0</v>
       </c>
@@ -19003,15 +19008,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S57"/>
+  <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S58" activeCellId="0" sqref="S58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19764,6 +19770,10 @@
         <f aca="false">SUM(B29:N29)</f>
         <v>0</v>
       </c>
+      <c r="S29" s="1" t="e">
+        <f aca="false">SUMPRODUCT(B29:N29,B60:N60)/SUM(B29:N29)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20511,6 +20521,28 @@
         <f aca="false">SUM(B57:N57)</f>
         <v>0</v>
       </c>
+      <c r="S57" s="1" t="e">
+        <f aca="false">SUMPRODUCT(B57:N57,B60:N60)/SUM(B57:N57)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+      <c r="N60" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -20541,7 +20573,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20549,7 +20581,7 @@
         <v>11</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20584,10 +20616,10 @@
         <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N4" s="1" t="n">
         <v>1</v>
@@ -22191,7 +22223,7 @@
         <v>12</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22226,10 +22258,10 @@
         <v>10</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N32" s="1" t="n">
         <v>1</v>
@@ -23891,7 +23923,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -23904,7 +23936,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -23935,7 +23967,7 @@
     </row>
     <row r="9" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C9" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -23948,20 +23980,20 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C10" s="23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I10" s="23"/>
       <c r="J10" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K10" s="24"/>
     </row>
@@ -23970,33 +24002,33 @@
         <v>14</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E11" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>69</v>
-      </c>
       <c r="G11" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="H11" s="26" t="s">
-        <v>69</v>
-      </c>
       <c r="I11" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="J11" s="28" t="s">
-        <v>69</v>
-      </c>
       <c r="K11" s="29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C12" s="31" t="n">
         <f aca="false">Data_day!B29</f>
@@ -24037,7 +24069,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C13" s="31" t="n">
         <f aca="false">Data_day!C29</f>
@@ -24078,7 +24110,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C14" s="31" t="n">
         <f aca="false">Data_day!D29</f>
@@ -24119,7 +24151,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="37" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C15" s="31" t="n">
         <f aca="false">Data_day!E29</f>
@@ -24160,7 +24192,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="40" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C16" s="31" t="n">
         <f aca="false">Data_day!F29</f>
@@ -24204,7 +24236,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="44" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C18" s="45" t="n">
         <f aca="false">Data_day!G29</f>
@@ -24245,7 +24277,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="51" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C19" s="45" t="n">
         <f aca="false">Data_day!H29</f>
@@ -24289,7 +24321,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B21" s="56"/>
       <c r="C21" s="57" t="n">
@@ -24331,7 +24363,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="59" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B22" s="60"/>
       <c r="C22" s="61" t="n">
@@ -24404,7 +24436,7 @@
     </row>
     <row r="27" s="1" customFormat="true" ht="19.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C27" s="68" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D27" s="68"/>
       <c r="E27" s="68"/>
@@ -24414,11 +24446,11 @@
     </row>
     <row r="28" s="1" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C28" s="69" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D28" s="69"/>
       <c r="E28" s="70" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F28" s="70"/>
       <c r="H28" s="12"/>
@@ -24426,7 +24458,7 @@
     </row>
     <row r="29" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="71" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B29" s="72"/>
       <c r="C29" s="73" t="n">
@@ -24443,7 +24475,7 @@
     </row>
     <row r="30" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="75" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B30" s="76"/>
       <c r="C30" s="77" t="n">
@@ -24460,7 +24492,7 @@
     </row>
     <row r="31" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B31" s="76"/>
       <c r="C31" s="77" t="n">
@@ -24477,7 +24509,7 @@
     </row>
     <row r="32" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="75" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B32" s="76"/>
       <c r="C32" s="77" t="n">
@@ -24494,7 +24526,7 @@
     </row>
     <row r="33" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="79" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B33" s="80"/>
       <c r="C33" s="81" t="n">
@@ -24521,7 +24553,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="71" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B35" s="85"/>
       <c r="C35" s="73" t="n">
@@ -24534,7 +24566,7 @@
       </c>
       <c r="F35" s="74"/>
       <c r="H35" s="86" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I35" s="86"/>
       <c r="J35" s="86"/>
@@ -24542,7 +24574,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="79" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B36" s="87"/>
       <c r="C36" s="81" t="n">
@@ -24606,7 +24638,7 @@
     </row>
     <row r="42" customFormat="false" ht="18.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C42" s="68" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D42" s="68"/>
       <c r="E42" s="68"/>
@@ -24680,7 +24712,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="98" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B45" s="99"/>
       <c r="C45" s="34" t="e">
@@ -24722,7 +24754,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="102" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B46" s="103"/>
       <c r="C46" s="38" t="e">
@@ -24764,7 +24796,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="102" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B47" s="103"/>
       <c r="C47" s="38" t="e">
@@ -24806,7 +24838,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="102" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B48" s="103"/>
       <c r="C48" s="38" t="e">
@@ -24848,7 +24880,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="109" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B49" s="110"/>
       <c r="C49" s="41" t="e">
@@ -24903,7 +24935,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="71" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B51" s="85"/>
       <c r="C51" s="48" t="e">
@@ -24945,7 +24977,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="79" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B52" s="87"/>
       <c r="C52" s="54" t="e">
@@ -24999,7 +25031,7 @@
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="120"/>
       <c r="B54" s="121" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C54" s="122" t="e">
         <f aca="false">AVERAGE(C45:C49)</f>
@@ -25041,7 +25073,7 @@
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="128"/>
       <c r="B55" s="129" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C55" s="130" t="e">
         <f aca="false">AVERAGE(C45:C49,C51:C52)</f>
@@ -25180,7 +25212,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -25194,7 +25226,7 @@
     </row>
     <row r="5" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -25262,34 +25294,34 @@
         <v>14</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E10" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>69</v>
-      </c>
       <c r="G10" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="26" t="s">
-        <v>69</v>
-      </c>
       <c r="I10" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="J10" s="26" t="s">
-        <v>69</v>
-      </c>
       <c r="K10" s="27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="136"/>
       <c r="B11" s="137" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C11" s="57" t="n">
         <f aca="false">CV_H!C21</f>
@@ -25331,7 +25363,7 @@
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="143"/>
       <c r="B12" s="144" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C12" s="145" t="n">
         <f aca="false">CV_H!C22</f>
@@ -25372,19 +25404,19 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="151" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B33" s="151"/>
       <c r="C33" s="151"/>
       <c r="D33" s="151"/>
       <c r="E33" s="43"/>
       <c r="F33" s="151" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G33" s="151"/>
       <c r="H33" s="151"/>
@@ -25392,19 +25424,19 @@
     </row>
     <row r="34" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="151" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B34" s="151" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C34" s="151" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D34" s="152" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F34" s="151" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G34" s="151"/>
       <c r="H34" s="151" t="str">
@@ -25412,7 +25444,7 @@
         <v>% de TJMO</v>
       </c>
       <c r="I34" s="152" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25453,7 +25485,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="157" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G36" s="157"/>
       <c r="H36" s="158"/>
@@ -25476,7 +25508,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="157" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G37" s="157"/>
       <c r="H37" s="158" t="e">
@@ -25526,7 +25558,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="157" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G39" s="157"/>
       <c r="H39" s="158"/>
@@ -25549,7 +25581,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="157" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G40" s="157"/>
       <c r="H40" s="158" t="e">
@@ -25599,7 +25631,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="157" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G42" s="157"/>
       <c r="H42" s="158"/>
@@ -25622,7 +25654,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="157" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G43" s="157"/>
       <c r="H43" s="158" t="e">
@@ -25672,7 +25704,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="157" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G45" s="157"/>
       <c r="H45" s="158"/>
@@ -25695,7 +25727,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="157" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G46" s="157"/>
       <c r="H46" s="158" t="e">
@@ -25745,7 +25777,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="157" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G48" s="157"/>
       <c r="H48" s="158"/>
@@ -25768,7 +25800,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="157" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G49" s="157"/>
       <c r="H49" s="158" t="e">
@@ -25818,7 +25850,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="168" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G51" s="168"/>
       <c r="H51" s="168"/>
@@ -25876,10 +25908,10 @@
         <v>% de TJMO</v>
       </c>
       <c r="I53" s="151" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J53" s="151" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25921,7 +25953,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="157" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G55" s="157"/>
       <c r="H55" s="172" t="e">
@@ -25976,7 +26008,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="157" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G57" s="157"/>
       <c r="H57" s="172" t="e">
@@ -26466,7 +26498,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -26480,7 +26512,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -26518,10 +26550,10 @@
       </c>
       <c r="D9" s="182"/>
       <c r="M9" s="183" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="W9" s="184" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -26530,7 +26562,7 @@
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="185" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D12" s="185"/>
       <c r="E12" s="185"/>
@@ -26542,7 +26574,7 @@
       <c r="K12" s="185"/>
       <c r="L12" s="186"/>
       <c r="M12" s="185" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N12" s="185"/>
       <c r="O12" s="185"/>
@@ -26554,7 +26586,7 @@
       <c r="U12" s="185"/>
       <c r="V12" s="186"/>
       <c r="W12" s="185" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="X12" s="185"/>
       <c r="Y12" s="185"/>
@@ -26568,34 +26600,34 @@
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="188"/>
       <c r="B13" s="189" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C13" s="190" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D13" s="191" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" s="191" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F13" s="191" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G13" s="191" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H13" s="192" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I13" s="193" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J13" s="194" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K13" s="195" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L13" s="188"/>
       <c r="M13" s="190" t="str">
@@ -29524,7 +29556,7 @@
     </row>
     <row r="40" s="188" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="209" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C40" s="210" t="n">
         <f aca="false">SUM(C14:C37)</f>
@@ -29756,7 +29788,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="17" t="n">
@@ -29766,7 +29798,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -29780,7 +29812,7 @@
     </row>
     <row r="5" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -29818,7 +29850,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="217" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B9" s="218" t="n">
         <f aca="false">B4</f>
@@ -29848,32 +29880,32 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="222" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B12" s="223" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C12" s="152" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D12" s="224" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F12" s="224" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G12" s="152" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H12" s="225" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="226" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K12" s="221"/>
     </row>
@@ -30866,7 +30898,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B38" s="235" t="e">
         <f aca="false">SUM(B13:B36)/Data_category!$L$29</f>
@@ -30907,7 +30939,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B39" s="239" t="e">
         <f aca="false">SUM(B19:B34)/Data_category!$L$29</f>
@@ -30948,7 +30980,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B40" s="243" t="e">
         <f aca="false">B38-B39</f>
@@ -30998,7 +31030,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="217" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B42" s="4" t="n">
         <f aca="false">B5</f>
@@ -31028,7 +31060,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="222" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B45" s="249" t="str">
         <f aca="false">B12</f>
@@ -31060,7 +31092,7 @@
       </c>
       <c r="I45" s="43"/>
       <c r="J45" s="226" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K45" s="221"/>
     </row>
@@ -32053,7 +32085,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B71" s="235" t="e">
         <f aca="false">SUM(B46:B69)/Data_category!$L$57</f>
@@ -32094,7 +32126,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B72" s="239" t="e">
         <f aca="false">SUM(B52:B67)/Data_category!$L$57</f>
@@ -32135,7 +32167,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B73" s="243" t="e">
         <f aca="false">B71-B72</f>
@@ -32176,17 +32208,17 @@
     </row>
     <row r="75" s="43" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="83" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B75" s="83"/>
       <c r="C75" s="83" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D75" s="156"/>
       <c r="E75" s="83"/>
       <c r="F75" s="83"/>
       <c r="G75" s="83" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H75" s="83"/>
       <c r="I75" s="1"/>
@@ -32195,16 +32227,16 @@
     </row>
     <row r="76" s="43" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="83" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B76" s="83"/>
       <c r="C76" s="83" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E76" s="83"/>
       <c r="F76" s="83"/>
       <c r="G76" s="83" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H76" s="83"/>
       <c r="I76" s="1"/>
@@ -32219,20 +32251,20 @@
       <c r="E77" s="83"/>
       <c r="F77" s="83"/>
       <c r="G77" s="83" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H77" s="83"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="253" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B78" s="253"/>
       <c r="C78" s="253"/>
       <c r="D78" s="253"/>
       <c r="E78" s="253"/>
       <c r="F78" s="253" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G78" s="253"/>
       <c r="H78" s="253"/>
@@ -32333,7 +32365,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="17" t="n">
@@ -32343,7 +32375,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -32357,7 +32389,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -32395,7 +32427,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="217" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B9" s="4" t="n">
         <f aca="false">B4</f>
@@ -32433,7 +32465,7 @@
       <c r="H12" s="178"/>
       <c r="I12" s="259"/>
       <c r="J12" s="260" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K12" s="221"/>
     </row>
@@ -32902,7 +32934,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B39" s="235" t="e">
         <f aca="false">SWISS7_H!B38</f>
@@ -32941,7 +32973,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B40" s="239" t="e">
         <f aca="false">SWISS7_H!B39</f>
@@ -32980,7 +33012,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B41" s="243" t="e">
         <f aca="false">SWISS7_H!B40</f>
@@ -33019,7 +33051,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="217" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B44" s="4" t="n">
         <f aca="false">B5</f>
@@ -33054,7 +33086,7 @@
       <c r="H47" s="284"/>
       <c r="I47" s="284"/>
       <c r="J47" s="226" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K47" s="221"/>
     </row>
@@ -33523,7 +33555,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B74" s="235" t="e">
         <f aca="false">SWISS7_H!B71</f>
@@ -33562,7 +33594,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="238" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B75" s="239" t="e">
         <f aca="false">SWISS7_H!B72</f>
@@ -33601,7 +33633,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="242" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B76" s="243" t="e">
         <f aca="false">SWISS7_H!B73</f>

</xml_diff>

<commit_message>
Add legend on CV_LV chart
Closes #81
</commit_message>
<xml_diff>
--- a/comptages/report/template.xlsx
+++ b/comptages/report/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data_count" sheetId="1" state="visible" r:id="rId2"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="185">
   <si>
     <t xml:space="preserve">Data of the count</t>
   </si>
@@ -90,6 +90,9 @@
     <t xml:space="preserve">Section</t>
   </si>
   <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mon</t>
   </si>
   <si>
@@ -115,9 +118,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mean Mon-Fri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%</t>
   </si>
   <si>
     <t xml:space="preserve">Std deviation</t>
@@ -198,10 +198,16 @@
     <t xml:space="preserve">Monthly coefficient</t>
   </si>
   <si>
+    <t xml:space="preserve">dir1</t>
+  </si>
+  <si>
     <t xml:space="preserve">light</t>
   </si>
   <si>
     <t xml:space="preserve">heavy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dir2</t>
   </si>
   <si>
     <t xml:space="preserve">Data speed </t>
@@ -3305,7 +3311,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J3" s="12"/>
       <c r="N3" s="17" t="n">
@@ -3315,7 +3321,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -3329,7 +3335,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -3367,7 +3373,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="217" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B9" s="218" t="n">
         <f aca="false">B4</f>
@@ -3391,49 +3397,49 @@
       <c r="K11" s="248"/>
       <c r="L11" s="291"/>
       <c r="M11" s="220" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="N11" s="221" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="222" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B12" s="249" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C12" s="151" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D12" s="250" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E12" s="151" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F12" s="250" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G12" s="151" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H12" s="250" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I12" s="151" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J12" s="250" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K12" s="292" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L12" s="65"/>
       <c r="M12" s="226" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="N12" s="221"/>
     </row>
@@ -4736,7 +4742,7 @@
     <row r="37" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B38" s="235" t="e">
         <f aca="false">SUM(B13:B36)/Data_category!$L$29</f>
@@ -4790,7 +4796,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B39" s="239" t="e">
         <f aca="false">SUM(B19:B34)/Data_category!$L$29</f>
@@ -4844,7 +4850,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B40" s="243" t="e">
         <f aca="false">B38-B39</f>
@@ -4908,7 +4914,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="217" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B42" s="4" t="n">
         <f aca="false">B5</f>
@@ -4932,7 +4938,7 @@
       <c r="K44" s="248"/>
       <c r="L44" s="291"/>
       <c r="M44" s="220" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="N44" s="221" t="str">
         <f aca="false">N11</f>
@@ -4941,7 +4947,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="222" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B45" s="249" t="str">
         <f aca="false">B12</f>
@@ -4985,7 +4991,7 @@
       </c>
       <c r="L45" s="65"/>
       <c r="M45" s="226" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="N45" s="221"/>
     </row>
@@ -6288,7 +6294,7 @@
     <row r="70" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B71" s="235" t="e">
         <f aca="false">SUM(B46:B69)/Data_category!$L$57</f>
@@ -6342,7 +6348,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B72" s="239" t="e">
         <f aca="false">SUM(B52:B67)/Data_category!$L$57</f>
@@ -6396,7 +6402,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B73" s="243" t="e">
         <f aca="false">B71-B72</f>
@@ -6450,23 +6456,23 @@
     </row>
     <row r="75" s="43" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="83" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B75" s="83"/>
       <c r="C75" s="83" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D75" s="156"/>
       <c r="E75" s="83"/>
       <c r="F75" s="83"/>
       <c r="G75" s="83" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H75" s="83"/>
       <c r="I75" s="83"/>
       <c r="J75" s="295"/>
       <c r="K75" s="83" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L75" s="83"/>
       <c r="M75" s="1"/>
@@ -6474,16 +6480,16 @@
     </row>
     <row r="76" s="43" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="83" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B76" s="83"/>
       <c r="C76" s="83" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E76" s="83"/>
       <c r="F76" s="83"/>
       <c r="G76" s="83" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H76" s="83"/>
       <c r="I76" s="83"/>
@@ -6495,16 +6501,16 @@
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="83" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B77" s="83"/>
       <c r="C77" s="83" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E77" s="83"/>
       <c r="F77" s="83"/>
       <c r="G77" s="83" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H77" s="83"/>
       <c r="I77" s="83"/>
@@ -6514,7 +6520,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="253" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B78" s="253"/>
       <c r="C78" s="253"/>
@@ -6523,7 +6529,7 @@
       <c r="F78" s="253"/>
       <c r="G78" s="253"/>
       <c r="H78" s="253" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I78" s="253"/>
       <c r="J78" s="253"/>
@@ -6634,7 +6640,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -6648,7 +6654,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -6668,7 +6674,7 @@
       <c r="A6" s="15"/>
       <c r="C6" s="19"/>
       <c r="G6" s="16" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J6" s="12"/>
       <c r="N6" s="119"/>
@@ -6696,7 +6702,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="217" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B9" s="4" t="n">
         <f aca="false">B4</f>
@@ -6722,7 +6728,7 @@
       <c r="L11" s="257"/>
       <c r="M11" s="258"/>
       <c r="N11" s="221" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6739,7 +6745,7 @@
       <c r="K12" s="178"/>
       <c r="L12" s="259"/>
       <c r="M12" s="260" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="N12" s="221"/>
     </row>
@@ -7292,7 +7298,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B39" s="235" t="e">
         <f aca="false">SWISS10_H!B38</f>
@@ -7343,7 +7349,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B40" s="239" t="e">
         <f aca="false">SWISS10_H!B39</f>
@@ -7394,7 +7400,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B41" s="243" t="e">
         <f aca="false">SWISS10_H!B40</f>
@@ -7445,7 +7451,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="217" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B44" s="4" t="n">
         <f aca="false">B5</f>
@@ -7486,7 +7492,7 @@
       <c r="K47" s="284"/>
       <c r="L47" s="284"/>
       <c r="M47" s="226" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="N47" s="221"/>
     </row>
@@ -8039,7 +8045,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B74" s="235" t="e">
         <f aca="false">SWISS10_H!B71</f>
@@ -8090,7 +8096,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B75" s="239" t="e">
         <f aca="false">SWISS10_H!B72</f>
@@ -8141,7 +8147,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B76" s="243" t="e">
         <f aca="false">SWISS10_H!B73</f>
@@ -8236,7 +8242,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
@@ -8300,7 +8306,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -8316,7 +8322,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -8351,13 +8357,13 @@
     </row>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H8" s="20" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="217" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B10" s="4" t="n">
         <f aca="false">B4</f>
@@ -8407,7 +8413,7 @@
       <c r="L12" s="248"/>
       <c r="M12" s="248"/>
       <c r="O12" s="220" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="P12" s="291"/>
       <c r="R12" s="0"/>
@@ -8422,46 +8428,46 @@
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="222" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B13" s="249" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C13" s="151" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D13" s="151" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E13" s="151" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F13" s="151" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G13" s="151" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H13" s="151" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="I13" s="151" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="J13" s="151" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="K13" s="151" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="L13" s="151" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="M13" s="252" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="O13" s="304" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="P13" s="119"/>
       <c r="R13" s="0"/>
@@ -9972,7 +9978,7 @@
     </row>
     <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B40" s="306" t="e">
         <f aca="false">SUM(B14:B37)/Data_speed!$O$29</f>
@@ -10034,7 +10040,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B41" s="307" t="e">
         <f aca="false">SUM(B20:B35)/Data_speed!$O$29</f>
@@ -10096,7 +10102,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B42" s="308" t="e">
         <f aca="false">B40-B41</f>
@@ -10171,7 +10177,7 @@
     <row r="45" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="217" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B46" s="4" t="n">
         <f aca="false">B5</f>
@@ -10233,7 +10239,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="222" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B49" s="249" t="str">
         <f aca="false">B13</f>
@@ -11796,7 +11802,7 @@
     </row>
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B76" s="306" t="e">
         <f aca="false">SUM(B50:B73)/Data_speed!$O$57</f>
@@ -11858,7 +11864,7 @@
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B77" s="307" t="e">
         <f aca="false">SUM(B56:B71)/Data_speed!$O$57</f>
@@ -11920,7 +11926,7 @@
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B78" s="308" t="e">
         <f aca="false">B76-B77</f>
@@ -12094,7 +12100,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -12109,7 +12115,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -12142,13 +12148,13 @@
     </row>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J8" s="20" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="217" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B10" s="4" t="n">
         <f aca="false">B4</f>
@@ -12199,11 +12205,11 @@
       <c r="M12" s="248"/>
       <c r="N12" s="311"/>
       <c r="P12" s="220" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="Q12" s="291"/>
       <c r="S12" s="312" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="T12" s="312"/>
       <c r="U12" s="312"/>
@@ -12211,62 +12217,62 @@
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="222" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B13" s="249" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="249" t="s">
+        <v>179</v>
+      </c>
+      <c r="D13" s="151" t="s">
+        <v>164</v>
+      </c>
+      <c r="E13" s="151" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" s="151" t="s">
+        <v>166</v>
+      </c>
+      <c r="G13" s="151" t="s">
+        <v>167</v>
+      </c>
+      <c r="H13" s="151" t="s">
+        <v>168</v>
+      </c>
+      <c r="I13" s="151" t="s">
+        <v>169</v>
+      </c>
+      <c r="J13" s="151" t="s">
+        <v>170</v>
+      </c>
+      <c r="K13" s="151" t="s">
+        <v>171</v>
+      </c>
+      <c r="L13" s="151" t="s">
+        <v>172</v>
+      </c>
+      <c r="M13" s="151" t="s">
+        <v>173</v>
+      </c>
+      <c r="N13" s="252" t="s">
+        <v>180</v>
+      </c>
+      <c r="P13" s="304" t="s">
         <v>176</v>
-      </c>
-      <c r="C13" s="249" t="s">
-        <v>177</v>
-      </c>
-      <c r="D13" s="151" t="s">
-        <v>162</v>
-      </c>
-      <c r="E13" s="151" t="s">
-        <v>163</v>
-      </c>
-      <c r="F13" s="151" t="s">
-        <v>164</v>
-      </c>
-      <c r="G13" s="151" t="s">
-        <v>165</v>
-      </c>
-      <c r="H13" s="151" t="s">
-        <v>166</v>
-      </c>
-      <c r="I13" s="151" t="s">
-        <v>167</v>
-      </c>
-      <c r="J13" s="151" t="s">
-        <v>168</v>
-      </c>
-      <c r="K13" s="151" t="s">
-        <v>169</v>
-      </c>
-      <c r="L13" s="151" t="s">
-        <v>170</v>
-      </c>
-      <c r="M13" s="151" t="s">
-        <v>171</v>
-      </c>
-      <c r="N13" s="252" t="s">
-        <v>178</v>
-      </c>
-      <c r="P13" s="304" t="s">
-        <v>174</v>
       </c>
       <c r="Q13" s="119"/>
       <c r="S13" s="313" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="T13" s="314" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="U13" s="315" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="V13" s="316" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14157,7 +14163,7 @@
     </row>
     <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B40" s="306" t="e">
         <f aca="false">SUM(B14:B37)/Data_speed!$O$29</f>
@@ -14235,7 +14241,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B41" s="307" t="e">
         <f aca="false">SUM(B20:B35)/Data_speed!$O$29</f>
@@ -14313,7 +14319,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B42" s="308" t="e">
         <f aca="false">B40-B41</f>
@@ -14409,7 +14415,7 @@
     </row>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="217" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B46" s="4" t="n">
         <f aca="false">B5</f>
@@ -14477,7 +14483,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="222" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B49" s="249" t="str">
         <f aca="false">B13</f>
@@ -16441,7 +16447,7 @@
     </row>
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B76" s="306" t="e">
         <f aca="false">SUM(B50:B73)/Data_speed!$O$57</f>
@@ -16519,7 +16525,7 @@
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B77" s="307" t="e">
         <f aca="false">SUM(B56:B71)/Data_speed!$O$57</f>
@@ -16597,7 +16603,7 @@
     </row>
     <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B78" s="308" t="e">
         <f aca="false">B76-B77</f>
@@ -16726,8 +16732,8 @@
   </sheetPr>
   <dimension ref="A1:T93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B92" activeCellId="0" sqref="B92"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K66" activeCellId="0" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16749,43 +16755,46 @@
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="K3" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17559,7 +17568,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B29" s="1" t="n">
         <f aca="false">SUM(B5:B28)</f>
@@ -17628,37 +17637,40 @@
       <c r="A33" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="K33" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18240,7 +18252,7 @@
     </row>
     <row r="59" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B59" s="1" t="n">
         <f aca="false">SUM(B35:B58)</f>
@@ -18286,7 +18298,7 @@
     <row r="60" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -18298,7 +18310,7 @@
     </row>
     <row r="62" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -18313,37 +18325,40 @@
       <c r="A64" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="K64" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18925,7 +18940,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B90" s="1" t="n">
         <f aca="false">SUM(B66:B89)</f>
@@ -18970,7 +18985,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -18982,7 +18997,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -19022,7 +19037,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19071,19 +19086,19 @@
         <v>13</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19712,7 +19727,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B29" s="1" t="n">
         <f aca="false">SUM(B5:B28)</f>
@@ -19822,19 +19837,19 @@
         <v>13</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20463,7 +20478,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B57" s="1" t="n">
         <f aca="false">SUM(B33:B56)</f>
@@ -20528,7 +20543,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -20573,7 +20588,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20581,7 +20596,7 @@
         <v>11</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20616,10 +20631,10 @@
         <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N4" s="1" t="n">
         <v>1</v>
@@ -22166,7 +22181,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B29" s="1" t="n">
         <f aca="false">SUM(B5:B28)</f>
@@ -22223,7 +22238,7 @@
         <v>12</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22258,10 +22273,10 @@
         <v>10</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N32" s="1" t="n">
         <v>1</v>
@@ -23808,7 +23823,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B57" s="1" t="n">
         <f aca="false">SUM(B33:B56)</f>
@@ -23923,7 +23938,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -23936,7 +23951,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -23967,7 +23982,7 @@
     </row>
     <row r="9" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C9" s="22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -23980,20 +23995,20 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C10" s="23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I10" s="23"/>
       <c r="J10" s="24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K10" s="24"/>
     </row>
@@ -24002,33 +24017,33 @@
         <v>14</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J11" s="28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="30" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C12" s="31" t="n">
         <f aca="false">Data_day!B29</f>
@@ -24069,7 +24084,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="37" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C13" s="31" t="n">
         <f aca="false">Data_day!C29</f>
@@ -24110,7 +24125,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="37" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C14" s="31" t="n">
         <f aca="false">Data_day!D29</f>
@@ -24151,7 +24166,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="37" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C15" s="31" t="n">
         <f aca="false">Data_day!E29</f>
@@ -24192,7 +24207,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="40" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C16" s="31" t="n">
         <f aca="false">Data_day!F29</f>
@@ -24236,7 +24251,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="44" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C18" s="45" t="n">
         <f aca="false">Data_day!G29</f>
@@ -24277,7 +24292,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="51" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C19" s="45" t="n">
         <f aca="false">Data_day!H29</f>
@@ -24321,7 +24336,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="55" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B21" s="56"/>
       <c r="C21" s="57" t="n">
@@ -24363,7 +24378,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="59" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B22" s="60"/>
       <c r="C22" s="61" t="n">
@@ -24436,7 +24451,7 @@
     </row>
     <row r="27" s="1" customFormat="true" ht="19.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C27" s="68" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D27" s="68"/>
       <c r="E27" s="68"/>
@@ -24446,11 +24461,11 @@
     </row>
     <row r="28" s="1" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C28" s="69" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D28" s="69"/>
       <c r="E28" s="70" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F28" s="70"/>
       <c r="H28" s="12"/>
@@ -24458,7 +24473,7 @@
     </row>
     <row r="29" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="71" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B29" s="72"/>
       <c r="C29" s="73" t="n">
@@ -24475,7 +24490,7 @@
     </row>
     <row r="30" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="75" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B30" s="76"/>
       <c r="C30" s="77" t="n">
@@ -24492,7 +24507,7 @@
     </row>
     <row r="31" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="75" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B31" s="76"/>
       <c r="C31" s="77" t="n">
@@ -24509,7 +24524,7 @@
     </row>
     <row r="32" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="75" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B32" s="76"/>
       <c r="C32" s="77" t="n">
@@ -24526,7 +24541,7 @@
     </row>
     <row r="33" s="1" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="79" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B33" s="80"/>
       <c r="C33" s="81" t="n">
@@ -24553,7 +24568,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="71" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B35" s="85"/>
       <c r="C35" s="73" t="n">
@@ -24566,7 +24581,7 @@
       </c>
       <c r="F35" s="74"/>
       <c r="H35" s="86" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I35" s="86"/>
       <c r="J35" s="86"/>
@@ -24574,7 +24589,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="79" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B36" s="87"/>
       <c r="C36" s="81" t="n">
@@ -24638,7 +24653,7 @@
     </row>
     <row r="42" customFormat="false" ht="18.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C42" s="68" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D42" s="68"/>
       <c r="E42" s="68"/>
@@ -24712,7 +24727,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="98" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B45" s="99"/>
       <c r="C45" s="34" t="e">
@@ -24754,7 +24769,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="102" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B46" s="103"/>
       <c r="C46" s="38" t="e">
@@ -24796,7 +24811,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="102" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B47" s="103"/>
       <c r="C47" s="38" t="e">
@@ -24838,7 +24853,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="102" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B48" s="103"/>
       <c r="C48" s="38" t="e">
@@ -24880,7 +24895,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="109" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B49" s="110"/>
       <c r="C49" s="41" t="e">
@@ -24935,7 +24950,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="71" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B51" s="85"/>
       <c r="C51" s="48" t="e">
@@ -24977,7 +24992,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="79" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B52" s="87"/>
       <c r="C52" s="54" t="e">
@@ -25031,7 +25046,7 @@
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="120"/>
       <c r="B54" s="121" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C54" s="122" t="e">
         <f aca="false">AVERAGE(C45:C49)</f>
@@ -25073,7 +25088,7 @@
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="128"/>
       <c r="B55" s="129" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C55" s="130" t="e">
         <f aca="false">AVERAGE(C45:C49,C51:C52)</f>
@@ -25212,7 +25227,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -25226,7 +25241,7 @@
     </row>
     <row r="5" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -25294,34 +25309,34 @@
         <v>14</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K10" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="136"/>
       <c r="B11" s="137" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C11" s="57" t="n">
         <f aca="false">CV_H!C21</f>
@@ -25363,7 +25378,7 @@
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="143"/>
       <c r="B12" s="144" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C12" s="145" t="n">
         <f aca="false">CV_H!C22</f>
@@ -25404,19 +25419,19 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="13" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="151" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B33" s="151"/>
       <c r="C33" s="151"/>
       <c r="D33" s="151"/>
       <c r="E33" s="43"/>
       <c r="F33" s="151" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G33" s="151"/>
       <c r="H33" s="151"/>
@@ -25424,19 +25439,19 @@
     </row>
     <row r="34" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="151" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B34" s="151" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C34" s="151" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D34" s="152" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F34" s="151" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G34" s="151"/>
       <c r="H34" s="151" t="str">
@@ -25444,7 +25459,7 @@
         <v>% de TJMO</v>
       </c>
       <c r="I34" s="152" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25485,7 +25500,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="157" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G36" s="157"/>
       <c r="H36" s="158"/>
@@ -25508,7 +25523,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="157" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G37" s="157"/>
       <c r="H37" s="158" t="e">
@@ -25558,7 +25573,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="157" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G39" s="157"/>
       <c r="H39" s="158"/>
@@ -25581,7 +25596,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="157" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G40" s="157"/>
       <c r="H40" s="158" t="e">
@@ -25631,7 +25646,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="157" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G42" s="157"/>
       <c r="H42" s="158"/>
@@ -25654,7 +25669,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="157" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G43" s="157"/>
       <c r="H43" s="158" t="e">
@@ -25704,7 +25719,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="157" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G45" s="157"/>
       <c r="H45" s="158"/>
@@ -25727,7 +25742,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="157" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G46" s="157"/>
       <c r="H46" s="158" t="e">
@@ -25777,7 +25792,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="157" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G48" s="157"/>
       <c r="H48" s="158"/>
@@ -25800,7 +25815,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="157" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G49" s="157"/>
       <c r="H49" s="158" t="e">
@@ -25850,7 +25865,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="168" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G51" s="168"/>
       <c r="H51" s="168"/>
@@ -25908,10 +25923,10 @@
         <v>% de TJMO</v>
       </c>
       <c r="I53" s="151" t="s">
+        <v>106</v>
+      </c>
+      <c r="J53" s="151" t="s">
         <v>104</v>
-      </c>
-      <c r="J53" s="151" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25953,7 +25968,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="157" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G55" s="157"/>
       <c r="H55" s="172" t="e">
@@ -26008,7 +26023,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="157" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G57" s="157"/>
       <c r="H57" s="172" t="e">
@@ -26498,7 +26513,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -26512,7 +26527,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -26550,10 +26565,10 @@
       </c>
       <c r="D9" s="182"/>
       <c r="M9" s="183" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="W9" s="184" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -26562,7 +26577,7 @@
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="185" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D12" s="185"/>
       <c r="E12" s="185"/>
@@ -26574,7 +26589,7 @@
       <c r="K12" s="185"/>
       <c r="L12" s="186"/>
       <c r="M12" s="185" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="N12" s="185"/>
       <c r="O12" s="185"/>
@@ -26586,7 +26601,7 @@
       <c r="U12" s="185"/>
       <c r="V12" s="186"/>
       <c r="W12" s="185" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="X12" s="185"/>
       <c r="Y12" s="185"/>
@@ -26600,34 +26615,34 @@
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="188"/>
       <c r="B13" s="189" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C13" s="190" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D13" s="191" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E13" s="191" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F13" s="191" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G13" s="191" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H13" s="192" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I13" s="193" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J13" s="194" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K13" s="195" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="L13" s="188"/>
       <c r="M13" s="190" t="str">
@@ -29556,7 +29571,7 @@
     </row>
     <row r="40" s="188" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="209" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C40" s="210" t="n">
         <f aca="false">SUM(C14:C37)</f>
@@ -29788,7 +29803,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="17" t="n">
@@ -29798,7 +29813,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -29812,7 +29827,7 @@
     </row>
     <row r="5" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -29850,7 +29865,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="217" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B9" s="218" t="n">
         <f aca="false">B4</f>
@@ -29880,32 +29895,32 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="222" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B12" s="223" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C12" s="152" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D12" s="224" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F12" s="224" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G12" s="152" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H12" s="225" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="226" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K12" s="221"/>
     </row>
@@ -30898,7 +30913,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B38" s="235" t="e">
         <f aca="false">SUM(B13:B36)/Data_category!$L$29</f>
@@ -30939,7 +30954,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B39" s="239" t="e">
         <f aca="false">SUM(B19:B34)/Data_category!$L$29</f>
@@ -30980,7 +30995,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B40" s="243" t="e">
         <f aca="false">B38-B39</f>
@@ -31030,7 +31045,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="217" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B42" s="4" t="n">
         <f aca="false">B5</f>
@@ -31060,7 +31075,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="222" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B45" s="249" t="str">
         <f aca="false">B12</f>
@@ -31092,7 +31107,7 @@
       </c>
       <c r="I45" s="43"/>
       <c r="J45" s="226" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K45" s="221"/>
     </row>
@@ -32085,7 +32100,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B71" s="235" t="e">
         <f aca="false">SUM(B46:B69)/Data_category!$L$57</f>
@@ -32126,7 +32141,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B72" s="239" t="e">
         <f aca="false">SUM(B52:B67)/Data_category!$L$57</f>
@@ -32167,7 +32182,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B73" s="243" t="e">
         <f aca="false">B71-B72</f>
@@ -32208,17 +32223,17 @@
     </row>
     <row r="75" s="43" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="83" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B75" s="83"/>
       <c r="C75" s="83" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D75" s="156"/>
       <c r="E75" s="83"/>
       <c r="F75" s="83"/>
       <c r="G75" s="83" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H75" s="83"/>
       <c r="I75" s="1"/>
@@ -32227,16 +32242,16 @@
     </row>
     <row r="76" s="43" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="83" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B76" s="83"/>
       <c r="C76" s="83" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E76" s="83"/>
       <c r="F76" s="83"/>
       <c r="G76" s="83" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H76" s="83"/>
       <c r="I76" s="1"/>
@@ -32251,20 +32266,20 @@
       <c r="E77" s="83"/>
       <c r="F77" s="83"/>
       <c r="G77" s="83" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H77" s="83"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="253" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B78" s="253"/>
       <c r="C78" s="253"/>
       <c r="D78" s="253"/>
       <c r="E78" s="253"/>
       <c r="F78" s="253" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G78" s="253"/>
       <c r="H78" s="253"/>
@@ -32365,7 +32380,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="17" t="n">
@@ -32375,7 +32390,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" s="18" t="n">
         <f aca="false">Data_count!B13</f>
@@ -32389,7 +32404,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="n">
         <f aca="false">Data_count!B14</f>
@@ -32427,7 +32442,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="217" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B9" s="4" t="n">
         <f aca="false">B4</f>
@@ -32465,7 +32480,7 @@
       <c r="H12" s="178"/>
       <c r="I12" s="259"/>
       <c r="J12" s="260" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K12" s="221"/>
     </row>
@@ -32934,7 +32949,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B39" s="235" t="e">
         <f aca="false">SWISS7_H!B38</f>
@@ -32973,7 +32988,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B40" s="239" t="e">
         <f aca="false">SWISS7_H!B39</f>
@@ -33012,7 +33027,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B41" s="243" t="e">
         <f aca="false">SWISS7_H!B40</f>
@@ -33051,7 +33066,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="217" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B44" s="4" t="n">
         <f aca="false">B5</f>
@@ -33086,7 +33101,7 @@
       <c r="H47" s="284"/>
       <c r="I47" s="284"/>
       <c r="J47" s="226" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K47" s="221"/>
     </row>
@@ -33555,7 +33570,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B74" s="235" t="e">
         <f aca="false">SWISS7_H!B71</f>
@@ -33594,7 +33609,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="238" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B75" s="239" t="e">
         <f aca="false">SWISS7_H!B72</f>
@@ -33633,7 +33648,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="242" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B76" s="243" t="e">
         <f aca="false">SWISS7_H!B73</f>

</xml_diff>

<commit_message>
Calculate % of average of heavy vehicles instead of average of %
As described in #89
</commit_message>
<xml_diff>
--- a/comptages/report/template.xlsx
+++ b/comptages/report/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Data_count" sheetId="1" state="visible" r:id="rId2"/>
@@ -16732,7 +16732,7 @@
   </sheetPr>
   <dimension ref="A1:T93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K66" activeCellId="0" sqref="K66"/>
     </sheetView>
   </sheetViews>
@@ -23892,8 +23892,8 @@
   </sheetPr>
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P25" activeCellId="0" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24368,11 +24368,11 @@
         <v>0</v>
       </c>
       <c r="J21" s="58" t="e">
-        <f aca="false">AVERAGE(J12:J16)</f>
+        <f aca="false">100/D21*H21%</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K21" s="58" t="e">
-        <f aca="false">AVERAGE(K12:K16)</f>
+        <f aca="false">100/E21*I21%</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -24410,11 +24410,11 @@
         <v>0</v>
       </c>
       <c r="J22" s="62" t="e">
-        <f aca="false">AVERAGE(J12:J19)</f>
+        <f aca="false">100/D22*H22%</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K22" s="62" t="e">
-        <f aca="false">AVERAGE(K12:K19)</f>
+        <f aca="false">100/E22*I22%</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -25180,7 +25180,7 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L42" activeCellId="0" sqref="L42"/>
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>